<commit_message>
Working with Edit RFQ buyer side
</commit_message>
<xml_diff>
--- a/AQPM Gantt.xlsx
+++ b/AQPM Gantt.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Issues" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'APQM Gantt'!$A$7:$EK$125</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'APQM Gantt'!$A$7:$EK$130</definedName>
     <definedName name="Actual" localSheetId="0">('APQM Gantt'!PeriodInActual*('APQM Gantt'!$F1&gt;0))*'APQM Gantt'!PeriodInPlan</definedName>
     <definedName name="Actual">(PeriodInActual*(#REF!&gt;0))*PeriodInPlan</definedName>
     <definedName name="ActualBeyond" localSheetId="0">'APQM Gantt'!PeriodInActual*('APQM Gantt'!$F1&gt;0)</definedName>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="161">
   <si>
     <t>Plan</t>
   </si>
@@ -663,6 +663,18 @@
   </si>
   <si>
     <t>See issue with NDA</t>
+  </si>
+  <si>
+    <t>Change BOM Component status when its RFQ award/selected has been deleted</t>
+  </si>
+  <si>
+    <t>Page inside emails</t>
+  </si>
+  <si>
+    <t>New Lead Times requested by Seth.</t>
+  </si>
+  <si>
+    <t>Allow edit RFQ about Buyers fields.</t>
   </si>
 </sst>
 </file>
@@ -1160,134 +1172,6 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0"/>
@@ -1542,6 +1426,134 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1565,15 +1577,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="24">
   <autoFilter ref="A4:F238"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="5"/>
-    <tableColumn id="2" name="Date" dataDxfId="4"/>
-    <tableColumn id="3" name="Creator" dataDxfId="3"/>
-    <tableColumn id="4" name="Issue" dataDxfId="2"/>
-    <tableColumn id="5" name="Status" dataDxfId="1"/>
-    <tableColumn id="6" name="Solution" dataDxfId="0"/>
+    <tableColumn id="1" name="#" dataDxfId="23"/>
+    <tableColumn id="2" name="Date" dataDxfId="22"/>
+    <tableColumn id="3" name="Creator" dataDxfId="21"/>
+    <tableColumn id="4" name="Issue" dataDxfId="20"/>
+    <tableColumn id="5" name="Status" dataDxfId="19"/>
+    <tableColumn id="6" name="Solution" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1809,13 +1821,13 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:EK135"/>
+  <dimension ref="A2:EK140"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="DV72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="7" topLeftCell="DV112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="H79" sqref="H79"/>
+      <selection pane="bottomRight" activeCell="DV122" sqref="DV122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25"/>
@@ -1852,7 +1864,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
@@ -9125,21 +9137,21 @@
     </row>
     <row r="115" spans="1:141" ht="18.95" customHeight="1">
       <c r="A115" s="25"/>
-      <c r="B115" s="26">
-        <v>2</v>
-      </c>
-      <c r="C115" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="D115" s="29">
-        <v>116</v>
-      </c>
-      <c r="E115" s="13">
-        <v>1</v>
-      </c>
-      <c r="F115" s="13"/>
-      <c r="G115" s="13"/>
-      <c r="H115" s="5"/>
+      <c r="B115" s="26"/>
+      <c r="C115" s="53" t="s">
+        <v>153</v>
+      </c>
+      <c r="D115" s="29"/>
+      <c r="E115" s="13"/>
+      <c r="F115" s="13">
+        <v>120</v>
+      </c>
+      <c r="G115" s="13">
+        <v>1</v>
+      </c>
+      <c r="H115" s="5">
+        <v>1</v>
+      </c>
       <c r="N115" s="28"/>
       <c r="O115" s="28"/>
       <c r="U115" s="28"/>
@@ -9185,8 +9197,8 @@
       <c r="B116" s="26">
         <v>3</v>
       </c>
-      <c r="C116" s="47" t="s">
-        <v>143</v>
+      <c r="C116" s="54" t="s">
+        <v>136</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="13"/>
@@ -9213,7 +9225,6 @@
       <c r="BS116" s="28"/>
       <c r="BY116" s="28"/>
       <c r="BZ116" s="28"/>
-      <c r="CE116" s="38"/>
       <c r="CF116" s="28"/>
       <c r="CG116" s="28"/>
       <c r="CM116" s="28"/>
@@ -9236,20 +9247,14 @@
     <row r="117" spans="1:141" ht="18.95" customHeight="1">
       <c r="A117" s="25"/>
       <c r="B117" s="26"/>
-      <c r="C117" s="53" t="s">
-        <v>153</v>
+      <c r="C117" s="47" t="s">
+        <v>157</v>
       </c>
       <c r="D117" s="29"/>
       <c r="E117" s="13"/>
-      <c r="F117" s="13">
-        <v>120</v>
-      </c>
-      <c r="G117" s="13">
-        <v>1</v>
-      </c>
-      <c r="H117" s="5">
-        <v>1</v>
-      </c>
+      <c r="F117" s="13"/>
+      <c r="G117" s="13"/>
+      <c r="H117" s="5"/>
       <c r="N117" s="28"/>
       <c r="O117" s="28"/>
       <c r="U117" s="28"/>
@@ -9292,17 +9297,23 @@
     </row>
     <row r="118" spans="1:141" ht="18.95" customHeight="1">
       <c r="A118" s="25"/>
-      <c r="B118" s="26">
-        <v>3</v>
-      </c>
-      <c r="C118" s="54" t="s">
-        <v>136</v>
+      <c r="B118" s="26"/>
+      <c r="C118" s="47" t="s">
+        <v>160</v>
       </c>
       <c r="D118" s="29"/>
-      <c r="E118" s="13"/>
-      <c r="F118" s="13"/>
-      <c r="G118" s="13"/>
-      <c r="H118" s="5"/>
+      <c r="E118" s="13">
+        <v>2</v>
+      </c>
+      <c r="F118" s="13">
+        <v>123</v>
+      </c>
+      <c r="G118" s="13">
+        <v>5</v>
+      </c>
+      <c r="H118" s="5">
+        <v>0.8</v>
+      </c>
       <c r="N118" s="28"/>
       <c r="O118" s="28"/>
       <c r="U118" s="28"/>
@@ -9323,6 +9334,7 @@
       <c r="BS118" s="28"/>
       <c r="BY118" s="28"/>
       <c r="BZ118" s="28"/>
+      <c r="CE118" s="38"/>
       <c r="CF118" s="28"/>
       <c r="CG118" s="28"/>
       <c r="CM118" s="28"/>
@@ -9345,7 +9357,9 @@
     <row r="119" spans="1:141" ht="18.95" customHeight="1">
       <c r="A119" s="25"/>
       <c r="B119" s="26"/>
-      <c r="C119" s="53"/>
+      <c r="C119" s="47" t="s">
+        <v>159</v>
+      </c>
       <c r="D119" s="29"/>
       <c r="E119" s="13"/>
       <c r="F119" s="13"/>
@@ -9392,13 +9406,19 @@
       <c r="EK119" s="28"/>
     </row>
     <row r="120" spans="1:141" ht="18.95" customHeight="1">
-      <c r="A120" s="55" t="s">
-        <v>148</v>
-      </c>
-      <c r="B120" s="55"/>
-      <c r="C120" s="55"/>
-      <c r="D120" s="29"/>
-      <c r="E120" s="13"/>
+      <c r="A120" s="25"/>
+      <c r="B120" s="26">
+        <v>2</v>
+      </c>
+      <c r="C120" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="D120" s="29">
+        <v>116</v>
+      </c>
+      <c r="E120" s="13">
+        <v>1</v>
+      </c>
       <c r="F120" s="13"/>
       <c r="G120" s="13"/>
       <c r="H120" s="5"/>
@@ -9445,10 +9465,10 @@
     <row r="121" spans="1:141" ht="18.95" customHeight="1">
       <c r="A121" s="25"/>
       <c r="B121" s="26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C121" s="47" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="13"/>
@@ -9497,12 +9517,8 @@
     </row>
     <row r="122" spans="1:141" ht="18.95" customHeight="1">
       <c r="A122" s="25"/>
-      <c r="B122" s="26">
-        <v>2</v>
-      </c>
-      <c r="C122" s="47" t="s">
-        <v>149</v>
-      </c>
+      <c r="B122" s="26"/>
+      <c r="C122" s="53"/>
       <c r="D122" s="29"/>
       <c r="E122" s="13"/>
       <c r="F122" s="13"/>
@@ -9550,18 +9566,10 @@
     </row>
     <row r="123" spans="1:141" ht="18.95" customHeight="1">
       <c r="A123" s="25"/>
-      <c r="B123" s="26">
-        <v>1</v>
-      </c>
-      <c r="C123" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="D123" s="29">
-        <v>116</v>
-      </c>
-      <c r="E123" s="13">
-        <v>1</v>
-      </c>
+      <c r="B123" s="26"/>
+      <c r="C123" s="53"/>
+      <c r="D123" s="29"/>
+      <c r="E123" s="13"/>
       <c r="F123" s="13"/>
       <c r="G123" s="13"/>
       <c r="H123" s="5"/>
@@ -9606,21 +9614,11 @@
       <c r="EK123" s="28"/>
     </row>
     <row r="124" spans="1:141" ht="18.95" customHeight="1">
-      <c r="A124" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B124" s="26">
-        <v>1</v>
-      </c>
-      <c r="C124" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="D124" s="29">
-        <v>112</v>
-      </c>
-      <c r="E124" s="13">
-        <v>1</v>
-      </c>
+      <c r="A124" s="25"/>
+      <c r="B124" s="26"/>
+      <c r="C124" s="53"/>
+      <c r="D124" s="29"/>
+      <c r="E124" s="13"/>
       <c r="F124" s="13"/>
       <c r="G124" s="13"/>
       <c r="H124" s="5"/>
@@ -9644,6 +9642,7 @@
       <c r="BS124" s="28"/>
       <c r="BY124" s="28"/>
       <c r="BZ124" s="28"/>
+      <c r="CE124" s="38"/>
       <c r="CF124" s="28"/>
       <c r="CG124" s="28"/>
       <c r="CM124" s="28"/>
@@ -9664,26 +9663,16 @@
       <c r="EK124" s="28"/>
     </row>
     <row r="125" spans="1:141" ht="18.95" customHeight="1">
-      <c r="A125" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B125" s="26">
-        <v>1</v>
-      </c>
-      <c r="C125" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D125" s="29">
-        <v>113</v>
-      </c>
-      <c r="E125" s="13">
-        <v>4</v>
-      </c>
+      <c r="A125" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="B125" s="55"/>
+      <c r="C125" s="55"/>
+      <c r="D125" s="29"/>
+      <c r="E125" s="13"/>
       <c r="F125" s="13"/>
       <c r="G125" s="13"/>
-      <c r="H125" s="5">
-        <v>0.5</v>
-      </c>
+      <c r="H125" s="5"/>
       <c r="N125" s="28"/>
       <c r="O125" s="28"/>
       <c r="U125" s="28"/>
@@ -9704,6 +9693,7 @@
       <c r="BS125" s="28"/>
       <c r="BY125" s="28"/>
       <c r="BZ125" s="28"/>
+      <c r="CE125" s="38"/>
       <c r="CF125" s="28"/>
       <c r="CG125" s="28"/>
       <c r="CM125" s="28"/>
@@ -9725,9 +9715,11 @@
     </row>
     <row r="126" spans="1:141" ht="18.95" customHeight="1">
       <c r="A126" s="25"/>
-      <c r="B126" s="26"/>
+      <c r="B126" s="26">
+        <v>2</v>
+      </c>
       <c r="C126" s="47" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D126" s="29"/>
       <c r="E126" s="13"/>
@@ -9777,10 +9769,10 @@
     <row r="127" spans="1:141" ht="18.95" customHeight="1">
       <c r="A127" s="25"/>
       <c r="B127" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C127" s="47" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D127" s="29"/>
       <c r="E127" s="13"/>
@@ -9829,12 +9821,18 @@
     </row>
     <row r="128" spans="1:141" ht="18.95" customHeight="1">
       <c r="A128" s="25"/>
-      <c r="B128" s="26"/>
+      <c r="B128" s="26">
+        <v>1</v>
+      </c>
       <c r="C128" s="47" t="s">
-        <v>155</v>
-      </c>
-      <c r="D128" s="29"/>
-      <c r="E128" s="13"/>
+        <v>139</v>
+      </c>
+      <c r="D128" s="29">
+        <v>116</v>
+      </c>
+      <c r="E128" s="13">
+        <v>1</v>
+      </c>
       <c r="F128" s="13"/>
       <c r="G128" s="13"/>
       <c r="H128" s="5"/>
@@ -9879,13 +9877,21 @@
       <c r="EK128" s="28"/>
     </row>
     <row r="129" spans="1:141" ht="18.95" customHeight="1">
-      <c r="A129" s="25"/>
-      <c r="B129" s="26"/>
+      <c r="A129" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B129" s="26">
+        <v>1</v>
+      </c>
       <c r="C129" s="47" t="s">
-        <v>156</v>
-      </c>
-      <c r="D129" s="29"/>
-      <c r="E129" s="13"/>
+        <v>74</v>
+      </c>
+      <c r="D129" s="29">
+        <v>112</v>
+      </c>
+      <c r="E129" s="13">
+        <v>1</v>
+      </c>
       <c r="F129" s="13"/>
       <c r="G129" s="13"/>
       <c r="H129" s="5"/>
@@ -9909,7 +9915,6 @@
       <c r="BS129" s="28"/>
       <c r="BY129" s="28"/>
       <c r="BZ129" s="28"/>
-      <c r="CE129" s="38"/>
       <c r="CF129" s="28"/>
       <c r="CG129" s="28"/>
       <c r="CM129" s="28"/>
@@ -9930,14 +9935,26 @@
       <c r="EK129" s="28"/>
     </row>
     <row r="130" spans="1:141" ht="18.95" customHeight="1">
-      <c r="A130" s="25"/>
-      <c r="B130" s="26"/>
-      <c r="C130" s="47"/>
-      <c r="D130" s="29"/>
-      <c r="E130" s="13"/>
+      <c r="A130" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B130" s="26">
+        <v>1</v>
+      </c>
+      <c r="C130" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D130" s="29">
+        <v>113</v>
+      </c>
+      <c r="E130" s="13">
+        <v>4</v>
+      </c>
       <c r="F130" s="13"/>
       <c r="G130" s="13"/>
-      <c r="H130" s="5"/>
+      <c r="H130" s="5">
+        <v>0.5</v>
+      </c>
       <c r="N130" s="28"/>
       <c r="O130" s="28"/>
       <c r="U130" s="28"/>
@@ -9958,7 +9975,6 @@
       <c r="BS130" s="28"/>
       <c r="BY130" s="28"/>
       <c r="BZ130" s="28"/>
-      <c r="CE130" s="38"/>
       <c r="CF130" s="28"/>
       <c r="CG130" s="28"/>
       <c r="CM130" s="28"/>
@@ -9981,7 +9997,9 @@
     <row r="131" spans="1:141" ht="18.95" customHeight="1">
       <c r="A131" s="25"/>
       <c r="B131" s="26"/>
-      <c r="C131" s="47"/>
+      <c r="C131" s="47" t="s">
+        <v>154</v>
+      </c>
       <c r="D131" s="29"/>
       <c r="E131" s="13"/>
       <c r="F131" s="13"/>
@@ -10029,8 +10047,12 @@
     </row>
     <row r="132" spans="1:141" ht="18.95" customHeight="1">
       <c r="A132" s="25"/>
-      <c r="B132" s="26"/>
-      <c r="C132" s="47"/>
+      <c r="B132" s="26">
+        <v>3</v>
+      </c>
+      <c r="C132" s="47" t="s">
+        <v>152</v>
+      </c>
       <c r="D132" s="29"/>
       <c r="E132" s="13"/>
       <c r="F132" s="13"/>
@@ -10079,7 +10101,9 @@
     <row r="133" spans="1:141" ht="18.95" customHeight="1">
       <c r="A133" s="25"/>
       <c r="B133" s="26"/>
-      <c r="C133" s="47"/>
+      <c r="C133" s="47" t="s">
+        <v>155</v>
+      </c>
       <c r="D133" s="29"/>
       <c r="E133" s="13"/>
       <c r="F133" s="13"/>
@@ -10128,7 +10152,9 @@
     <row r="134" spans="1:141" ht="18.95" customHeight="1">
       <c r="A134" s="25"/>
       <c r="B134" s="26"/>
-      <c r="C134" s="47"/>
+      <c r="C134" s="47" t="s">
+        <v>156</v>
+      </c>
       <c r="D134" s="29"/>
       <c r="E134" s="13"/>
       <c r="F134" s="13"/>
@@ -10174,13 +10200,260 @@
       <c r="EJ134" s="28"/>
       <c r="EK134" s="28"/>
     </row>
-    <row r="135" spans="1:141">
-      <c r="A135" s="14"/>
-      <c r="B135" s="14"/>
+    <row r="135" spans="1:141" ht="18.95" customHeight="1">
+      <c r="A135" s="25"/>
+      <c r="B135" s="26"/>
+      <c r="C135" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="D135" s="29"/>
+      <c r="E135" s="13"/>
+      <c r="F135" s="13"/>
+      <c r="G135" s="13"/>
+      <c r="H135" s="5"/>
+      <c r="N135" s="28"/>
+      <c r="O135" s="28"/>
+      <c r="U135" s="28"/>
+      <c r="V135" s="28"/>
+      <c r="AB135" s="28"/>
+      <c r="AC135" s="28"/>
+      <c r="AI135" s="28"/>
+      <c r="AJ135" s="28"/>
+      <c r="AP135" s="28"/>
+      <c r="AQ135" s="28"/>
+      <c r="AW135" s="28"/>
+      <c r="AX135" s="28"/>
+      <c r="BD135" s="28"/>
+      <c r="BE135" s="28"/>
+      <c r="BK135" s="28"/>
+      <c r="BL135" s="28"/>
+      <c r="BR135" s="28"/>
+      <c r="BS135" s="28"/>
+      <c r="BY135" s="28"/>
+      <c r="BZ135" s="28"/>
       <c r="CE135" s="38"/>
-      <c r="CG135" s="38"/>
-      <c r="CI135" s="38"/>
-      <c r="CK135" s="38"/>
+      <c r="CF135" s="28"/>
+      <c r="CG135" s="28"/>
+      <c r="CM135" s="28"/>
+      <c r="CN135" s="28"/>
+      <c r="CT135" s="28"/>
+      <c r="CU135" s="28"/>
+      <c r="DA135" s="28"/>
+      <c r="DB135" s="28"/>
+      <c r="DH135" s="28"/>
+      <c r="DI135" s="28"/>
+      <c r="DO135" s="28"/>
+      <c r="DP135" s="28"/>
+      <c r="DV135" s="28"/>
+      <c r="DW135" s="28"/>
+      <c r="EC135" s="28"/>
+      <c r="ED135" s="28"/>
+      <c r="EJ135" s="28"/>
+      <c r="EK135" s="28"/>
+    </row>
+    <row r="136" spans="1:141" ht="18.95" customHeight="1">
+      <c r="A136" s="25"/>
+      <c r="B136" s="26"/>
+      <c r="C136" s="47"/>
+      <c r="D136" s="29"/>
+      <c r="E136" s="13"/>
+      <c r="F136" s="13"/>
+      <c r="G136" s="13"/>
+      <c r="H136" s="5"/>
+      <c r="N136" s="28"/>
+      <c r="O136" s="28"/>
+      <c r="U136" s="28"/>
+      <c r="V136" s="28"/>
+      <c r="AB136" s="28"/>
+      <c r="AC136" s="28"/>
+      <c r="AI136" s="28"/>
+      <c r="AJ136" s="28"/>
+      <c r="AP136" s="28"/>
+      <c r="AQ136" s="28"/>
+      <c r="AW136" s="28"/>
+      <c r="AX136" s="28"/>
+      <c r="BD136" s="28"/>
+      <c r="BE136" s="28"/>
+      <c r="BK136" s="28"/>
+      <c r="BL136" s="28"/>
+      <c r="BR136" s="28"/>
+      <c r="BS136" s="28"/>
+      <c r="BY136" s="28"/>
+      <c r="BZ136" s="28"/>
+      <c r="CE136" s="38"/>
+      <c r="CF136" s="28"/>
+      <c r="CG136" s="28"/>
+      <c r="CM136" s="28"/>
+      <c r="CN136" s="28"/>
+      <c r="CT136" s="28"/>
+      <c r="CU136" s="28"/>
+      <c r="DA136" s="28"/>
+      <c r="DB136" s="28"/>
+      <c r="DH136" s="28"/>
+      <c r="DI136" s="28"/>
+      <c r="DO136" s="28"/>
+      <c r="DP136" s="28"/>
+      <c r="DV136" s="28"/>
+      <c r="DW136" s="28"/>
+      <c r="EC136" s="28"/>
+      <c r="ED136" s="28"/>
+      <c r="EJ136" s="28"/>
+      <c r="EK136" s="28"/>
+    </row>
+    <row r="137" spans="1:141" ht="18.95" customHeight="1">
+      <c r="A137" s="25"/>
+      <c r="B137" s="26"/>
+      <c r="C137" s="47"/>
+      <c r="D137" s="29"/>
+      <c r="E137" s="13"/>
+      <c r="F137" s="13"/>
+      <c r="G137" s="13"/>
+      <c r="H137" s="5"/>
+      <c r="N137" s="28"/>
+      <c r="O137" s="28"/>
+      <c r="U137" s="28"/>
+      <c r="V137" s="28"/>
+      <c r="AB137" s="28"/>
+      <c r="AC137" s="28"/>
+      <c r="AI137" s="28"/>
+      <c r="AJ137" s="28"/>
+      <c r="AP137" s="28"/>
+      <c r="AQ137" s="28"/>
+      <c r="AW137" s="28"/>
+      <c r="AX137" s="28"/>
+      <c r="BD137" s="28"/>
+      <c r="BE137" s="28"/>
+      <c r="BK137" s="28"/>
+      <c r="BL137" s="28"/>
+      <c r="BR137" s="28"/>
+      <c r="BS137" s="28"/>
+      <c r="BY137" s="28"/>
+      <c r="BZ137" s="28"/>
+      <c r="CE137" s="38"/>
+      <c r="CF137" s="28"/>
+      <c r="CG137" s="28"/>
+      <c r="CM137" s="28"/>
+      <c r="CN137" s="28"/>
+      <c r="CT137" s="28"/>
+      <c r="CU137" s="28"/>
+      <c r="DA137" s="28"/>
+      <c r="DB137" s="28"/>
+      <c r="DH137" s="28"/>
+      <c r="DI137" s="28"/>
+      <c r="DO137" s="28"/>
+      <c r="DP137" s="28"/>
+      <c r="DV137" s="28"/>
+      <c r="DW137" s="28"/>
+      <c r="EC137" s="28"/>
+      <c r="ED137" s="28"/>
+      <c r="EJ137" s="28"/>
+      <c r="EK137" s="28"/>
+    </row>
+    <row r="138" spans="1:141" ht="18.95" customHeight="1">
+      <c r="A138" s="25"/>
+      <c r="B138" s="26"/>
+      <c r="C138" s="47"/>
+      <c r="D138" s="29"/>
+      <c r="E138" s="13"/>
+      <c r="F138" s="13"/>
+      <c r="G138" s="13"/>
+      <c r="H138" s="5"/>
+      <c r="N138" s="28"/>
+      <c r="O138" s="28"/>
+      <c r="U138" s="28"/>
+      <c r="V138" s="28"/>
+      <c r="AB138" s="28"/>
+      <c r="AC138" s="28"/>
+      <c r="AI138" s="28"/>
+      <c r="AJ138" s="28"/>
+      <c r="AP138" s="28"/>
+      <c r="AQ138" s="28"/>
+      <c r="AW138" s="28"/>
+      <c r="AX138" s="28"/>
+      <c r="BD138" s="28"/>
+      <c r="BE138" s="28"/>
+      <c r="BK138" s="28"/>
+      <c r="BL138" s="28"/>
+      <c r="BR138" s="28"/>
+      <c r="BS138" s="28"/>
+      <c r="BY138" s="28"/>
+      <c r="BZ138" s="28"/>
+      <c r="CE138" s="38"/>
+      <c r="CF138" s="28"/>
+      <c r="CG138" s="28"/>
+      <c r="CM138" s="28"/>
+      <c r="CN138" s="28"/>
+      <c r="CT138" s="28"/>
+      <c r="CU138" s="28"/>
+      <c r="DA138" s="28"/>
+      <c r="DB138" s="28"/>
+      <c r="DH138" s="28"/>
+      <c r="DI138" s="28"/>
+      <c r="DO138" s="28"/>
+      <c r="DP138" s="28"/>
+      <c r="DV138" s="28"/>
+      <c r="DW138" s="28"/>
+      <c r="EC138" s="28"/>
+      <c r="ED138" s="28"/>
+      <c r="EJ138" s="28"/>
+      <c r="EK138" s="28"/>
+    </row>
+    <row r="139" spans="1:141" ht="18.95" customHeight="1">
+      <c r="A139" s="25"/>
+      <c r="B139" s="26"/>
+      <c r="C139" s="47"/>
+      <c r="D139" s="29"/>
+      <c r="E139" s="13"/>
+      <c r="F139" s="13"/>
+      <c r="G139" s="13"/>
+      <c r="H139" s="5"/>
+      <c r="N139" s="28"/>
+      <c r="O139" s="28"/>
+      <c r="U139" s="28"/>
+      <c r="V139" s="28"/>
+      <c r="AB139" s="28"/>
+      <c r="AC139" s="28"/>
+      <c r="AI139" s="28"/>
+      <c r="AJ139" s="28"/>
+      <c r="AP139" s="28"/>
+      <c r="AQ139" s="28"/>
+      <c r="AW139" s="28"/>
+      <c r="AX139" s="28"/>
+      <c r="BD139" s="28"/>
+      <c r="BE139" s="28"/>
+      <c r="BK139" s="28"/>
+      <c r="BL139" s="28"/>
+      <c r="BR139" s="28"/>
+      <c r="BS139" s="28"/>
+      <c r="BY139" s="28"/>
+      <c r="BZ139" s="28"/>
+      <c r="CE139" s="38"/>
+      <c r="CF139" s="28"/>
+      <c r="CG139" s="28"/>
+      <c r="CM139" s="28"/>
+      <c r="CN139" s="28"/>
+      <c r="CT139" s="28"/>
+      <c r="CU139" s="28"/>
+      <c r="DA139" s="28"/>
+      <c r="DB139" s="28"/>
+      <c r="DH139" s="28"/>
+      <c r="DI139" s="28"/>
+      <c r="DO139" s="28"/>
+      <c r="DP139" s="28"/>
+      <c r="DV139" s="28"/>
+      <c r="DW139" s="28"/>
+      <c r="EC139" s="28"/>
+      <c r="ED139" s="28"/>
+      <c r="EJ139" s="28"/>
+      <c r="EK139" s="28"/>
+    </row>
+    <row r="140" spans="1:141">
+      <c r="A140" s="14"/>
+      <c r="B140" s="14"/>
+      <c r="CE140" s="38"/>
+      <c r="CG140" s="38"/>
+      <c r="CI140" s="38"/>
+      <c r="CK140" s="38"/>
     </row>
   </sheetData>
   <sortState ref="B101:C109">
@@ -10190,67 +10463,67 @@
     <mergeCell ref="A70:C70"/>
     <mergeCell ref="A2:C4"/>
     <mergeCell ref="A87:C87"/>
-    <mergeCell ref="A120:C120"/>
+    <mergeCell ref="A125:C125"/>
   </mergeCells>
-  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 CO69:CS134 CV60:CZ134 P60:T134 W78:AA134 BT66:BX134 BM66:BQ134 BF66:BJ134 AD8:AH134 AK8:AO134 AR8:AV134 AY8:BC134 CA8:CE134 EE8:EI134 DC8:DG134 DJ8:DN134 DQ8:DU134 J69:M134 CH60:CL134 DY8:EB134 DX8:DX108 DX110:DX134">
-    <cfRule type="expression" dxfId="24" priority="12">
+  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX8:DX108 DX110:DX114 DX115:EB139 DY8:EB114 CH60:CL139 J69:M139 DQ8:DU139 DJ8:DN139 DC8:DG139 EE8:EI139 CA8:CE139 AY8:BC139 AR8:AV139 AK8:AO139 AD8:AH139 BF66:BJ139 BM66:BQ139 BT66:BX139 W78:AA139 P60:T139 CV60:CZ139 CO69:CS139">
+    <cfRule type="expression" dxfId="17" priority="12">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="13">
+    <cfRule type="expression" dxfId="16" priority="13">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="14">
+    <cfRule type="expression" dxfId="15" priority="14">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="16">
+    <cfRule type="expression" dxfId="13" priority="16">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="17">
+    <cfRule type="expression" dxfId="12" priority="17">
       <formula>J$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="18">
+    <cfRule type="expression" dxfId="11" priority="18">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="19">
+    <cfRule type="expression" dxfId="10" priority="19">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A135:EK135">
-    <cfRule type="expression" dxfId="16" priority="11">
+  <conditionalFormatting sqref="A140:EK140">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:EK7">
-    <cfRule type="expression" dxfId="15" priority="10">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>J$7=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL56:CL57">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>CL$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
-Sales comments in BOM complete. -Session's Timeout increased. -Multiple components to RFQ in progress. -EAU as requested by Tom and Seth in progress.
</commit_message>
<xml_diff>
--- a/AQPM Gantt.xlsx
+++ b/AQPM Gantt.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Issues" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'APQM Gantt'!$A$7:$EK$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'APQM Gantt'!$A$7:$EK$129</definedName>
     <definedName name="Actual" localSheetId="0">('APQM Gantt'!PeriodInActual*('APQM Gantt'!$F1&gt;0))*'APQM Gantt'!PeriodInPlan</definedName>
     <definedName name="Actual">(PeriodInActual*(#REF!&gt;0))*PeriodInPlan</definedName>
     <definedName name="ActualBeyond" localSheetId="0">'APQM Gantt'!PeriodInActual*('APQM Gantt'!$F1&gt;0)</definedName>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="165">
   <si>
     <t>Plan</t>
   </si>
@@ -681,6 +681,12 @@
   </si>
   <si>
     <t>Create RFQ per each EAU pulled from SIF requested by Seth and Tom</t>
+  </si>
+  <si>
+    <t>Session timeout increased.</t>
+  </si>
+  <si>
+    <t>Sales comments in BOM</t>
   </si>
 </sst>
 </file>
@@ -1178,134 +1184,6 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0"/>
@@ -1560,6 +1438,134 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1583,15 +1589,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="24">
   <autoFilter ref="A4:F238"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="5"/>
-    <tableColumn id="2" name="Date" dataDxfId="4"/>
-    <tableColumn id="3" name="Creator" dataDxfId="3"/>
-    <tableColumn id="4" name="Issue" dataDxfId="2"/>
-    <tableColumn id="5" name="Status" dataDxfId="1"/>
-    <tableColumn id="6" name="Solution" dataDxfId="0"/>
+    <tableColumn id="1" name="#" dataDxfId="23"/>
+    <tableColumn id="2" name="Date" dataDxfId="22"/>
+    <tableColumn id="3" name="Creator" dataDxfId="21"/>
+    <tableColumn id="4" name="Issue" dataDxfId="20"/>
+    <tableColumn id="5" name="Status" dataDxfId="19"/>
+    <tableColumn id="6" name="Solution" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1827,13 +1833,13 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:EK140"/>
+  <dimension ref="A2:EK142"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="DD112" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <pane xSplit="9" ySplit="7" topLeftCell="DZ105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="DZ129" sqref="DZ129"/>
+      <selection pane="bottomRight" activeCell="H117" sqref="H117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25"/>
@@ -1870,7 +1876,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
@@ -9202,14 +9208,20 @@
     <row r="116" spans="1:141" ht="18.95" customHeight="1">
       <c r="A116" s="25"/>
       <c r="B116" s="26"/>
-      <c r="C116" s="47" t="s">
-        <v>159</v>
+      <c r="C116" s="53" t="s">
+        <v>163</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="13"/>
-      <c r="F116" s="13"/>
-      <c r="G116" s="13"/>
-      <c r="H116" s="5"/>
+      <c r="F116" s="13">
+        <v>130</v>
+      </c>
+      <c r="G116" s="13">
+        <v>1</v>
+      </c>
+      <c r="H116" s="5">
+        <v>1</v>
+      </c>
       <c r="N116" s="28"/>
       <c r="O116" s="28"/>
       <c r="U116" s="28"/>
@@ -9252,17 +9264,21 @@
     </row>
     <row r="117" spans="1:141" ht="18.95" customHeight="1">
       <c r="A117" s="25"/>
-      <c r="B117" s="26">
-        <v>3</v>
-      </c>
-      <c r="C117" s="47" t="s">
-        <v>143</v>
+      <c r="B117" s="26"/>
+      <c r="C117" s="53" t="s">
+        <v>164</v>
       </c>
       <c r="D117" s="29"/>
       <c r="E117" s="13"/>
-      <c r="F117" s="13"/>
-      <c r="G117" s="13"/>
-      <c r="H117" s="5"/>
+      <c r="F117" s="13">
+        <v>130</v>
+      </c>
+      <c r="G117" s="13">
+        <v>1</v>
+      </c>
+      <c r="H117" s="5">
+        <v>1</v>
+      </c>
       <c r="N117" s="28"/>
       <c r="O117" s="28"/>
       <c r="U117" s="28"/>
@@ -9305,18 +9321,12 @@
     </row>
     <row r="118" spans="1:141" ht="18.95" customHeight="1">
       <c r="A118" s="25"/>
-      <c r="B118" s="26">
-        <v>2</v>
-      </c>
+      <c r="B118" s="26"/>
       <c r="C118" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="D118" s="29">
-        <v>116</v>
-      </c>
-      <c r="E118" s="13">
-        <v>1</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="D118" s="29"/>
+      <c r="E118" s="13"/>
       <c r="F118" s="13"/>
       <c r="G118" s="13"/>
       <c r="H118" s="5"/>
@@ -9362,8 +9372,12 @@
     </row>
     <row r="119" spans="1:141" ht="18.95" customHeight="1">
       <c r="A119" s="25"/>
-      <c r="B119" s="26"/>
-      <c r="C119" s="53"/>
+      <c r="B119" s="26">
+        <v>3</v>
+      </c>
+      <c r="C119" s="47" t="s">
+        <v>143</v>
+      </c>
       <c r="D119" s="29"/>
       <c r="E119" s="13"/>
       <c r="F119" s="13"/>
@@ -9411,10 +9425,18 @@
     </row>
     <row r="120" spans="1:141" ht="18.95" customHeight="1">
       <c r="A120" s="25"/>
-      <c r="B120" s="26"/>
-      <c r="C120" s="53"/>
-      <c r="D120" s="29"/>
-      <c r="E120" s="13"/>
+      <c r="B120" s="26">
+        <v>2</v>
+      </c>
+      <c r="C120" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="D120" s="29">
+        <v>116</v>
+      </c>
+      <c r="E120" s="13">
+        <v>1</v>
+      </c>
       <c r="F120" s="13"/>
       <c r="G120" s="13"/>
       <c r="H120" s="5"/>
@@ -9508,11 +9530,9 @@
       <c r="EK121" s="28"/>
     </row>
     <row r="122" spans="1:141" ht="18.95" customHeight="1">
-      <c r="A122" s="55" t="s">
-        <v>148</v>
-      </c>
-      <c r="B122" s="55"/>
-      <c r="C122" s="55"/>
+      <c r="A122" s="25"/>
+      <c r="B122" s="26"/>
+      <c r="C122" s="53"/>
       <c r="D122" s="29"/>
       <c r="E122" s="13"/>
       <c r="F122" s="13"/>
@@ -9560,12 +9580,8 @@
     </row>
     <row r="123" spans="1:141" ht="18.95" customHeight="1">
       <c r="A123" s="25"/>
-      <c r="B123" s="26">
-        <v>2</v>
-      </c>
-      <c r="C123" s="47" t="s">
-        <v>150</v>
-      </c>
+      <c r="B123" s="26"/>
+      <c r="C123" s="53"/>
       <c r="D123" s="29"/>
       <c r="E123" s="13"/>
       <c r="F123" s="13"/>
@@ -9612,13 +9628,11 @@
       <c r="EK123" s="28"/>
     </row>
     <row r="124" spans="1:141" ht="18.95" customHeight="1">
-      <c r="A124" s="25"/>
-      <c r="B124" s="26">
-        <v>2</v>
-      </c>
-      <c r="C124" s="47" t="s">
-        <v>149</v>
-      </c>
+      <c r="A124" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="B124" s="55"/>
+      <c r="C124" s="55"/>
       <c r="D124" s="29"/>
       <c r="E124" s="13"/>
       <c r="F124" s="13"/>
@@ -9667,17 +9681,13 @@
     <row r="125" spans="1:141" ht="18.95" customHeight="1">
       <c r="A125" s="25"/>
       <c r="B125" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C125" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="D125" s="29">
-        <v>116</v>
-      </c>
-      <c r="E125" s="13">
-        <v>1</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="D125" s="29"/>
+      <c r="E125" s="13"/>
       <c r="F125" s="13"/>
       <c r="G125" s="13"/>
       <c r="H125" s="5"/>
@@ -9722,21 +9732,15 @@
       <c r="EK125" s="28"/>
     </row>
     <row r="126" spans="1:141" ht="18.95" customHeight="1">
-      <c r="A126" s="25" t="s">
-        <v>20</v>
-      </c>
+      <c r="A126" s="25"/>
       <c r="B126" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C126" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="D126" s="29">
-        <v>112</v>
-      </c>
-      <c r="E126" s="13">
-        <v>1</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="D126" s="29"/>
+      <c r="E126" s="13"/>
       <c r="F126" s="13"/>
       <c r="G126" s="13"/>
       <c r="H126" s="5"/>
@@ -9760,6 +9764,7 @@
       <c r="BS126" s="28"/>
       <c r="BY126" s="28"/>
       <c r="BZ126" s="28"/>
+      <c r="CE126" s="38"/>
       <c r="CF126" s="28"/>
       <c r="CG126" s="28"/>
       <c r="CM126" s="28"/>
@@ -9780,26 +9785,22 @@
       <c r="EK126" s="28"/>
     </row>
     <row r="127" spans="1:141" ht="18.95" customHeight="1">
-      <c r="A127" s="25" t="s">
-        <v>20</v>
-      </c>
+      <c r="A127" s="25"/>
       <c r="B127" s="26">
         <v>1</v>
       </c>
-      <c r="C127" s="45" t="s">
-        <v>44</v>
+      <c r="C127" s="47" t="s">
+        <v>139</v>
       </c>
       <c r="D127" s="29">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E127" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F127" s="13"/>
       <c r="G127" s="13"/>
-      <c r="H127" s="5">
-        <v>0.5</v>
-      </c>
+      <c r="H127" s="5"/>
       <c r="N127" s="28"/>
       <c r="O127" s="28"/>
       <c r="U127" s="28"/>
@@ -9820,6 +9821,7 @@
       <c r="BS127" s="28"/>
       <c r="BY127" s="28"/>
       <c r="BZ127" s="28"/>
+      <c r="CE127" s="38"/>
       <c r="CF127" s="28"/>
       <c r="CG127" s="28"/>
       <c r="CM127" s="28"/>
@@ -9840,13 +9842,21 @@
       <c r="EK127" s="28"/>
     </row>
     <row r="128" spans="1:141" ht="18.95" customHeight="1">
-      <c r="A128" s="25"/>
-      <c r="B128" s="26"/>
+      <c r="A128" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B128" s="26">
+        <v>1</v>
+      </c>
       <c r="C128" s="47" t="s">
-        <v>154</v>
-      </c>
-      <c r="D128" s="29"/>
-      <c r="E128" s="13"/>
+        <v>74</v>
+      </c>
+      <c r="D128" s="29">
+        <v>112</v>
+      </c>
+      <c r="E128" s="13">
+        <v>1</v>
+      </c>
       <c r="F128" s="13"/>
       <c r="G128" s="13"/>
       <c r="H128" s="5"/>
@@ -9870,7 +9880,6 @@
       <c r="BS128" s="28"/>
       <c r="BY128" s="28"/>
       <c r="BZ128" s="28"/>
-      <c r="CE128" s="38"/>
       <c r="CF128" s="28"/>
       <c r="CG128" s="28"/>
       <c r="CM128" s="28"/>
@@ -9891,18 +9900,26 @@
       <c r="EK128" s="28"/>
     </row>
     <row r="129" spans="1:141" ht="18.95" customHeight="1">
-      <c r="A129" s="25"/>
+      <c r="A129" s="25" t="s">
+        <v>20</v>
+      </c>
       <c r="B129" s="26">
-        <v>3</v>
-      </c>
-      <c r="C129" s="47" t="s">
-        <v>152</v>
-      </c>
-      <c r="D129" s="29"/>
-      <c r="E129" s="13"/>
+        <v>1</v>
+      </c>
+      <c r="C129" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D129" s="29">
+        <v>113</v>
+      </c>
+      <c r="E129" s="13">
+        <v>4</v>
+      </c>
       <c r="F129" s="13"/>
       <c r="G129" s="13"/>
-      <c r="H129" s="5"/>
+      <c r="H129" s="5">
+        <v>0.5</v>
+      </c>
       <c r="N129" s="28"/>
       <c r="O129" s="28"/>
       <c r="U129" s="28"/>
@@ -9923,7 +9940,6 @@
       <c r="BS129" s="28"/>
       <c r="BY129" s="28"/>
       <c r="BZ129" s="28"/>
-      <c r="CE129" s="38"/>
       <c r="CF129" s="28"/>
       <c r="CG129" s="28"/>
       <c r="CM129" s="28"/>
@@ -9947,7 +9963,7 @@
       <c r="A130" s="25"/>
       <c r="B130" s="26"/>
       <c r="C130" s="47" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D130" s="29"/>
       <c r="E130" s="13"/>
@@ -9996,9 +10012,11 @@
     </row>
     <row r="131" spans="1:141" ht="18.95" customHeight="1">
       <c r="A131" s="25"/>
-      <c r="B131" s="26"/>
+      <c r="B131" s="26">
+        <v>3</v>
+      </c>
       <c r="C131" s="47" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="13"/>
@@ -10049,7 +10067,7 @@
       <c r="A132" s="25"/>
       <c r="B132" s="26"/>
       <c r="C132" s="47" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D132" s="29"/>
       <c r="E132" s="13"/>
@@ -10097,21 +10115,13 @@
       <c r="EK132" s="28"/>
     </row>
     <row r="133" spans="1:141" ht="18.95" customHeight="1">
-      <c r="A133" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B133" s="26">
-        <v>1</v>
-      </c>
-      <c r="C133" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="D133" s="29">
-        <v>100</v>
-      </c>
-      <c r="E133" s="13">
-        <v>1</v>
-      </c>
+      <c r="A133" s="25"/>
+      <c r="B133" s="26"/>
+      <c r="C133" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="D133" s="29"/>
+      <c r="E133" s="13"/>
       <c r="F133" s="13"/>
       <c r="G133" s="13"/>
       <c r="H133" s="5"/>
@@ -10135,6 +10145,7 @@
       <c r="BS133" s="28"/>
       <c r="BY133" s="28"/>
       <c r="BZ133" s="28"/>
+      <c r="CE133" s="38"/>
       <c r="CF133" s="28"/>
       <c r="CG133" s="28"/>
       <c r="CM133" s="28"/>
@@ -10158,7 +10169,7 @@
       <c r="A134" s="25"/>
       <c r="B134" s="26"/>
       <c r="C134" s="47" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D134" s="29"/>
       <c r="E134" s="13"/>
@@ -10206,15 +10217,21 @@
       <c r="EK134" s="28"/>
     </row>
     <row r="135" spans="1:141" ht="18.95" customHeight="1">
-      <c r="A135" s="25"/>
+      <c r="A135" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="B135" s="26">
-        <v>3</v>
-      </c>
-      <c r="C135" s="54" t="s">
-        <v>136</v>
-      </c>
-      <c r="D135" s="29"/>
-      <c r="E135" s="13"/>
+        <v>1</v>
+      </c>
+      <c r="C135" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="D135" s="29">
+        <v>100</v>
+      </c>
+      <c r="E135" s="13">
+        <v>1</v>
+      </c>
       <c r="F135" s="13"/>
       <c r="G135" s="13"/>
       <c r="H135" s="5"/>
@@ -10261,7 +10278,7 @@
       <c r="A136" s="25"/>
       <c r="B136" s="26"/>
       <c r="C136" s="47" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D136" s="29"/>
       <c r="E136" s="13"/>
@@ -10310,9 +10327,11 @@
     </row>
     <row r="137" spans="1:141" ht="18.95" customHeight="1">
       <c r="A137" s="25"/>
-      <c r="B137" s="26"/>
-      <c r="C137" s="47" t="s">
-        <v>162</v>
+      <c r="B137" s="26">
+        <v>3</v>
+      </c>
+      <c r="C137" s="54" t="s">
+        <v>136</v>
       </c>
       <c r="D137" s="29"/>
       <c r="E137" s="13"/>
@@ -10339,7 +10358,6 @@
       <c r="BS137" s="28"/>
       <c r="BY137" s="28"/>
       <c r="BZ137" s="28"/>
-      <c r="CE137" s="38"/>
       <c r="CF137" s="28"/>
       <c r="CG137" s="28"/>
       <c r="CM137" s="28"/>
@@ -10362,7 +10380,9 @@
     <row r="138" spans="1:141" ht="18.95" customHeight="1">
       <c r="A138" s="25"/>
       <c r="B138" s="26"/>
-      <c r="C138" s="47"/>
+      <c r="C138" s="47" t="s">
+        <v>157</v>
+      </c>
       <c r="D138" s="29"/>
       <c r="E138" s="13"/>
       <c r="F138" s="13"/>
@@ -10411,7 +10431,9 @@
     <row r="139" spans="1:141" ht="18.95" customHeight="1">
       <c r="A139" s="25"/>
       <c r="B139" s="26"/>
-      <c r="C139" s="47"/>
+      <c r="C139" s="47" t="s">
+        <v>162</v>
+      </c>
       <c r="D139" s="29"/>
       <c r="E139" s="13"/>
       <c r="F139" s="13"/>
@@ -10457,13 +10479,111 @@
       <c r="EJ139" s="28"/>
       <c r="EK139" s="28"/>
     </row>
-    <row r="140" spans="1:141">
-      <c r="A140" s="14"/>
-      <c r="B140" s="14"/>
+    <row r="140" spans="1:141" ht="18.95" customHeight="1">
+      <c r="A140" s="25"/>
+      <c r="B140" s="26"/>
+      <c r="C140" s="47"/>
+      <c r="D140" s="29"/>
+      <c r="E140" s="13"/>
+      <c r="F140" s="13"/>
+      <c r="G140" s="13"/>
+      <c r="H140" s="5"/>
+      <c r="N140" s="28"/>
+      <c r="O140" s="28"/>
+      <c r="U140" s="28"/>
+      <c r="V140" s="28"/>
+      <c r="AB140" s="28"/>
+      <c r="AC140" s="28"/>
+      <c r="AI140" s="28"/>
+      <c r="AJ140" s="28"/>
+      <c r="AP140" s="28"/>
+      <c r="AQ140" s="28"/>
+      <c r="AW140" s="28"/>
+      <c r="AX140" s="28"/>
+      <c r="BD140" s="28"/>
+      <c r="BE140" s="28"/>
+      <c r="BK140" s="28"/>
+      <c r="BL140" s="28"/>
+      <c r="BR140" s="28"/>
+      <c r="BS140" s="28"/>
+      <c r="BY140" s="28"/>
+      <c r="BZ140" s="28"/>
       <c r="CE140" s="38"/>
-      <c r="CG140" s="38"/>
-      <c r="CI140" s="38"/>
-      <c r="CK140" s="38"/>
+      <c r="CF140" s="28"/>
+      <c r="CG140" s="28"/>
+      <c r="CM140" s="28"/>
+      <c r="CN140" s="28"/>
+      <c r="CT140" s="28"/>
+      <c r="CU140" s="28"/>
+      <c r="DA140" s="28"/>
+      <c r="DB140" s="28"/>
+      <c r="DH140" s="28"/>
+      <c r="DI140" s="28"/>
+      <c r="DO140" s="28"/>
+      <c r="DP140" s="28"/>
+      <c r="DV140" s="28"/>
+      <c r="DW140" s="28"/>
+      <c r="EC140" s="28"/>
+      <c r="ED140" s="28"/>
+      <c r="EJ140" s="28"/>
+      <c r="EK140" s="28"/>
+    </row>
+    <row r="141" spans="1:141" ht="18.95" customHeight="1">
+      <c r="A141" s="25"/>
+      <c r="B141" s="26"/>
+      <c r="C141" s="47"/>
+      <c r="D141" s="29"/>
+      <c r="E141" s="13"/>
+      <c r="F141" s="13"/>
+      <c r="G141" s="13"/>
+      <c r="H141" s="5"/>
+      <c r="N141" s="28"/>
+      <c r="O141" s="28"/>
+      <c r="U141" s="28"/>
+      <c r="V141" s="28"/>
+      <c r="AB141" s="28"/>
+      <c r="AC141" s="28"/>
+      <c r="AI141" s="28"/>
+      <c r="AJ141" s="28"/>
+      <c r="AP141" s="28"/>
+      <c r="AQ141" s="28"/>
+      <c r="AW141" s="28"/>
+      <c r="AX141" s="28"/>
+      <c r="BD141" s="28"/>
+      <c r="BE141" s="28"/>
+      <c r="BK141" s="28"/>
+      <c r="BL141" s="28"/>
+      <c r="BR141" s="28"/>
+      <c r="BS141" s="28"/>
+      <c r="BY141" s="28"/>
+      <c r="BZ141" s="28"/>
+      <c r="CE141" s="38"/>
+      <c r="CF141" s="28"/>
+      <c r="CG141" s="28"/>
+      <c r="CM141" s="28"/>
+      <c r="CN141" s="28"/>
+      <c r="CT141" s="28"/>
+      <c r="CU141" s="28"/>
+      <c r="DA141" s="28"/>
+      <c r="DB141" s="28"/>
+      <c r="DH141" s="28"/>
+      <c r="DI141" s="28"/>
+      <c r="DO141" s="28"/>
+      <c r="DP141" s="28"/>
+      <c r="DV141" s="28"/>
+      <c r="DW141" s="28"/>
+      <c r="EC141" s="28"/>
+      <c r="ED141" s="28"/>
+      <c r="EJ141" s="28"/>
+      <c r="EK141" s="28"/>
+    </row>
+    <row r="142" spans="1:141">
+      <c r="A142" s="14"/>
+      <c r="B142" s="14"/>
+      <c r="CE142" s="38"/>
+      <c r="CG142" s="38"/>
+      <c r="CI142" s="38"/>
+      <c r="CK142" s="38"/>
     </row>
   </sheetData>
   <sortState ref="B101:C109">
@@ -10473,67 +10593,67 @@
     <mergeCell ref="A70:C70"/>
     <mergeCell ref="A2:C4"/>
     <mergeCell ref="A86:C86"/>
-    <mergeCell ref="A122:C122"/>
+    <mergeCell ref="A124:C124"/>
   </mergeCells>
-  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 J69:M139 DQ8:DU139 DJ8:DN139 DC8:DG139 EE8:EI139 CA8:CE139 AY8:BC139 AR8:AV139 AK8:AO139 AD8:AH139 BF66:BJ139 BM66:BQ139 BT66:BX139 W78:AA139 P60:T139 CV60:CZ139 CO69:CS139 DX114:EB139 CH60:CL139">
-    <cfRule type="expression" dxfId="24" priority="12">
+  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 J69:M141 DQ8:DU141 DJ8:DN141 DC8:DG141 EE8:EI141 CA8:CE141 AY8:BC141 AR8:AV141 AK8:AO141 AD8:AH141 BF66:BJ141 BM66:BQ141 BT66:BX141 W78:AA141 P60:T141 CV60:CZ141 CO69:CS141 DX114:EB141 CH60:CL141">
+    <cfRule type="expression" dxfId="17" priority="12">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="13">
+    <cfRule type="expression" dxfId="16" priority="13">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="14">
+    <cfRule type="expression" dxfId="15" priority="14">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="16">
+    <cfRule type="expression" dxfId="13" priority="16">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="17">
+    <cfRule type="expression" dxfId="12" priority="17">
       <formula>J$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="18">
+    <cfRule type="expression" dxfId="11" priority="18">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="19">
+    <cfRule type="expression" dxfId="10" priority="19">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A140:EK140">
-    <cfRule type="expression" dxfId="16" priority="11">
+  <conditionalFormatting sqref="A142:EK142">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:EK7">
-    <cfRule type="expression" dxfId="15" priority="10">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>J$7=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL56:CL57">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>CL$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
-Multiple Components to RFQ complete. -EAU funcionality when creating new RFQs complete. -Adding new Lead Time fields to RFQ. -Delete BOM Volume entity. -Cleaning Default page. -Removing old Send New RFQ form.
</commit_message>
<xml_diff>
--- a/AQPM Gantt.xlsx
+++ b/AQPM Gantt.xlsx
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="167">
   <si>
     <t>Plan</t>
   </si>
@@ -690,6 +690,9 @@
   </si>
   <si>
     <t>RFQ form without javascript</t>
+  </si>
+  <si>
+    <t>Manfucaturing Location and Ship fields belongs to RFQ as well</t>
   </si>
 </sst>
 </file>
@@ -1185,1250 +1188,7 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="113">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <fill>
         <patternFill>
@@ -2835,15 +1595,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="24">
   <autoFilter ref="A4:F238"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="111"/>
-    <tableColumn id="2" name="Date" dataDxfId="110"/>
-    <tableColumn id="3" name="Creator" dataDxfId="109"/>
-    <tableColumn id="4" name="Issue" dataDxfId="108"/>
-    <tableColumn id="5" name="Status" dataDxfId="107"/>
-    <tableColumn id="6" name="Solution" dataDxfId="106"/>
+    <tableColumn id="1" name="#" dataDxfId="23"/>
+    <tableColumn id="2" name="Date" dataDxfId="22"/>
+    <tableColumn id="3" name="Creator" dataDxfId="21"/>
+    <tableColumn id="4" name="Issue" dataDxfId="20"/>
+    <tableColumn id="5" name="Status" dataDxfId="19"/>
+    <tableColumn id="6" name="Solution" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3079,13 +1839,13 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:HC142"/>
+  <dimension ref="A2:HC141"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="EA99" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="7" topLeftCell="DM107" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="EI120" sqref="EI120"/>
+      <selection pane="bottomRight" activeCell="DX122" sqref="DX122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25"/>
@@ -3122,7 +1882,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
@@ -10092,7 +8852,7 @@
       <c r="B78" s="26">
         <v>3</v>
       </c>
-      <c r="C78" s="45" t="s">
+      <c r="C78" s="40" t="s">
         <v>78</v>
       </c>
       <c r="D78" s="29">
@@ -10101,9 +8861,15 @@
       <c r="E78" s="13">
         <v>2</v>
       </c>
-      <c r="F78" s="13"/>
-      <c r="G78" s="13"/>
-      <c r="H78" s="5"/>
+      <c r="F78" s="13">
+        <v>133</v>
+      </c>
+      <c r="G78" s="13">
+        <v>3</v>
+      </c>
+      <c r="H78" s="5">
+        <v>1</v>
+      </c>
       <c r="N78" s="28"/>
       <c r="O78" s="28"/>
       <c r="U78" s="28"/>
@@ -13188,14 +11954,20 @@
     <row r="118" spans="1:211" ht="18.95" customHeight="1">
       <c r="A118" s="25"/>
       <c r="B118" s="26"/>
-      <c r="C118" s="47" t="s">
+      <c r="C118" s="53" t="s">
         <v>159</v>
       </c>
       <c r="D118" s="29"/>
       <c r="E118" s="13"/>
-      <c r="F118" s="13"/>
-      <c r="G118" s="13"/>
-      <c r="H118" s="5"/>
+      <c r="F118" s="13">
+        <v>135</v>
+      </c>
+      <c r="G118" s="13">
+        <v>1</v>
+      </c>
+      <c r="H118" s="5">
+        <v>1</v>
+      </c>
       <c r="N118" s="28"/>
       <c r="O118" s="28"/>
       <c r="U118" s="28"/>
@@ -13343,9 +12115,15 @@
       <c r="E120" s="13">
         <v>1</v>
       </c>
-      <c r="F120" s="13"/>
-      <c r="G120" s="13"/>
-      <c r="H120" s="5"/>
+      <c r="F120" s="13">
+        <v>135</v>
+      </c>
+      <c r="G120" s="13">
+        <v>1</v>
+      </c>
+      <c r="H120" s="5">
+        <v>1</v>
+      </c>
       <c r="N120" s="28"/>
       <c r="O120" s="28"/>
       <c r="U120" s="28"/>
@@ -13409,7 +12187,9 @@
     <row r="121" spans="1:211" ht="18.95" customHeight="1">
       <c r="A121" s="25"/>
       <c r="B121" s="26"/>
-      <c r="C121" s="53"/>
+      <c r="C121" s="53" t="s">
+        <v>162</v>
+      </c>
       <c r="D121" s="29"/>
       <c r="E121" s="13"/>
       <c r="F121" s="13"/>
@@ -14718,7 +13498,7 @@
       <c r="A139" s="25"/>
       <c r="B139" s="26"/>
       <c r="C139" s="47" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D139" s="29"/>
       <c r="E139" s="13"/>
@@ -14789,7 +13569,7 @@
       <c r="A140" s="25"/>
       <c r="B140" s="26"/>
       <c r="C140" s="47" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D140" s="29"/>
       <c r="E140" s="13"/>
@@ -14856,82 +13636,13 @@
       <c r="HB140" s="28"/>
       <c r="HC140" s="28"/>
     </row>
-    <row r="141" spans="1:211" ht="18.95" customHeight="1">
-      <c r="A141" s="25"/>
-      <c r="B141" s="26"/>
-      <c r="C141" s="47"/>
-      <c r="D141" s="29"/>
-      <c r="E141" s="13"/>
-      <c r="F141" s="13"/>
-      <c r="G141" s="13"/>
-      <c r="H141" s="5"/>
-      <c r="N141" s="28"/>
-      <c r="O141" s="28"/>
-      <c r="U141" s="28"/>
-      <c r="V141" s="28"/>
-      <c r="AB141" s="28"/>
-      <c r="AC141" s="28"/>
-      <c r="AI141" s="28"/>
-      <c r="AJ141" s="28"/>
-      <c r="AP141" s="28"/>
-      <c r="AQ141" s="28"/>
-      <c r="AW141" s="28"/>
-      <c r="AX141" s="28"/>
-      <c r="BD141" s="28"/>
-      <c r="BE141" s="28"/>
-      <c r="BK141" s="28"/>
-      <c r="BL141" s="28"/>
-      <c r="BR141" s="28"/>
-      <c r="BS141" s="28"/>
-      <c r="BY141" s="28"/>
-      <c r="BZ141" s="28"/>
+    <row r="141" spans="1:211">
+      <c r="A141" s="14"/>
+      <c r="B141" s="14"/>
       <c r="CE141" s="38"/>
-      <c r="CF141" s="28"/>
-      <c r="CG141" s="28"/>
-      <c r="CM141" s="28"/>
-      <c r="CN141" s="28"/>
-      <c r="CT141" s="28"/>
-      <c r="CU141" s="28"/>
-      <c r="DA141" s="28"/>
-      <c r="DB141" s="28"/>
-      <c r="DH141" s="28"/>
-      <c r="DI141" s="28"/>
-      <c r="DO141" s="28"/>
-      <c r="DP141" s="28"/>
-      <c r="DV141" s="28"/>
-      <c r="DW141" s="28"/>
-      <c r="EC141" s="28"/>
-      <c r="ED141" s="28"/>
-      <c r="EJ141" s="28"/>
-      <c r="EK141" s="28"/>
-      <c r="EQ141" s="28"/>
-      <c r="ER141" s="28"/>
-      <c r="EX141" s="28"/>
-      <c r="EY141" s="28"/>
-      <c r="FE141" s="28"/>
-      <c r="FF141" s="28"/>
-      <c r="FL141" s="28"/>
-      <c r="FM141" s="28"/>
-      <c r="FS141" s="28"/>
-      <c r="FT141" s="28"/>
-      <c r="FZ141" s="28"/>
-      <c r="GA141" s="28"/>
-      <c r="GG141" s="28"/>
-      <c r="GH141" s="28"/>
-      <c r="GN141" s="28"/>
-      <c r="GO141" s="28"/>
-      <c r="GU141" s="28"/>
-      <c r="GV141" s="28"/>
-      <c r="HB141" s="28"/>
-      <c r="HC141" s="28"/>
-    </row>
-    <row r="142" spans="1:211">
-      <c r="A142" s="14"/>
-      <c r="B142" s="14"/>
-      <c r="CE142" s="38"/>
-      <c r="CG142" s="38"/>
-      <c r="CI142" s="38"/>
-      <c r="CK142" s="38"/>
+      <c r="CG141" s="38"/>
+      <c r="CI141" s="38"/>
+      <c r="CK141" s="38"/>
     </row>
   </sheetData>
   <sortState ref="B101:C109">
@@ -14943,325 +13654,65 @@
     <mergeCell ref="A86:C86"/>
     <mergeCell ref="A124:C124"/>
   </mergeCells>
-  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 J69:M141 DQ8:DU141 DJ8:DN141 DC8:DG141 EE8:EI141 CA8:CE141 AY8:BC141 AR8:AV141 AK8:AO141 AD8:AH141 BF66:BJ141 BM66:BQ141 BT66:BX141 W78:AA141 P60:T141 CV60:CZ141 CO69:CS141 DX114:EB141 CH60:CL141">
-    <cfRule type="expression" dxfId="105" priority="92">
+  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 J69:M140 DQ8:DU140 DJ8:DN140 DC8:DG140 EE8:EI140 CA8:CE140 AY8:BC140 AR8:AV140 AK8:AO140 AD8:AH140 BF66:BJ140 BM66:BQ140 BT66:BX140 W78:AA140 P60:T140 CV60:CZ140 CO69:CS140 DX114:EB140 CH60:CL140 EL8:EP140 ES8:EW140 EZ8:FD140 FG8:FK140 FN8:FR140 FU8:FY140 GB8:GF140 GI8:GM140 GP8:GT140 GW8:HA140">
+    <cfRule type="expression" dxfId="17" priority="92">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="93">
+    <cfRule type="expression" dxfId="16" priority="93">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="94">
+    <cfRule type="expression" dxfId="15" priority="94">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="95">
+    <cfRule type="expression" dxfId="14" priority="95">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="96">
+    <cfRule type="expression" dxfId="13" priority="96">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="97">
+    <cfRule type="expression" dxfId="12" priority="97">
       <formula>J$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="98">
+    <cfRule type="expression" dxfId="11" priority="98">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="99">
+    <cfRule type="expression" dxfId="10" priority="99">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A142:HC142">
-    <cfRule type="expression" dxfId="97" priority="91">
+  <conditionalFormatting sqref="A141:HC141">
+    <cfRule type="expression" dxfId="9" priority="91">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:HC7">
-    <cfRule type="expression" dxfId="96" priority="90">
+    <cfRule type="expression" dxfId="8" priority="90">
       <formula>J$7=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL56:CL57">
-    <cfRule type="expression" dxfId="95" priority="81">
+    <cfRule type="expression" dxfId="7" priority="81">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="82">
+    <cfRule type="expression" dxfId="6" priority="82">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="83">
+    <cfRule type="expression" dxfId="5" priority="83">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="84">
+    <cfRule type="expression" dxfId="4" priority="84">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="85">
+    <cfRule type="expression" dxfId="3" priority="85">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="86">
+    <cfRule type="expression" dxfId="2" priority="86">
       <formula>CL$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="87">
+    <cfRule type="expression" dxfId="1" priority="87">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="88">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="EL8:EP141">
-    <cfRule type="expression" dxfId="87" priority="73">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="86" priority="74">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="75">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="84" priority="76">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="83" priority="77">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="78">
-      <formula>EL$7=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="79">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="80" priority="80">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="ES8:EW141">
-    <cfRule type="expression" dxfId="79" priority="65">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="78" priority="66">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="77" priority="67">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="68">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="75" priority="69">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="74" priority="70">
-      <formula>ES$7=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="73" priority="71">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="72">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="EZ8:FD141">
-    <cfRule type="expression" dxfId="71" priority="57">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="58">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="69" priority="59">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="68" priority="60">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="61">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="62">
-      <formula>EZ$7=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="63">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="64">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="FG8:FK141">
-    <cfRule type="expression" dxfId="63" priority="49">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="50">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="61" priority="51">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="60" priority="52">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="53">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="54">
-      <formula>FG$7=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="55">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="56">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="FN8:FR141">
-    <cfRule type="expression" dxfId="55" priority="41">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="42">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="53" priority="43">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="44">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="51" priority="45">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="50" priority="46">
-      <formula>FN$7=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="49" priority="47">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="48">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="FU8:FY141">
-    <cfRule type="expression" dxfId="47" priority="33">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="34">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="35">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="36">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="37">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="38">
-      <formula>FU$7=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="39">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="40">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="GB8:GF141">
-    <cfRule type="expression" dxfId="39" priority="25">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="26">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="27">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="28">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="29">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="30">
-      <formula>GB$7=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="31">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="32">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="GI8:GM141">
-    <cfRule type="expression" dxfId="31" priority="17">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="18">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="19">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="20">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="21">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="22">
-      <formula>GI$7=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="23">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="24">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="GP8:GT141">
-    <cfRule type="expression" dxfId="23" priority="9">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="10">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="11">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="12">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="13">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="14">
-      <formula>GP$7=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="15">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="16">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="GW8:HA141">
-    <cfRule type="expression" dxfId="7" priority="1">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
-      <formula>GW$7=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="0" priority="88">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Editing RFQ Buyer side complete
</commit_message>
<xml_diff>
--- a/AQPM Gantt.xlsx
+++ b/AQPM Gantt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10305" yWindow="4335" windowWidth="10230" windowHeight="4350"/>
+    <workbookView xWindow="10305" yWindow="4335" windowWidth="10230" windowHeight="4350" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="APQM Gantt" sheetId="2" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="169">
   <si>
     <t>Plan</t>
   </si>
@@ -693,6 +693,12 @@
   </si>
   <si>
     <t>Manfucaturing Location and Ship fields belongs to RFQ as well</t>
+  </si>
+  <si>
+    <t>Magdeline</t>
+  </si>
+  <si>
+    <t>Supplier is adding by itself when creating RFQs.</t>
   </si>
 </sst>
 </file>
@@ -1190,6 +1196,134 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0"/>
@@ -1444,134 +1578,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1595,15 +1601,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A4:F238"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="23"/>
-    <tableColumn id="2" name="Date" dataDxfId="22"/>
-    <tableColumn id="3" name="Creator" dataDxfId="21"/>
-    <tableColumn id="4" name="Issue" dataDxfId="20"/>
-    <tableColumn id="5" name="Status" dataDxfId="19"/>
-    <tableColumn id="6" name="Solution" dataDxfId="18"/>
+    <tableColumn id="1" name="#" dataDxfId="5"/>
+    <tableColumn id="2" name="Date" dataDxfId="4"/>
+    <tableColumn id="3" name="Creator" dataDxfId="3"/>
+    <tableColumn id="4" name="Issue" dataDxfId="2"/>
+    <tableColumn id="5" name="Status" dataDxfId="1"/>
+    <tableColumn id="6" name="Solution" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1841,11 +1847,11 @@
   </sheetPr>
   <dimension ref="A2:HC141"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="DM107" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <pane xSplit="9" ySplit="7" topLeftCell="DM119" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="DX122" sqref="DX122"/>
+      <selection pane="bottomRight" activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25"/>
@@ -13655,64 +13661,64 @@
     <mergeCell ref="A124:C124"/>
   </mergeCells>
   <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 J69:M140 DQ8:DU140 DJ8:DN140 DC8:DG140 EE8:EI140 CA8:CE140 AY8:BC140 AR8:AV140 AK8:AO140 AD8:AH140 BF66:BJ140 BM66:BQ140 BT66:BX140 W78:AA140 P60:T140 CV60:CZ140 CO69:CS140 DX114:EB140 CH60:CL140 EL8:EP140 ES8:EW140 EZ8:FD140 FG8:FK140 FN8:FR140 FU8:FY140 GB8:GF140 GI8:GM140 GP8:GT140 GW8:HA140">
-    <cfRule type="expression" dxfId="17" priority="92">
+    <cfRule type="expression" dxfId="24" priority="92">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="93">
+    <cfRule type="expression" dxfId="23" priority="93">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="94">
+    <cfRule type="expression" dxfId="22" priority="94">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="95">
+    <cfRule type="expression" dxfId="21" priority="95">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="96">
+    <cfRule type="expression" dxfId="20" priority="96">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="97">
+    <cfRule type="expression" dxfId="19" priority="97">
       <formula>J$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="98">
+    <cfRule type="expression" dxfId="18" priority="98">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="99">
+    <cfRule type="expression" dxfId="17" priority="99">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A141:HC141">
-    <cfRule type="expression" dxfId="9" priority="91">
+    <cfRule type="expression" dxfId="16" priority="91">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:HC7">
-    <cfRule type="expression" dxfId="8" priority="90">
+    <cfRule type="expression" dxfId="15" priority="90">
       <formula>J$7=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL56:CL57">
-    <cfRule type="expression" dxfId="7" priority="81">
+    <cfRule type="expression" dxfId="14" priority="81">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="82">
+    <cfRule type="expression" dxfId="13" priority="82">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="83">
+    <cfRule type="expression" dxfId="12" priority="83">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="84">
+    <cfRule type="expression" dxfId="11" priority="84">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="85">
+    <cfRule type="expression" dxfId="10" priority="85">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="86">
+    <cfRule type="expression" dxfId="9" priority="86">
       <formula>CL$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="87">
+    <cfRule type="expression" dxfId="8" priority="87">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="88">
+    <cfRule type="expression" dxfId="7" priority="88">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13726,9 +13732,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AO238"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13798,6 +13804,15 @@
     <row r="6" spans="1:41">
       <c r="A6" s="36">
         <v>2</v>
+      </c>
+      <c r="B6" s="33">
+        <v>41690</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>168</v>
       </c>
       <c r="AO6" s="35" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
-HTML report to sales with all RFQs done. -Multiplying EAU with Qty required when creating new RFQs.
</commit_message>
<xml_diff>
--- a/AQPM Gantt.xlsx
+++ b/AQPM Gantt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10305" yWindow="4335" windowWidth="10230" windowHeight="4350" activeTab="1"/>
+    <workbookView xWindow="10305" yWindow="4335" windowWidth="10230" windowHeight="4350"/>
   </bookViews>
   <sheets>
     <sheet name="APQM Gantt" sheetId="2" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="176">
   <si>
     <t>Plan</t>
   </si>
@@ -617,9 +617,6 @@
     <t>Delete BOM from SIF list.</t>
   </si>
   <si>
-    <t>Add Prototype Tooling and Prototype quantity to RFQ Summary (by Martha)</t>
-  </si>
-  <si>
     <t>Remove Multiview controls, instead, use normal webpages.</t>
   </si>
   <si>
@@ -647,9 +644,6 @@
     <t>Use FS Commodities.</t>
   </si>
   <si>
-    <t>Ordered by Actual Start. LMD: 1/30/2014</t>
-  </si>
-  <si>
     <t>Leyend when sending RFQ depending id Aerospacial or Automotive</t>
   </si>
   <si>
@@ -699,6 +693,33 @@
   </si>
   <si>
     <t>Supplier is adding by itself when creating RFQs.</t>
+  </si>
+  <si>
+    <t>Don’t delete records, just set to inactive</t>
+  </si>
+  <si>
+    <t>Close RFQ after  hiting save or cancel</t>
+  </si>
+  <si>
+    <t>Remove from SIF List column Cost Model Loc</t>
+  </si>
+  <si>
+    <t>Brand and Revision level uppercase</t>
+  </si>
+  <si>
+    <t>UM in Report to Sales</t>
+  </si>
+  <si>
+    <t>Days/Wks for Lead Times</t>
+  </si>
+  <si>
+    <t>Handle manual process by attaching in SIF</t>
+  </si>
+  <si>
+    <t>Add Prototype Tooling and Prototype quantity to RFQ Summary</t>
+  </si>
+  <si>
+    <t>Ordered by Actual Start. LMD: 2/24/2014</t>
   </si>
 </sst>
 </file>
@@ -1196,134 +1217,6 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0"/>
@@ -1578,6 +1471,134 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1601,15 +1622,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="24">
   <autoFilter ref="A4:F238"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="5"/>
-    <tableColumn id="2" name="Date" dataDxfId="4"/>
-    <tableColumn id="3" name="Creator" dataDxfId="3"/>
-    <tableColumn id="4" name="Issue" dataDxfId="2"/>
-    <tableColumn id="5" name="Status" dataDxfId="1"/>
-    <tableColumn id="6" name="Solution" dataDxfId="0"/>
+    <tableColumn id="1" name="#" dataDxfId="23"/>
+    <tableColumn id="2" name="Date" dataDxfId="22"/>
+    <tableColumn id="3" name="Creator" dataDxfId="21"/>
+    <tableColumn id="4" name="Issue" dataDxfId="20"/>
+    <tableColumn id="5" name="Status" dataDxfId="19"/>
+    <tableColumn id="6" name="Solution" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1845,13 +1866,13 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:HC141"/>
+  <dimension ref="A2:HC152"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="DM119" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <pane xSplit="9" ySplit="7" topLeftCell="J118" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="C122" sqref="C122"/>
+      <selection pane="bottomRight" activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25"/>
@@ -1925,7 +1946,7 @@
     </row>
     <row r="5" spans="1:211" ht="28.5">
       <c r="A5" s="17" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="15"/>
@@ -11099,7 +11120,7 @@
         <v>2</v>
       </c>
       <c r="C107" s="53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D107" s="29"/>
       <c r="E107" s="13"/>
@@ -11178,7 +11199,7 @@
         <v>3</v>
       </c>
       <c r="C108" s="53" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D108" s="29"/>
       <c r="E108" s="13"/>
@@ -11335,7 +11356,7 @@
       <c r="A110" s="25"/>
       <c r="B110" s="26"/>
       <c r="C110" s="53" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D110" s="29"/>
       <c r="E110" s="13"/>
@@ -11414,7 +11435,7 @@
         <v>3</v>
       </c>
       <c r="C111" s="53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D111" s="29"/>
       <c r="E111" s="13"/>
@@ -11491,7 +11512,7 @@
       <c r="A112" s="25"/>
       <c r="B112" s="26"/>
       <c r="C112" s="53" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D112" s="29"/>
       <c r="E112" s="13"/>
@@ -11651,7 +11672,7 @@
       <c r="A114" s="25"/>
       <c r="B114" s="26"/>
       <c r="C114" s="53" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D114" s="29"/>
       <c r="E114" s="13"/>
@@ -11728,7 +11749,7 @@
       <c r="A115" s="25"/>
       <c r="B115" s="26"/>
       <c r="C115" s="53" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="13">
@@ -11807,7 +11828,7 @@
       <c r="A116" s="25"/>
       <c r="B116" s="26"/>
       <c r="C116" s="53" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="13"/>
@@ -11884,7 +11905,7 @@
       <c r="A117" s="25"/>
       <c r="B117" s="26"/>
       <c r="C117" s="53" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D117" s="29"/>
       <c r="E117" s="13"/>
@@ -11961,7 +11982,7 @@
       <c r="A118" s="25"/>
       <c r="B118" s="26"/>
       <c r="C118" s="53" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D118" s="29"/>
       <c r="E118" s="13"/>
@@ -12040,7 +12061,7 @@
         <v>3</v>
       </c>
       <c r="C119" s="47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="13"/>
@@ -12113,7 +12134,7 @@
         <v>2</v>
       </c>
       <c r="C120" s="47" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
       <c r="D120" s="29">
         <v>116</v>
@@ -12194,7 +12215,7 @@
       <c r="A121" s="25"/>
       <c r="B121" s="26"/>
       <c r="C121" s="53" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="13"/>
@@ -12401,7 +12422,7 @@
     </row>
     <row r="124" spans="1:211" ht="18.95" customHeight="1">
       <c r="A124" s="55" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B124" s="55"/>
       <c r="C124" s="55"/>
@@ -12476,7 +12497,7 @@
         <v>2</v>
       </c>
       <c r="C125" s="47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D125" s="29"/>
       <c r="E125" s="13"/>
@@ -12549,7 +12570,7 @@
         <v>2</v>
       </c>
       <c r="C126" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D126" s="29"/>
       <c r="E126" s="13"/>
@@ -12855,7 +12876,7 @@
       <c r="A130" s="25"/>
       <c r="B130" s="26"/>
       <c r="C130" s="47" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D130" s="29"/>
       <c r="E130" s="13"/>
@@ -12928,7 +12949,7 @@
         <v>3</v>
       </c>
       <c r="C131" s="47" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="13"/>
@@ -12999,7 +13020,7 @@
       <c r="A132" s="25"/>
       <c r="B132" s="26"/>
       <c r="C132" s="47" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D132" s="29"/>
       <c r="E132" s="13"/>
@@ -13070,7 +13091,7 @@
       <c r="A133" s="25"/>
       <c r="B133" s="26"/>
       <c r="C133" s="47" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D133" s="29"/>
       <c r="E133" s="13"/>
@@ -13141,7 +13162,7 @@
       <c r="A134" s="25"/>
       <c r="B134" s="26"/>
       <c r="C134" s="47" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D134" s="29"/>
       <c r="E134" s="13"/>
@@ -13290,7 +13311,7 @@
       <c r="A136" s="25"/>
       <c r="B136" s="26"/>
       <c r="C136" s="47" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D136" s="29"/>
       <c r="E136" s="13"/>
@@ -13433,7 +13454,7 @@
       <c r="A138" s="25"/>
       <c r="B138" s="26"/>
       <c r="C138" s="47" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D138" s="29"/>
       <c r="E138" s="13"/>
@@ -13504,7 +13525,7 @@
       <c r="A139" s="25"/>
       <c r="B139" s="26"/>
       <c r="C139" s="47" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D139" s="29"/>
       <c r="E139" s="13"/>
@@ -13575,7 +13596,7 @@
       <c r="A140" s="25"/>
       <c r="B140" s="26"/>
       <c r="C140" s="47" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D140" s="29"/>
       <c r="E140" s="13"/>
@@ -13642,13 +13663,786 @@
       <c r="HB140" s="28"/>
       <c r="HC140" s="28"/>
     </row>
-    <row r="141" spans="1:211">
-      <c r="A141" s="14"/>
-      <c r="B141" s="14"/>
+    <row r="141" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A141" s="25"/>
+      <c r="B141" s="26"/>
+      <c r="C141" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="D141" s="29"/>
+      <c r="E141" s="13"/>
+      <c r="F141" s="13"/>
+      <c r="G141" s="13"/>
+      <c r="H141" s="5"/>
+      <c r="N141" s="28"/>
+      <c r="O141" s="28"/>
+      <c r="U141" s="28"/>
+      <c r="V141" s="28"/>
+      <c r="AB141" s="28"/>
+      <c r="AC141" s="28"/>
+      <c r="AI141" s="28"/>
+      <c r="AJ141" s="28"/>
+      <c r="AP141" s="28"/>
+      <c r="AQ141" s="28"/>
+      <c r="AW141" s="28"/>
+      <c r="AX141" s="28"/>
+      <c r="BD141" s="28"/>
+      <c r="BE141" s="28"/>
+      <c r="BK141" s="28"/>
+      <c r="BL141" s="28"/>
+      <c r="BR141" s="28"/>
+      <c r="BS141" s="28"/>
+      <c r="BY141" s="28"/>
+      <c r="BZ141" s="28"/>
       <c r="CE141" s="38"/>
-      <c r="CG141" s="38"/>
-      <c r="CI141" s="38"/>
-      <c r="CK141" s="38"/>
+      <c r="CF141" s="28"/>
+      <c r="CG141" s="28"/>
+      <c r="CM141" s="28"/>
+      <c r="CN141" s="28"/>
+      <c r="CT141" s="28"/>
+      <c r="CU141" s="28"/>
+      <c r="DA141" s="28"/>
+      <c r="DB141" s="28"/>
+      <c r="DH141" s="28"/>
+      <c r="DI141" s="28"/>
+      <c r="DO141" s="28"/>
+      <c r="DP141" s="28"/>
+      <c r="DV141" s="28"/>
+      <c r="DW141" s="28"/>
+      <c r="EC141" s="28"/>
+      <c r="ED141" s="28"/>
+      <c r="EJ141" s="28"/>
+      <c r="EK141" s="28"/>
+      <c r="EQ141" s="28"/>
+      <c r="ER141" s="28"/>
+      <c r="EX141" s="28"/>
+      <c r="EY141" s="28"/>
+      <c r="FE141" s="28"/>
+      <c r="FF141" s="28"/>
+      <c r="FL141" s="28"/>
+      <c r="FM141" s="28"/>
+      <c r="FS141" s="28"/>
+      <c r="FT141" s="28"/>
+      <c r="FZ141" s="28"/>
+      <c r="GA141" s="28"/>
+      <c r="GG141" s="28"/>
+      <c r="GH141" s="28"/>
+      <c r="GN141" s="28"/>
+      <c r="GO141" s="28"/>
+      <c r="GU141" s="28"/>
+      <c r="GV141" s="28"/>
+      <c r="HB141" s="28"/>
+      <c r="HC141" s="28"/>
+    </row>
+    <row r="142" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A142" s="25"/>
+      <c r="B142" s="26"/>
+      <c r="C142" s="47" t="s">
+        <v>171</v>
+      </c>
+      <c r="D142" s="29"/>
+      <c r="E142" s="13"/>
+      <c r="F142" s="13"/>
+      <c r="G142" s="13"/>
+      <c r="H142" s="5"/>
+      <c r="N142" s="28"/>
+      <c r="O142" s="28"/>
+      <c r="U142" s="28"/>
+      <c r="V142" s="28"/>
+      <c r="AB142" s="28"/>
+      <c r="AC142" s="28"/>
+      <c r="AI142" s="28"/>
+      <c r="AJ142" s="28"/>
+      <c r="AP142" s="28"/>
+      <c r="AQ142" s="28"/>
+      <c r="AW142" s="28"/>
+      <c r="AX142" s="28"/>
+      <c r="BD142" s="28"/>
+      <c r="BE142" s="28"/>
+      <c r="BK142" s="28"/>
+      <c r="BL142" s="28"/>
+      <c r="BR142" s="28"/>
+      <c r="BS142" s="28"/>
+      <c r="BY142" s="28"/>
+      <c r="BZ142" s="28"/>
+      <c r="CE142" s="38"/>
+      <c r="CF142" s="28"/>
+      <c r="CG142" s="28"/>
+      <c r="CM142" s="28"/>
+      <c r="CN142" s="28"/>
+      <c r="CT142" s="28"/>
+      <c r="CU142" s="28"/>
+      <c r="DA142" s="28"/>
+      <c r="DB142" s="28"/>
+      <c r="DH142" s="28"/>
+      <c r="DI142" s="28"/>
+      <c r="DO142" s="28"/>
+      <c r="DP142" s="28"/>
+      <c r="DV142" s="28"/>
+      <c r="DW142" s="28"/>
+      <c r="EC142" s="28"/>
+      <c r="ED142" s="28"/>
+      <c r="EJ142" s="28"/>
+      <c r="EK142" s="28"/>
+      <c r="EQ142" s="28"/>
+      <c r="ER142" s="28"/>
+      <c r="EX142" s="28"/>
+      <c r="EY142" s="28"/>
+      <c r="FE142" s="28"/>
+      <c r="FF142" s="28"/>
+      <c r="FL142" s="28"/>
+      <c r="FM142" s="28"/>
+      <c r="FS142" s="28"/>
+      <c r="FT142" s="28"/>
+      <c r="FZ142" s="28"/>
+      <c r="GA142" s="28"/>
+      <c r="GG142" s="28"/>
+      <c r="GH142" s="28"/>
+      <c r="GN142" s="28"/>
+      <c r="GO142" s="28"/>
+      <c r="GU142" s="28"/>
+      <c r="GV142" s="28"/>
+      <c r="HB142" s="28"/>
+      <c r="HC142" s="28"/>
+    </row>
+    <row r="143" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A143" s="25"/>
+      <c r="B143" s="26"/>
+      <c r="C143" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="D143" s="29"/>
+      <c r="E143" s="13"/>
+      <c r="F143" s="13"/>
+      <c r="G143" s="13"/>
+      <c r="H143" s="5"/>
+      <c r="N143" s="28"/>
+      <c r="O143" s="28"/>
+      <c r="U143" s="28"/>
+      <c r="V143" s="28"/>
+      <c r="AB143" s="28"/>
+      <c r="AC143" s="28"/>
+      <c r="AI143" s="28"/>
+      <c r="AJ143" s="28"/>
+      <c r="AP143" s="28"/>
+      <c r="AQ143" s="28"/>
+      <c r="AW143" s="28"/>
+      <c r="AX143" s="28"/>
+      <c r="BD143" s="28"/>
+      <c r="BE143" s="28"/>
+      <c r="BK143" s="28"/>
+      <c r="BL143" s="28"/>
+      <c r="BR143" s="28"/>
+      <c r="BS143" s="28"/>
+      <c r="BY143" s="28"/>
+      <c r="BZ143" s="28"/>
+      <c r="CE143" s="38"/>
+      <c r="CF143" s="28"/>
+      <c r="CG143" s="28"/>
+      <c r="CM143" s="28"/>
+      <c r="CN143" s="28"/>
+      <c r="CT143" s="28"/>
+      <c r="CU143" s="28"/>
+      <c r="DA143" s="28"/>
+      <c r="DB143" s="28"/>
+      <c r="DH143" s="28"/>
+      <c r="DI143" s="28"/>
+      <c r="DO143" s="28"/>
+      <c r="DP143" s="28"/>
+      <c r="DV143" s="28"/>
+      <c r="DW143" s="28"/>
+      <c r="EC143" s="28"/>
+      <c r="ED143" s="28"/>
+      <c r="EJ143" s="28"/>
+      <c r="EK143" s="28"/>
+      <c r="EQ143" s="28"/>
+      <c r="ER143" s="28"/>
+      <c r="EX143" s="28"/>
+      <c r="EY143" s="28"/>
+      <c r="FE143" s="28"/>
+      <c r="FF143" s="28"/>
+      <c r="FL143" s="28"/>
+      <c r="FM143" s="28"/>
+      <c r="FS143" s="28"/>
+      <c r="FT143" s="28"/>
+      <c r="FZ143" s="28"/>
+      <c r="GA143" s="28"/>
+      <c r="GG143" s="28"/>
+      <c r="GH143" s="28"/>
+      <c r="GN143" s="28"/>
+      <c r="GO143" s="28"/>
+      <c r="GU143" s="28"/>
+      <c r="GV143" s="28"/>
+      <c r="HB143" s="28"/>
+      <c r="HC143" s="28"/>
+    </row>
+    <row r="144" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A144" s="25"/>
+      <c r="B144" s="26"/>
+      <c r="C144" s="47" t="s">
+        <v>173</v>
+      </c>
+      <c r="D144" s="29"/>
+      <c r="E144" s="13"/>
+      <c r="F144" s="13"/>
+      <c r="G144" s="13"/>
+      <c r="H144" s="5"/>
+      <c r="N144" s="28"/>
+      <c r="O144" s="28"/>
+      <c r="U144" s="28"/>
+      <c r="V144" s="28"/>
+      <c r="AB144" s="28"/>
+      <c r="AC144" s="28"/>
+      <c r="AI144" s="28"/>
+      <c r="AJ144" s="28"/>
+      <c r="AP144" s="28"/>
+      <c r="AQ144" s="28"/>
+      <c r="AW144" s="28"/>
+      <c r="AX144" s="28"/>
+      <c r="BD144" s="28"/>
+      <c r="BE144" s="28"/>
+      <c r="BK144" s="28"/>
+      <c r="BL144" s="28"/>
+      <c r="BR144" s="28"/>
+      <c r="BS144" s="28"/>
+      <c r="BY144" s="28"/>
+      <c r="BZ144" s="28"/>
+      <c r="CE144" s="38"/>
+      <c r="CF144" s="28"/>
+      <c r="CG144" s="28"/>
+      <c r="CM144" s="28"/>
+      <c r="CN144" s="28"/>
+      <c r="CT144" s="28"/>
+      <c r="CU144" s="28"/>
+      <c r="DA144" s="28"/>
+      <c r="DB144" s="28"/>
+      <c r="DH144" s="28"/>
+      <c r="DI144" s="28"/>
+      <c r="DO144" s="28"/>
+      <c r="DP144" s="28"/>
+      <c r="DV144" s="28"/>
+      <c r="DW144" s="28"/>
+      <c r="EC144" s="28"/>
+      <c r="ED144" s="28"/>
+      <c r="EJ144" s="28"/>
+      <c r="EK144" s="28"/>
+      <c r="EQ144" s="28"/>
+      <c r="ER144" s="28"/>
+      <c r="EX144" s="28"/>
+      <c r="EY144" s="28"/>
+      <c r="FE144" s="28"/>
+      <c r="FF144" s="28"/>
+      <c r="FL144" s="28"/>
+      <c r="FM144" s="28"/>
+      <c r="FS144" s="28"/>
+      <c r="FT144" s="28"/>
+      <c r="FZ144" s="28"/>
+      <c r="GA144" s="28"/>
+      <c r="GG144" s="28"/>
+      <c r="GH144" s="28"/>
+      <c r="GN144" s="28"/>
+      <c r="GO144" s="28"/>
+      <c r="GU144" s="28"/>
+      <c r="GV144" s="28"/>
+      <c r="HB144" s="28"/>
+      <c r="HC144" s="28"/>
+    </row>
+    <row r="145" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A145" s="25"/>
+      <c r="B145" s="26"/>
+      <c r="C145" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="D145" s="29"/>
+      <c r="E145" s="13"/>
+      <c r="F145" s="13"/>
+      <c r="G145" s="13"/>
+      <c r="H145" s="5"/>
+      <c r="N145" s="28"/>
+      <c r="O145" s="28"/>
+      <c r="U145" s="28"/>
+      <c r="V145" s="28"/>
+      <c r="AB145" s="28"/>
+      <c r="AC145" s="28"/>
+      <c r="AI145" s="28"/>
+      <c r="AJ145" s="28"/>
+      <c r="AP145" s="28"/>
+      <c r="AQ145" s="28"/>
+      <c r="AW145" s="28"/>
+      <c r="AX145" s="28"/>
+      <c r="BD145" s="28"/>
+      <c r="BE145" s="28"/>
+      <c r="BK145" s="28"/>
+      <c r="BL145" s="28"/>
+      <c r="BR145" s="28"/>
+      <c r="BS145" s="28"/>
+      <c r="BY145" s="28"/>
+      <c r="BZ145" s="28"/>
+      <c r="CE145" s="38"/>
+      <c r="CF145" s="28"/>
+      <c r="CG145" s="28"/>
+      <c r="CM145" s="28"/>
+      <c r="CN145" s="28"/>
+      <c r="CT145" s="28"/>
+      <c r="CU145" s="28"/>
+      <c r="DA145" s="28"/>
+      <c r="DB145" s="28"/>
+      <c r="DH145" s="28"/>
+      <c r="DI145" s="28"/>
+      <c r="DO145" s="28"/>
+      <c r="DP145" s="28"/>
+      <c r="DV145" s="28"/>
+      <c r="DW145" s="28"/>
+      <c r="EC145" s="28"/>
+      <c r="ED145" s="28"/>
+      <c r="EJ145" s="28"/>
+      <c r="EK145" s="28"/>
+      <c r="EQ145" s="28"/>
+      <c r="ER145" s="28"/>
+      <c r="EX145" s="28"/>
+      <c r="EY145" s="28"/>
+      <c r="FE145" s="28"/>
+      <c r="FF145" s="28"/>
+      <c r="FL145" s="28"/>
+      <c r="FM145" s="28"/>
+      <c r="FS145" s="28"/>
+      <c r="FT145" s="28"/>
+      <c r="FZ145" s="28"/>
+      <c r="GA145" s="28"/>
+      <c r="GG145" s="28"/>
+      <c r="GH145" s="28"/>
+      <c r="GN145" s="28"/>
+      <c r="GO145" s="28"/>
+      <c r="GU145" s="28"/>
+      <c r="GV145" s="28"/>
+      <c r="HB145" s="28"/>
+      <c r="HC145" s="28"/>
+    </row>
+    <row r="146" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A146" s="25"/>
+      <c r="B146" s="26"/>
+      <c r="C146" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="D146" s="29"/>
+      <c r="E146" s="13"/>
+      <c r="F146" s="13"/>
+      <c r="G146" s="13"/>
+      <c r="H146" s="5"/>
+      <c r="N146" s="28"/>
+      <c r="O146" s="28"/>
+      <c r="U146" s="28"/>
+      <c r="V146" s="28"/>
+      <c r="AB146" s="28"/>
+      <c r="AC146" s="28"/>
+      <c r="AI146" s="28"/>
+      <c r="AJ146" s="28"/>
+      <c r="AP146" s="28"/>
+      <c r="AQ146" s="28"/>
+      <c r="AW146" s="28"/>
+      <c r="AX146" s="28"/>
+      <c r="BD146" s="28"/>
+      <c r="BE146" s="28"/>
+      <c r="BK146" s="28"/>
+      <c r="BL146" s="28"/>
+      <c r="BR146" s="28"/>
+      <c r="BS146" s="28"/>
+      <c r="BY146" s="28"/>
+      <c r="BZ146" s="28"/>
+      <c r="CE146" s="38"/>
+      <c r="CF146" s="28"/>
+      <c r="CG146" s="28"/>
+      <c r="CM146" s="28"/>
+      <c r="CN146" s="28"/>
+      <c r="CT146" s="28"/>
+      <c r="CU146" s="28"/>
+      <c r="DA146" s="28"/>
+      <c r="DB146" s="28"/>
+      <c r="DH146" s="28"/>
+      <c r="DI146" s="28"/>
+      <c r="DO146" s="28"/>
+      <c r="DP146" s="28"/>
+      <c r="DV146" s="28"/>
+      <c r="DW146" s="28"/>
+      <c r="EC146" s="28"/>
+      <c r="ED146" s="28"/>
+      <c r="EJ146" s="28"/>
+      <c r="EK146" s="28"/>
+      <c r="EQ146" s="28"/>
+      <c r="ER146" s="28"/>
+      <c r="EX146" s="28"/>
+      <c r="EY146" s="28"/>
+      <c r="FE146" s="28"/>
+      <c r="FF146" s="28"/>
+      <c r="FL146" s="28"/>
+      <c r="FM146" s="28"/>
+      <c r="FS146" s="28"/>
+      <c r="FT146" s="28"/>
+      <c r="FZ146" s="28"/>
+      <c r="GA146" s="28"/>
+      <c r="GG146" s="28"/>
+      <c r="GH146" s="28"/>
+      <c r="GN146" s="28"/>
+      <c r="GO146" s="28"/>
+      <c r="GU146" s="28"/>
+      <c r="GV146" s="28"/>
+      <c r="HB146" s="28"/>
+      <c r="HC146" s="28"/>
+    </row>
+    <row r="147" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A147" s="25"/>
+      <c r="B147" s="26"/>
+      <c r="C147" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="D147" s="29"/>
+      <c r="E147" s="13"/>
+      <c r="F147" s="13"/>
+      <c r="G147" s="13"/>
+      <c r="H147" s="5"/>
+      <c r="N147" s="28"/>
+      <c r="O147" s="28"/>
+      <c r="U147" s="28"/>
+      <c r="V147" s="28"/>
+      <c r="AB147" s="28"/>
+      <c r="AC147" s="28"/>
+      <c r="AI147" s="28"/>
+      <c r="AJ147" s="28"/>
+      <c r="AP147" s="28"/>
+      <c r="AQ147" s="28"/>
+      <c r="AW147" s="28"/>
+      <c r="AX147" s="28"/>
+      <c r="BD147" s="28"/>
+      <c r="BE147" s="28"/>
+      <c r="BK147" s="28"/>
+      <c r="BL147" s="28"/>
+      <c r="BR147" s="28"/>
+      <c r="BS147" s="28"/>
+      <c r="BY147" s="28"/>
+      <c r="BZ147" s="28"/>
+      <c r="CE147" s="38"/>
+      <c r="CF147" s="28"/>
+      <c r="CG147" s="28"/>
+      <c r="CM147" s="28"/>
+      <c r="CN147" s="28"/>
+      <c r="CT147" s="28"/>
+      <c r="CU147" s="28"/>
+      <c r="DA147" s="28"/>
+      <c r="DB147" s="28"/>
+      <c r="DH147" s="28"/>
+      <c r="DI147" s="28"/>
+      <c r="DO147" s="28"/>
+      <c r="DP147" s="28"/>
+      <c r="DV147" s="28"/>
+      <c r="DW147" s="28"/>
+      <c r="EC147" s="28"/>
+      <c r="ED147" s="28"/>
+      <c r="EJ147" s="28"/>
+      <c r="EK147" s="28"/>
+      <c r="EQ147" s="28"/>
+      <c r="ER147" s="28"/>
+      <c r="EX147" s="28"/>
+      <c r="EY147" s="28"/>
+      <c r="FE147" s="28"/>
+      <c r="FF147" s="28"/>
+      <c r="FL147" s="28"/>
+      <c r="FM147" s="28"/>
+      <c r="FS147" s="28"/>
+      <c r="FT147" s="28"/>
+      <c r="FZ147" s="28"/>
+      <c r="GA147" s="28"/>
+      <c r="GG147" s="28"/>
+      <c r="GH147" s="28"/>
+      <c r="GN147" s="28"/>
+      <c r="GO147" s="28"/>
+      <c r="GU147" s="28"/>
+      <c r="GV147" s="28"/>
+      <c r="HB147" s="28"/>
+      <c r="HC147" s="28"/>
+    </row>
+    <row r="148" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A148" s="25"/>
+      <c r="B148" s="26"/>
+      <c r="C148" s="47"/>
+      <c r="D148" s="29"/>
+      <c r="E148" s="13"/>
+      <c r="F148" s="13"/>
+      <c r="G148" s="13"/>
+      <c r="H148" s="5"/>
+      <c r="N148" s="28"/>
+      <c r="O148" s="28"/>
+      <c r="U148" s="28"/>
+      <c r="V148" s="28"/>
+      <c r="AB148" s="28"/>
+      <c r="AC148" s="28"/>
+      <c r="AI148" s="28"/>
+      <c r="AJ148" s="28"/>
+      <c r="AP148" s="28"/>
+      <c r="AQ148" s="28"/>
+      <c r="AW148" s="28"/>
+      <c r="AX148" s="28"/>
+      <c r="BD148" s="28"/>
+      <c r="BE148" s="28"/>
+      <c r="BK148" s="28"/>
+      <c r="BL148" s="28"/>
+      <c r="BR148" s="28"/>
+      <c r="BS148" s="28"/>
+      <c r="BY148" s="28"/>
+      <c r="BZ148" s="28"/>
+      <c r="CE148" s="38"/>
+      <c r="CF148" s="28"/>
+      <c r="CG148" s="28"/>
+      <c r="CM148" s="28"/>
+      <c r="CN148" s="28"/>
+      <c r="CT148" s="28"/>
+      <c r="CU148" s="28"/>
+      <c r="DA148" s="28"/>
+      <c r="DB148" s="28"/>
+      <c r="DH148" s="28"/>
+      <c r="DI148" s="28"/>
+      <c r="DO148" s="28"/>
+      <c r="DP148" s="28"/>
+      <c r="DV148" s="28"/>
+      <c r="DW148" s="28"/>
+      <c r="EC148" s="28"/>
+      <c r="ED148" s="28"/>
+      <c r="EJ148" s="28"/>
+      <c r="EK148" s="28"/>
+      <c r="EQ148" s="28"/>
+      <c r="ER148" s="28"/>
+      <c r="EX148" s="28"/>
+      <c r="EY148" s="28"/>
+      <c r="FE148" s="28"/>
+      <c r="FF148" s="28"/>
+      <c r="FL148" s="28"/>
+      <c r="FM148" s="28"/>
+      <c r="FS148" s="28"/>
+      <c r="FT148" s="28"/>
+      <c r="FZ148" s="28"/>
+      <c r="GA148" s="28"/>
+      <c r="GG148" s="28"/>
+      <c r="GH148" s="28"/>
+      <c r="GN148" s="28"/>
+      <c r="GO148" s="28"/>
+      <c r="GU148" s="28"/>
+      <c r="GV148" s="28"/>
+      <c r="HB148" s="28"/>
+      <c r="HC148" s="28"/>
+    </row>
+    <row r="149" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A149" s="25"/>
+      <c r="B149" s="26"/>
+      <c r="C149" s="47"/>
+      <c r="D149" s="29"/>
+      <c r="E149" s="13"/>
+      <c r="F149" s="13"/>
+      <c r="G149" s="13"/>
+      <c r="H149" s="5"/>
+      <c r="N149" s="28"/>
+      <c r="O149" s="28"/>
+      <c r="U149" s="28"/>
+      <c r="V149" s="28"/>
+      <c r="AB149" s="28"/>
+      <c r="AC149" s="28"/>
+      <c r="AI149" s="28"/>
+      <c r="AJ149" s="28"/>
+      <c r="AP149" s="28"/>
+      <c r="AQ149" s="28"/>
+      <c r="AW149" s="28"/>
+      <c r="AX149" s="28"/>
+      <c r="BD149" s="28"/>
+      <c r="BE149" s="28"/>
+      <c r="BK149" s="28"/>
+      <c r="BL149" s="28"/>
+      <c r="BR149" s="28"/>
+      <c r="BS149" s="28"/>
+      <c r="BY149" s="28"/>
+      <c r="BZ149" s="28"/>
+      <c r="CE149" s="38"/>
+      <c r="CF149" s="28"/>
+      <c r="CG149" s="28"/>
+      <c r="CM149" s="28"/>
+      <c r="CN149" s="28"/>
+      <c r="CT149" s="28"/>
+      <c r="CU149" s="28"/>
+      <c r="DA149" s="28"/>
+      <c r="DB149" s="28"/>
+      <c r="DH149" s="28"/>
+      <c r="DI149" s="28"/>
+      <c r="DO149" s="28"/>
+      <c r="DP149" s="28"/>
+      <c r="DV149" s="28"/>
+      <c r="DW149" s="28"/>
+      <c r="EC149" s="28"/>
+      <c r="ED149" s="28"/>
+      <c r="EJ149" s="28"/>
+      <c r="EK149" s="28"/>
+      <c r="EQ149" s="28"/>
+      <c r="ER149" s="28"/>
+      <c r="EX149" s="28"/>
+      <c r="EY149" s="28"/>
+      <c r="FE149" s="28"/>
+      <c r="FF149" s="28"/>
+      <c r="FL149" s="28"/>
+      <c r="FM149" s="28"/>
+      <c r="FS149" s="28"/>
+      <c r="FT149" s="28"/>
+      <c r="FZ149" s="28"/>
+      <c r="GA149" s="28"/>
+      <c r="GG149" s="28"/>
+      <c r="GH149" s="28"/>
+      <c r="GN149" s="28"/>
+      <c r="GO149" s="28"/>
+      <c r="GU149" s="28"/>
+      <c r="GV149" s="28"/>
+      <c r="HB149" s="28"/>
+      <c r="HC149" s="28"/>
+    </row>
+    <row r="150" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A150" s="25"/>
+      <c r="B150" s="26"/>
+      <c r="C150" s="47"/>
+      <c r="D150" s="29"/>
+      <c r="E150" s="13"/>
+      <c r="F150" s="13"/>
+      <c r="G150" s="13"/>
+      <c r="H150" s="5"/>
+      <c r="N150" s="28"/>
+      <c r="O150" s="28"/>
+      <c r="U150" s="28"/>
+      <c r="V150" s="28"/>
+      <c r="AB150" s="28"/>
+      <c r="AC150" s="28"/>
+      <c r="AI150" s="28"/>
+      <c r="AJ150" s="28"/>
+      <c r="AP150" s="28"/>
+      <c r="AQ150" s="28"/>
+      <c r="AW150" s="28"/>
+      <c r="AX150" s="28"/>
+      <c r="BD150" s="28"/>
+      <c r="BE150" s="28"/>
+      <c r="BK150" s="28"/>
+      <c r="BL150" s="28"/>
+      <c r="BR150" s="28"/>
+      <c r="BS150" s="28"/>
+      <c r="BY150" s="28"/>
+      <c r="BZ150" s="28"/>
+      <c r="CE150" s="38"/>
+      <c r="CF150" s="28"/>
+      <c r="CG150" s="28"/>
+      <c r="CM150" s="28"/>
+      <c r="CN150" s="28"/>
+      <c r="CT150" s="28"/>
+      <c r="CU150" s="28"/>
+      <c r="DA150" s="28"/>
+      <c r="DB150" s="28"/>
+      <c r="DH150" s="28"/>
+      <c r="DI150" s="28"/>
+      <c r="DO150" s="28"/>
+      <c r="DP150" s="28"/>
+      <c r="DV150" s="28"/>
+      <c r="DW150" s="28"/>
+      <c r="EC150" s="28"/>
+      <c r="ED150" s="28"/>
+      <c r="EJ150" s="28"/>
+      <c r="EK150" s="28"/>
+      <c r="EQ150" s="28"/>
+      <c r="ER150" s="28"/>
+      <c r="EX150" s="28"/>
+      <c r="EY150" s="28"/>
+      <c r="FE150" s="28"/>
+      <c r="FF150" s="28"/>
+      <c r="FL150" s="28"/>
+      <c r="FM150" s="28"/>
+      <c r="FS150" s="28"/>
+      <c r="FT150" s="28"/>
+      <c r="FZ150" s="28"/>
+      <c r="GA150" s="28"/>
+      <c r="GG150" s="28"/>
+      <c r="GH150" s="28"/>
+      <c r="GN150" s="28"/>
+      <c r="GO150" s="28"/>
+      <c r="GU150" s="28"/>
+      <c r="GV150" s="28"/>
+      <c r="HB150" s="28"/>
+      <c r="HC150" s="28"/>
+    </row>
+    <row r="151" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A151" s="25"/>
+      <c r="B151" s="26"/>
+      <c r="C151" s="47"/>
+      <c r="D151" s="29"/>
+      <c r="E151" s="13"/>
+      <c r="F151" s="13"/>
+      <c r="G151" s="13"/>
+      <c r="H151" s="5"/>
+      <c r="N151" s="28"/>
+      <c r="O151" s="28"/>
+      <c r="U151" s="28"/>
+      <c r="V151" s="28"/>
+      <c r="AB151" s="28"/>
+      <c r="AC151" s="28"/>
+      <c r="AI151" s="28"/>
+      <c r="AJ151" s="28"/>
+      <c r="AP151" s="28"/>
+      <c r="AQ151" s="28"/>
+      <c r="AW151" s="28"/>
+      <c r="AX151" s="28"/>
+      <c r="BD151" s="28"/>
+      <c r="BE151" s="28"/>
+      <c r="BK151" s="28"/>
+      <c r="BL151" s="28"/>
+      <c r="BR151" s="28"/>
+      <c r="BS151" s="28"/>
+      <c r="BY151" s="28"/>
+      <c r="BZ151" s="28"/>
+      <c r="CE151" s="38"/>
+      <c r="CF151" s="28"/>
+      <c r="CG151" s="28"/>
+      <c r="CM151" s="28"/>
+      <c r="CN151" s="28"/>
+      <c r="CT151" s="28"/>
+      <c r="CU151" s="28"/>
+      <c r="DA151" s="28"/>
+      <c r="DB151" s="28"/>
+      <c r="DH151" s="28"/>
+      <c r="DI151" s="28"/>
+      <c r="DO151" s="28"/>
+      <c r="DP151" s="28"/>
+      <c r="DV151" s="28"/>
+      <c r="DW151" s="28"/>
+      <c r="EC151" s="28"/>
+      <c r="ED151" s="28"/>
+      <c r="EJ151" s="28"/>
+      <c r="EK151" s="28"/>
+      <c r="EQ151" s="28"/>
+      <c r="ER151" s="28"/>
+      <c r="EX151" s="28"/>
+      <c r="EY151" s="28"/>
+      <c r="FE151" s="28"/>
+      <c r="FF151" s="28"/>
+      <c r="FL151" s="28"/>
+      <c r="FM151" s="28"/>
+      <c r="FS151" s="28"/>
+      <c r="FT151" s="28"/>
+      <c r="FZ151" s="28"/>
+      <c r="GA151" s="28"/>
+      <c r="GG151" s="28"/>
+      <c r="GH151" s="28"/>
+      <c r="GN151" s="28"/>
+      <c r="GO151" s="28"/>
+      <c r="GU151" s="28"/>
+      <c r="GV151" s="28"/>
+      <c r="HB151" s="28"/>
+      <c r="HC151" s="28"/>
+    </row>
+    <row r="152" spans="1:211">
+      <c r="A152" s="14"/>
+      <c r="B152" s="14"/>
+      <c r="CE152" s="38"/>
+      <c r="CG152" s="38"/>
+      <c r="CI152" s="38"/>
+      <c r="CK152" s="38"/>
     </row>
   </sheetData>
   <sortState ref="B101:C109">
@@ -13660,65 +14454,65 @@
     <mergeCell ref="A86:C86"/>
     <mergeCell ref="A124:C124"/>
   </mergeCells>
-  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 J69:M140 DQ8:DU140 DJ8:DN140 DC8:DG140 EE8:EI140 CA8:CE140 AY8:BC140 AR8:AV140 AK8:AO140 AD8:AH140 BF66:BJ140 BM66:BQ140 BT66:BX140 W78:AA140 P60:T140 CV60:CZ140 CO69:CS140 DX114:EB140 CH60:CL140 EL8:EP140 ES8:EW140 EZ8:FD140 FG8:FK140 FN8:FR140 FU8:FY140 GB8:GF140 GI8:GM140 GP8:GT140 GW8:HA140">
-    <cfRule type="expression" dxfId="24" priority="92">
+  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 J69:M151 DQ8:DU151 DJ8:DN151 DC8:DG151 EE8:EI151 CA8:CE151 AY8:BC151 AR8:AV151 AK8:AO151 AD8:AH151 BF66:BJ151 BM66:BQ151 BT66:BX151 W78:AA151 P60:T151 CV60:CZ151 CO69:CS151 DX114:EB151 CH60:CL151 EL8:EP151 ES8:EW151 EZ8:FD151 FG8:FK151 FN8:FR151 FU8:FY151 GB8:GF151 GI8:GM151 GP8:GT151 GW8:HA151">
+    <cfRule type="expression" dxfId="17" priority="92">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="93">
+    <cfRule type="expression" dxfId="16" priority="93">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="94">
+    <cfRule type="expression" dxfId="15" priority="94">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="95">
+    <cfRule type="expression" dxfId="14" priority="95">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="96">
+    <cfRule type="expression" dxfId="13" priority="96">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="97">
+    <cfRule type="expression" dxfId="12" priority="97">
       <formula>J$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="98">
+    <cfRule type="expression" dxfId="11" priority="98">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="99">
+    <cfRule type="expression" dxfId="10" priority="99">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A141:HC141">
-    <cfRule type="expression" dxfId="16" priority="91">
+  <conditionalFormatting sqref="A152:HC152">
+    <cfRule type="expression" dxfId="9" priority="91">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:HC7">
-    <cfRule type="expression" dxfId="15" priority="90">
+    <cfRule type="expression" dxfId="8" priority="90">
       <formula>J$7=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL56:CL57">
-    <cfRule type="expression" dxfId="14" priority="81">
+    <cfRule type="expression" dxfId="7" priority="81">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="82">
+    <cfRule type="expression" dxfId="6" priority="82">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="83">
+    <cfRule type="expression" dxfId="5" priority="83">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="84">
+    <cfRule type="expression" dxfId="4" priority="84">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="85">
+    <cfRule type="expression" dxfId="3" priority="85">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="86">
+    <cfRule type="expression" dxfId="2" priority="86">
       <formula>CL$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="87">
+    <cfRule type="expression" dxfId="1" priority="87">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="88">
+    <cfRule type="expression" dxfId="0" priority="88">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13732,7 +14526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AO238"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
@@ -13809,10 +14603,10 @@
         <v>41690</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AO6" s="35" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
-Internet explorer 8 compatibility for vendors. -Showing message to Vendor when a RFQ has been deleted.
</commit_message>
<xml_diff>
--- a/AQPM Gantt.xlsx
+++ b/AQPM Gantt.xlsx
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="179">
   <si>
     <t>Plan</t>
   </si>
@@ -726,6 +726,9 @@
   </si>
   <si>
     <t>Report to Sales (copy) showing all RFQs</t>
+  </si>
+  <si>
+    <t>PPAP/FAIR cost</t>
   </si>
 </sst>
 </file>
@@ -1223,6 +1226,134 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0"/>
@@ -1477,134 +1608,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1628,15 +1631,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A4:F238"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="23"/>
-    <tableColumn id="2" name="Date" dataDxfId="22"/>
-    <tableColumn id="3" name="Creator" dataDxfId="21"/>
-    <tableColumn id="4" name="Issue" dataDxfId="20"/>
-    <tableColumn id="5" name="Status" dataDxfId="19"/>
-    <tableColumn id="6" name="Solution" dataDxfId="18"/>
+    <tableColumn id="1" name="#" dataDxfId="5"/>
+    <tableColumn id="2" name="Date" dataDxfId="4"/>
+    <tableColumn id="3" name="Creator" dataDxfId="3"/>
+    <tableColumn id="4" name="Issue" dataDxfId="2"/>
+    <tableColumn id="5" name="Status" dataDxfId="1"/>
+    <tableColumn id="6" name="Solution" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1875,10 +1878,10 @@
   <dimension ref="A2:HC154"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="EF122" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="7" topLeftCell="EF137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="C126" sqref="C126"/>
+      <selection pane="bottomRight" activeCell="C151" sqref="C151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25"/>
@@ -14359,7 +14362,9 @@
     <row r="150" spans="1:211" ht="18.95" customHeight="1">
       <c r="A150" s="25"/>
       <c r="B150" s="26"/>
-      <c r="C150" s="47"/>
+      <c r="C150" s="47" t="s">
+        <v>178</v>
+      </c>
       <c r="D150" s="29"/>
       <c r="E150" s="13"/>
       <c r="F150" s="13"/>
@@ -14651,64 +14656,64 @@
     <mergeCell ref="A125:C125"/>
   </mergeCells>
   <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU153 DJ8:DN153 DC8:DG153 EE8:EI153 CA8:CE153 AY8:BC153 AR8:AV153 AK8:AO153 AD8:AH153 BF66:BJ153 BM66:BQ153 BT66:BX153 W78:AA153 P60:T153 CV60:CZ153 CO69:CS153 DX114:EB153 CH60:CL153 EL8:EP153 ES8:EW153 EZ8:FD153 FG8:FK153 FN8:FR153 FU8:FY153 GB8:GF153 GI8:GM153 GP8:GT153 GW8:HA153 J69:M153">
-    <cfRule type="expression" dxfId="17" priority="92">
+    <cfRule type="expression" dxfId="24" priority="92">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="93">
+    <cfRule type="expression" dxfId="23" priority="93">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="94">
+    <cfRule type="expression" dxfId="22" priority="94">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="95">
+    <cfRule type="expression" dxfId="21" priority="95">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="96">
+    <cfRule type="expression" dxfId="20" priority="96">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="97">
+    <cfRule type="expression" dxfId="19" priority="97">
       <formula>J$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="98">
+    <cfRule type="expression" dxfId="18" priority="98">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="99">
+    <cfRule type="expression" dxfId="17" priority="99">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A154:HC154">
-    <cfRule type="expression" dxfId="9" priority="91">
+    <cfRule type="expression" dxfId="16" priority="91">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:HC7">
-    <cfRule type="expression" dxfId="8" priority="90">
+    <cfRule type="expression" dxfId="15" priority="90">
       <formula>J$7=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL56:CL57">
-    <cfRule type="expression" dxfId="7" priority="81">
+    <cfRule type="expression" dxfId="14" priority="81">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="82">
+    <cfRule type="expression" dxfId="13" priority="82">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="83">
+    <cfRule type="expression" dxfId="12" priority="83">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="84">
+    <cfRule type="expression" dxfId="11" priority="84">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="85">
+    <cfRule type="expression" dxfId="10" priority="85">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="86">
+    <cfRule type="expression" dxfId="9" priority="86">
       <formula>CL$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="87">
+    <cfRule type="expression" dxfId="8" priority="87">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="88">
+    <cfRule type="expression" dxfId="7" priority="88">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Some new issues added to Gantt
</commit_message>
<xml_diff>
--- a/AQPM Gantt.xlsx
+++ b/AQPM Gantt.xlsx
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="183">
   <si>
     <t>Plan</t>
   </si>
@@ -729,6 +729,18 @@
   </si>
   <si>
     <t>PPAP/FAIR cost</t>
+  </si>
+  <si>
+    <t>Filter by dates SIF list</t>
+  </si>
+  <si>
+    <t>Separate RFQ Summaries by EAUs</t>
+  </si>
+  <si>
+    <t>RFQ Number and Component PN inside email</t>
+  </si>
+  <si>
+    <t>Export reports to Excel format</t>
   </si>
 </sst>
 </file>
@@ -1226,134 +1238,6 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0"/>
@@ -1608,6 +1492,134 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1631,15 +1643,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="24">
   <autoFilter ref="A4:F238"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="5"/>
-    <tableColumn id="2" name="Date" dataDxfId="4"/>
-    <tableColumn id="3" name="Creator" dataDxfId="3"/>
-    <tableColumn id="4" name="Issue" dataDxfId="2"/>
-    <tableColumn id="5" name="Status" dataDxfId="1"/>
-    <tableColumn id="6" name="Solution" dataDxfId="0"/>
+    <tableColumn id="1" name="#" dataDxfId="23"/>
+    <tableColumn id="2" name="Date" dataDxfId="22"/>
+    <tableColumn id="3" name="Creator" dataDxfId="21"/>
+    <tableColumn id="4" name="Issue" dataDxfId="20"/>
+    <tableColumn id="5" name="Status" dataDxfId="19"/>
+    <tableColumn id="6" name="Solution" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1875,13 +1887,13 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:HC154"/>
+  <dimension ref="A2:HC158"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
       <pane xSplit="9" ySplit="7" topLeftCell="EF137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="C151" sqref="C151"/>
+      <selection pane="bottomRight" activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25"/>
@@ -14433,7 +14445,9 @@
     <row r="151" spans="1:211" ht="18.95" customHeight="1">
       <c r="A151" s="25"/>
       <c r="B151" s="26"/>
-      <c r="C151" s="47"/>
+      <c r="C151" s="47" t="s">
+        <v>179</v>
+      </c>
       <c r="D151" s="29"/>
       <c r="E151" s="13"/>
       <c r="F151" s="13"/>
@@ -14502,7 +14516,9 @@
     <row r="152" spans="1:211" ht="18.95" customHeight="1">
       <c r="A152" s="25"/>
       <c r="B152" s="26"/>
-      <c r="C152" s="47"/>
+      <c r="C152" s="47" t="s">
+        <v>180</v>
+      </c>
       <c r="D152" s="29"/>
       <c r="E152" s="13"/>
       <c r="F152" s="13"/>
@@ -14571,7 +14587,9 @@
     <row r="153" spans="1:211" ht="18.95" customHeight="1">
       <c r="A153" s="25"/>
       <c r="B153" s="26"/>
-      <c r="C153" s="47"/>
+      <c r="C153" s="47" t="s">
+        <v>181</v>
+      </c>
       <c r="D153" s="29"/>
       <c r="E153" s="13"/>
       <c r="F153" s="13"/>
@@ -14637,13 +14655,291 @@
       <c r="HB153" s="28"/>
       <c r="HC153" s="28"/>
     </row>
-    <row r="154" spans="1:211">
-      <c r="A154" s="14"/>
-      <c r="B154" s="14"/>
+    <row r="154" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A154" s="25"/>
+      <c r="B154" s="26"/>
+      <c r="C154" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="D154" s="29"/>
+      <c r="E154" s="13"/>
+      <c r="F154" s="13"/>
+      <c r="G154" s="13"/>
+      <c r="H154" s="5"/>
+      <c r="N154" s="28"/>
+      <c r="O154" s="28"/>
+      <c r="U154" s="28"/>
+      <c r="V154" s="28"/>
+      <c r="AB154" s="28"/>
+      <c r="AC154" s="28"/>
+      <c r="AI154" s="28"/>
+      <c r="AJ154" s="28"/>
+      <c r="AP154" s="28"/>
+      <c r="AQ154" s="28"/>
+      <c r="AW154" s="28"/>
+      <c r="AX154" s="28"/>
+      <c r="BD154" s="28"/>
+      <c r="BE154" s="28"/>
+      <c r="BK154" s="28"/>
+      <c r="BL154" s="28"/>
+      <c r="BR154" s="28"/>
+      <c r="BS154" s="28"/>
+      <c r="BY154" s="28"/>
+      <c r="BZ154" s="28"/>
       <c r="CE154" s="38"/>
-      <c r="CG154" s="38"/>
-      <c r="CI154" s="38"/>
-      <c r="CK154" s="38"/>
+      <c r="CF154" s="28"/>
+      <c r="CG154" s="28"/>
+      <c r="CM154" s="28"/>
+      <c r="CN154" s="28"/>
+      <c r="CT154" s="28"/>
+      <c r="CU154" s="28"/>
+      <c r="DA154" s="28"/>
+      <c r="DB154" s="28"/>
+      <c r="DH154" s="28"/>
+      <c r="DI154" s="28"/>
+      <c r="DO154" s="28"/>
+      <c r="DP154" s="28"/>
+      <c r="DV154" s="28"/>
+      <c r="DW154" s="28"/>
+      <c r="EC154" s="28"/>
+      <c r="ED154" s="28"/>
+      <c r="EJ154" s="28"/>
+      <c r="EK154" s="28"/>
+      <c r="EQ154" s="28"/>
+      <c r="ER154" s="28"/>
+      <c r="EX154" s="28"/>
+      <c r="EY154" s="28"/>
+      <c r="FE154" s="28"/>
+      <c r="FF154" s="28"/>
+      <c r="FL154" s="28"/>
+      <c r="FM154" s="28"/>
+      <c r="FS154" s="28"/>
+      <c r="FT154" s="28"/>
+      <c r="FZ154" s="28"/>
+      <c r="GA154" s="28"/>
+      <c r="GG154" s="28"/>
+      <c r="GH154" s="28"/>
+      <c r="GN154" s="28"/>
+      <c r="GO154" s="28"/>
+      <c r="GU154" s="28"/>
+      <c r="GV154" s="28"/>
+      <c r="HB154" s="28"/>
+      <c r="HC154" s="28"/>
+    </row>
+    <row r="155" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A155" s="25"/>
+      <c r="B155" s="26"/>
+      <c r="C155" s="47"/>
+      <c r="D155" s="29"/>
+      <c r="E155" s="13"/>
+      <c r="F155" s="13"/>
+      <c r="G155" s="13"/>
+      <c r="H155" s="5"/>
+      <c r="N155" s="28"/>
+      <c r="O155" s="28"/>
+      <c r="U155" s="28"/>
+      <c r="V155" s="28"/>
+      <c r="AB155" s="28"/>
+      <c r="AC155" s="28"/>
+      <c r="AI155" s="28"/>
+      <c r="AJ155" s="28"/>
+      <c r="AP155" s="28"/>
+      <c r="AQ155" s="28"/>
+      <c r="AW155" s="28"/>
+      <c r="AX155" s="28"/>
+      <c r="BD155" s="28"/>
+      <c r="BE155" s="28"/>
+      <c r="BK155" s="28"/>
+      <c r="BL155" s="28"/>
+      <c r="BR155" s="28"/>
+      <c r="BS155" s="28"/>
+      <c r="BY155" s="28"/>
+      <c r="BZ155" s="28"/>
+      <c r="CE155" s="38"/>
+      <c r="CF155" s="28"/>
+      <c r="CG155" s="28"/>
+      <c r="CM155" s="28"/>
+      <c r="CN155" s="28"/>
+      <c r="CT155" s="28"/>
+      <c r="CU155" s="28"/>
+      <c r="DA155" s="28"/>
+      <c r="DB155" s="28"/>
+      <c r="DH155" s="28"/>
+      <c r="DI155" s="28"/>
+      <c r="DO155" s="28"/>
+      <c r="DP155" s="28"/>
+      <c r="DV155" s="28"/>
+      <c r="DW155" s="28"/>
+      <c r="EC155" s="28"/>
+      <c r="ED155" s="28"/>
+      <c r="EJ155" s="28"/>
+      <c r="EK155" s="28"/>
+      <c r="EQ155" s="28"/>
+      <c r="ER155" s="28"/>
+      <c r="EX155" s="28"/>
+      <c r="EY155" s="28"/>
+      <c r="FE155" s="28"/>
+      <c r="FF155" s="28"/>
+      <c r="FL155" s="28"/>
+      <c r="FM155" s="28"/>
+      <c r="FS155" s="28"/>
+      <c r="FT155" s="28"/>
+      <c r="FZ155" s="28"/>
+      <c r="GA155" s="28"/>
+      <c r="GG155" s="28"/>
+      <c r="GH155" s="28"/>
+      <c r="GN155" s="28"/>
+      <c r="GO155" s="28"/>
+      <c r="GU155" s="28"/>
+      <c r="GV155" s="28"/>
+      <c r="HB155" s="28"/>
+      <c r="HC155" s="28"/>
+    </row>
+    <row r="156" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A156" s="25"/>
+      <c r="B156" s="26"/>
+      <c r="C156" s="47"/>
+      <c r="D156" s="29"/>
+      <c r="E156" s="13"/>
+      <c r="F156" s="13"/>
+      <c r="G156" s="13"/>
+      <c r="H156" s="5"/>
+      <c r="N156" s="28"/>
+      <c r="O156" s="28"/>
+      <c r="U156" s="28"/>
+      <c r="V156" s="28"/>
+      <c r="AB156" s="28"/>
+      <c r="AC156" s="28"/>
+      <c r="AI156" s="28"/>
+      <c r="AJ156" s="28"/>
+      <c r="AP156" s="28"/>
+      <c r="AQ156" s="28"/>
+      <c r="AW156" s="28"/>
+      <c r="AX156" s="28"/>
+      <c r="BD156" s="28"/>
+      <c r="BE156" s="28"/>
+      <c r="BK156" s="28"/>
+      <c r="BL156" s="28"/>
+      <c r="BR156" s="28"/>
+      <c r="BS156" s="28"/>
+      <c r="BY156" s="28"/>
+      <c r="BZ156" s="28"/>
+      <c r="CE156" s="38"/>
+      <c r="CF156" s="28"/>
+      <c r="CG156" s="28"/>
+      <c r="CM156" s="28"/>
+      <c r="CN156" s="28"/>
+      <c r="CT156" s="28"/>
+      <c r="CU156" s="28"/>
+      <c r="DA156" s="28"/>
+      <c r="DB156" s="28"/>
+      <c r="DH156" s="28"/>
+      <c r="DI156" s="28"/>
+      <c r="DO156" s="28"/>
+      <c r="DP156" s="28"/>
+      <c r="DV156" s="28"/>
+      <c r="DW156" s="28"/>
+      <c r="EC156" s="28"/>
+      <c r="ED156" s="28"/>
+      <c r="EJ156" s="28"/>
+      <c r="EK156" s="28"/>
+      <c r="EQ156" s="28"/>
+      <c r="ER156" s="28"/>
+      <c r="EX156" s="28"/>
+      <c r="EY156" s="28"/>
+      <c r="FE156" s="28"/>
+      <c r="FF156" s="28"/>
+      <c r="FL156" s="28"/>
+      <c r="FM156" s="28"/>
+      <c r="FS156" s="28"/>
+      <c r="FT156" s="28"/>
+      <c r="FZ156" s="28"/>
+      <c r="GA156" s="28"/>
+      <c r="GG156" s="28"/>
+      <c r="GH156" s="28"/>
+      <c r="GN156" s="28"/>
+      <c r="GO156" s="28"/>
+      <c r="GU156" s="28"/>
+      <c r="GV156" s="28"/>
+      <c r="HB156" s="28"/>
+      <c r="HC156" s="28"/>
+    </row>
+    <row r="157" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A157" s="25"/>
+      <c r="B157" s="26"/>
+      <c r="C157" s="47"/>
+      <c r="D157" s="29"/>
+      <c r="E157" s="13"/>
+      <c r="F157" s="13"/>
+      <c r="G157" s="13"/>
+      <c r="H157" s="5"/>
+      <c r="N157" s="28"/>
+      <c r="O157" s="28"/>
+      <c r="U157" s="28"/>
+      <c r="V157" s="28"/>
+      <c r="AB157" s="28"/>
+      <c r="AC157" s="28"/>
+      <c r="AI157" s="28"/>
+      <c r="AJ157" s="28"/>
+      <c r="AP157" s="28"/>
+      <c r="AQ157" s="28"/>
+      <c r="AW157" s="28"/>
+      <c r="AX157" s="28"/>
+      <c r="BD157" s="28"/>
+      <c r="BE157" s="28"/>
+      <c r="BK157" s="28"/>
+      <c r="BL157" s="28"/>
+      <c r="BR157" s="28"/>
+      <c r="BS157" s="28"/>
+      <c r="BY157" s="28"/>
+      <c r="BZ157" s="28"/>
+      <c r="CE157" s="38"/>
+      <c r="CF157" s="28"/>
+      <c r="CG157" s="28"/>
+      <c r="CM157" s="28"/>
+      <c r="CN157" s="28"/>
+      <c r="CT157" s="28"/>
+      <c r="CU157" s="28"/>
+      <c r="DA157" s="28"/>
+      <c r="DB157" s="28"/>
+      <c r="DH157" s="28"/>
+      <c r="DI157" s="28"/>
+      <c r="DO157" s="28"/>
+      <c r="DP157" s="28"/>
+      <c r="DV157" s="28"/>
+      <c r="DW157" s="28"/>
+      <c r="EC157" s="28"/>
+      <c r="ED157" s="28"/>
+      <c r="EJ157" s="28"/>
+      <c r="EK157" s="28"/>
+      <c r="EQ157" s="28"/>
+      <c r="ER157" s="28"/>
+      <c r="EX157" s="28"/>
+      <c r="EY157" s="28"/>
+      <c r="FE157" s="28"/>
+      <c r="FF157" s="28"/>
+      <c r="FL157" s="28"/>
+      <c r="FM157" s="28"/>
+      <c r="FS157" s="28"/>
+      <c r="FT157" s="28"/>
+      <c r="FZ157" s="28"/>
+      <c r="GA157" s="28"/>
+      <c r="GG157" s="28"/>
+      <c r="GH157" s="28"/>
+      <c r="GN157" s="28"/>
+      <c r="GO157" s="28"/>
+      <c r="GU157" s="28"/>
+      <c r="GV157" s="28"/>
+      <c r="HB157" s="28"/>
+      <c r="HC157" s="28"/>
+    </row>
+    <row r="158" spans="1:211">
+      <c r="A158" s="14"/>
+      <c r="B158" s="14"/>
+      <c r="CE158" s="38"/>
+      <c r="CG158" s="38"/>
+      <c r="CI158" s="38"/>
+      <c r="CK158" s="38"/>
     </row>
   </sheetData>
   <sortState ref="A125:GL149">
@@ -14655,65 +14951,65 @@
     <mergeCell ref="A86:C86"/>
     <mergeCell ref="A125:C125"/>
   </mergeCells>
-  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU153 DJ8:DN153 DC8:DG153 EE8:EI153 CA8:CE153 AY8:BC153 AR8:AV153 AK8:AO153 AD8:AH153 BF66:BJ153 BM66:BQ153 BT66:BX153 W78:AA153 P60:T153 CV60:CZ153 CO69:CS153 DX114:EB153 CH60:CL153 EL8:EP153 ES8:EW153 EZ8:FD153 FG8:FK153 FN8:FR153 FU8:FY153 GB8:GF153 GI8:GM153 GP8:GT153 GW8:HA153 J69:M153">
-    <cfRule type="expression" dxfId="24" priority="92">
+  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU157 DJ8:DN157 DC8:DG157 EE8:EI157 CA8:CE157 AY8:BC157 AR8:AV157 AK8:AO157 AD8:AH157 BF66:BJ157 BM66:BQ157 BT66:BX157 W78:AA157 P60:T157 CV60:CZ157 CO69:CS157 DX114:EB157 CH60:CL157 EL8:EP157 ES8:EW157 EZ8:FD157 FG8:FK157 FN8:FR157 FU8:FY157 GB8:GF157 GI8:GM157 GP8:GT157 GW8:HA157 J69:M157">
+    <cfRule type="expression" dxfId="17" priority="92">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="93">
+    <cfRule type="expression" dxfId="16" priority="93">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="94">
+    <cfRule type="expression" dxfId="15" priority="94">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="95">
+    <cfRule type="expression" dxfId="14" priority="95">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="96">
+    <cfRule type="expression" dxfId="13" priority="96">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="97">
+    <cfRule type="expression" dxfId="12" priority="97">
       <formula>J$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="98">
+    <cfRule type="expression" dxfId="11" priority="98">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="99">
+    <cfRule type="expression" dxfId="10" priority="99">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A154:HC154">
-    <cfRule type="expression" dxfId="16" priority="91">
+  <conditionalFormatting sqref="A158:HC158">
+    <cfRule type="expression" dxfId="9" priority="91">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:HC7">
-    <cfRule type="expression" dxfId="15" priority="90">
+    <cfRule type="expression" dxfId="8" priority="90">
       <formula>J$7=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL56:CL57">
-    <cfRule type="expression" dxfId="14" priority="81">
+    <cfRule type="expression" dxfId="7" priority="81">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="82">
+    <cfRule type="expression" dxfId="6" priority="82">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="83">
+    <cfRule type="expression" dxfId="5" priority="83">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="84">
+    <cfRule type="expression" dxfId="4" priority="84">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="85">
+    <cfRule type="expression" dxfId="3" priority="85">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="86">
+    <cfRule type="expression" dxfId="2" priority="86">
       <formula>CL$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="87">
+    <cfRule type="expression" dxfId="1" priority="87">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="88">
+    <cfRule type="expression" dxfId="0" priority="88">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
-Upload files when creating new RFQs fixed. -Firefox compatibility for RFQ form done.
</commit_message>
<xml_diff>
--- a/AQPM Gantt.xlsx
+++ b/AQPM Gantt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10305" yWindow="4335" windowWidth="10230" windowHeight="4350"/>
+    <workbookView xWindow="10305" yWindow="4335" windowWidth="10230" windowHeight="4350" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="APQM Gantt" sheetId="2" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="190">
   <si>
     <t>Plan</t>
   </si>
@@ -734,13 +734,34 @@
     <t>Filter by dates SIF list</t>
   </si>
   <si>
-    <t>Separate RFQ Summaries by EAUs</t>
-  </si>
-  <si>
     <t>RFQ Number and Component PN inside email</t>
   </si>
   <si>
     <t>Export reports to Excel format</t>
+  </si>
+  <si>
+    <t>Increase Inquiry Number font size inside BOM</t>
+  </si>
+  <si>
+    <t>To be able to quote some component that was before estimated, but not remove the estimated information</t>
+  </si>
+  <si>
+    <t>Separate RFQ Summaries by EAUs (Show EAU in RFQ Summary)</t>
+  </si>
+  <si>
+    <t>UM in RFQ Summary</t>
+  </si>
+  <si>
+    <t>Failing when trying to upload files when creating RFQs</t>
+  </si>
+  <si>
+    <t>I had been moved some code to other folder, but I forgot changing I code line</t>
+  </si>
+  <si>
+    <t>RFQ form asks for credentials in Mozilla Firefox</t>
+  </si>
+  <si>
+    <t>There were some compaitiblity issues with javascript code when using  srcElement</t>
   </si>
 </sst>
 </file>
@@ -1238,6 +1259,134 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0"/>
@@ -1492,134 +1641,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1643,15 +1664,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A4:F238"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="23"/>
-    <tableColumn id="2" name="Date" dataDxfId="22"/>
-    <tableColumn id="3" name="Creator" dataDxfId="21"/>
-    <tableColumn id="4" name="Issue" dataDxfId="20"/>
-    <tableColumn id="5" name="Status" dataDxfId="19"/>
-    <tableColumn id="6" name="Solution" dataDxfId="18"/>
+    <tableColumn id="1" name="#" dataDxfId="5"/>
+    <tableColumn id="2" name="Date" dataDxfId="4"/>
+    <tableColumn id="3" name="Creator" dataDxfId="3"/>
+    <tableColumn id="4" name="Issue" dataDxfId="2"/>
+    <tableColumn id="5" name="Status" dataDxfId="1"/>
+    <tableColumn id="6" name="Solution" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1889,11 +1910,11 @@
   </sheetPr>
   <dimension ref="A2:HC158"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="EF137" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <pane xSplit="9" ySplit="7" topLeftCell="J139" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="C155" sqref="C155"/>
+      <selection pane="bottomRight" activeCell="C158" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25"/>
@@ -14517,7 +14538,7 @@
       <c r="A152" s="25"/>
       <c r="B152" s="26"/>
       <c r="C152" s="47" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D152" s="29"/>
       <c r="E152" s="13"/>
@@ -14588,7 +14609,7 @@
       <c r="A153" s="25"/>
       <c r="B153" s="26"/>
       <c r="C153" s="47" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D153" s="29"/>
       <c r="E153" s="13"/>
@@ -14659,7 +14680,7 @@
       <c r="A154" s="25"/>
       <c r="B154" s="26"/>
       <c r="C154" s="47" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D154" s="29"/>
       <c r="E154" s="13"/>
@@ -14729,7 +14750,9 @@
     <row r="155" spans="1:211" ht="18.95" customHeight="1">
       <c r="A155" s="25"/>
       <c r="B155" s="26"/>
-      <c r="C155" s="47"/>
+      <c r="C155" s="47" t="s">
+        <v>182</v>
+      </c>
       <c r="D155" s="29"/>
       <c r="E155" s="13"/>
       <c r="F155" s="13"/>
@@ -14798,7 +14821,9 @@
     <row r="156" spans="1:211" ht="18.95" customHeight="1">
       <c r="A156" s="25"/>
       <c r="B156" s="26"/>
-      <c r="C156" s="47"/>
+      <c r="C156" s="47" t="s">
+        <v>183</v>
+      </c>
       <c r="D156" s="29"/>
       <c r="E156" s="13"/>
       <c r="F156" s="13"/>
@@ -14867,7 +14892,9 @@
     <row r="157" spans="1:211" ht="18.95" customHeight="1">
       <c r="A157" s="25"/>
       <c r="B157" s="26"/>
-      <c r="C157" s="47"/>
+      <c r="C157" s="47" t="s">
+        <v>185</v>
+      </c>
       <c r="D157" s="29"/>
       <c r="E157" s="13"/>
       <c r="F157" s="13"/>
@@ -14952,64 +14979,64 @@
     <mergeCell ref="A125:C125"/>
   </mergeCells>
   <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU157 DJ8:DN157 DC8:DG157 EE8:EI157 CA8:CE157 AY8:BC157 AR8:AV157 AK8:AO157 AD8:AH157 BF66:BJ157 BM66:BQ157 BT66:BX157 W78:AA157 P60:T157 CV60:CZ157 CO69:CS157 DX114:EB157 CH60:CL157 EL8:EP157 ES8:EW157 EZ8:FD157 FG8:FK157 FN8:FR157 FU8:FY157 GB8:GF157 GI8:GM157 GP8:GT157 GW8:HA157 J69:M157">
-    <cfRule type="expression" dxfId="17" priority="92">
+    <cfRule type="expression" dxfId="24" priority="92">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="93">
+    <cfRule type="expression" dxfId="23" priority="93">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="94">
+    <cfRule type="expression" dxfId="22" priority="94">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="95">
+    <cfRule type="expression" dxfId="21" priority="95">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="96">
+    <cfRule type="expression" dxfId="20" priority="96">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="97">
+    <cfRule type="expression" dxfId="19" priority="97">
       <formula>J$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="98">
+    <cfRule type="expression" dxfId="18" priority="98">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="99">
+    <cfRule type="expression" dxfId="17" priority="99">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A158:HC158">
-    <cfRule type="expression" dxfId="9" priority="91">
+    <cfRule type="expression" dxfId="16" priority="91">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:HC7">
-    <cfRule type="expression" dxfId="8" priority="90">
+    <cfRule type="expression" dxfId="15" priority="90">
       <formula>J$7=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL56:CL57">
-    <cfRule type="expression" dxfId="7" priority="81">
+    <cfRule type="expression" dxfId="14" priority="81">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="82">
+    <cfRule type="expression" dxfId="13" priority="82">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="83">
+    <cfRule type="expression" dxfId="12" priority="83">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="84">
+    <cfRule type="expression" dxfId="11" priority="84">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="85">
+    <cfRule type="expression" dxfId="10" priority="85">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="86">
+    <cfRule type="expression" dxfId="9" priority="86">
       <formula>CL$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="87">
+    <cfRule type="expression" dxfId="8" priority="87">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="88">
+    <cfRule type="expression" dxfId="7" priority="88">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15023,9 +15050,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AO238"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15035,7 +15062,7 @@
     <col min="3" max="3" width="16.375" style="33" customWidth="1"/>
     <col min="4" max="4" width="46" style="36" customWidth="1"/>
     <col min="5" max="5" width="11.625" style="34" customWidth="1"/>
-    <col min="6" max="6" width="63.375" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66.125" style="36" bestFit="1" customWidth="1"/>
     <col min="7" max="40" width="9" style="36"/>
     <col min="41" max="41" width="9" style="35" hidden="1" customWidth="1"/>
     <col min="42" max="16384" width="9" style="36"/>
@@ -15113,6 +15140,21 @@
       <c r="A7" s="36">
         <v>3</v>
       </c>
+      <c r="B7" s="33">
+        <v>41705</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>187</v>
+      </c>
       <c r="AO7" s="35" t="s">
         <v>56</v>
       </c>
@@ -15120,6 +15162,21 @@
     <row r="8" spans="1:41">
       <c r="A8" s="36">
         <v>4</v>
+      </c>
+      <c r="B8" s="33">
+        <v>41705</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:41">

</xml_diff>

<commit_message>
-Showing UM in Report To Sales -Adding Cubic Meter for UM
</commit_message>
<xml_diff>
--- a/AQPM Gantt.xlsx
+++ b/AQPM Gantt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10305" yWindow="4335" windowWidth="10230" windowHeight="4350" activeTab="1"/>
+    <workbookView xWindow="10305" yWindow="4335" windowWidth="10230" windowHeight="4350"/>
   </bookViews>
   <sheets>
     <sheet name="APQM Gantt" sheetId="2" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="194">
   <si>
     <t>Plan</t>
   </si>
@@ -762,6 +762,18 @@
   </si>
   <si>
     <t>There were some compaitiblity issues with javascript code when using  srcElement</t>
+  </si>
+  <si>
+    <t>Know the last email used when a RFQ was sent</t>
+  </si>
+  <si>
+    <t>Martha</t>
+  </si>
+  <si>
+    <t>Cannot set focus for create new vendor from popup</t>
+  </si>
+  <si>
+    <t>Export Sales Report component processed without RFQ</t>
   </si>
 </sst>
 </file>
@@ -1908,13 +1920,13 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:HC158"/>
+  <dimension ref="A2:HC160"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="J139" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <pane xSplit="9" ySplit="7" topLeftCell="FO125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="C158" sqref="C158"/>
+      <selection pane="bottomRight" activeCell="F137" sqref="F137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25"/>
@@ -13436,9 +13448,15 @@
       </c>
       <c r="D137" s="29"/>
       <c r="E137" s="13"/>
-      <c r="F137" s="13"/>
-      <c r="G137" s="13"/>
-      <c r="H137" s="5"/>
+      <c r="F137" s="13">
+        <v>171</v>
+      </c>
+      <c r="G137" s="13">
+        <v>1</v>
+      </c>
+      <c r="H137" s="5">
+        <v>1</v>
+      </c>
       <c r="N137" s="28"/>
       <c r="O137" s="28"/>
       <c r="U137" s="28"/>
@@ -14960,13 +14978,155 @@
       <c r="HB157" s="28"/>
       <c r="HC157" s="28"/>
     </row>
-    <row r="158" spans="1:211">
-      <c r="A158" s="14"/>
-      <c r="B158" s="14"/>
+    <row r="158" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A158" s="25"/>
+      <c r="B158" s="26"/>
+      <c r="C158" s="47" t="s">
+        <v>190</v>
+      </c>
+      <c r="D158" s="29"/>
+      <c r="E158" s="13"/>
+      <c r="F158" s="13"/>
+      <c r="G158" s="13"/>
+      <c r="H158" s="5"/>
+      <c r="N158" s="28"/>
+      <c r="O158" s="28"/>
+      <c r="U158" s="28"/>
+      <c r="V158" s="28"/>
+      <c r="AB158" s="28"/>
+      <c r="AC158" s="28"/>
+      <c r="AI158" s="28"/>
+      <c r="AJ158" s="28"/>
+      <c r="AP158" s="28"/>
+      <c r="AQ158" s="28"/>
+      <c r="AW158" s="28"/>
+      <c r="AX158" s="28"/>
+      <c r="BD158" s="28"/>
+      <c r="BE158" s="28"/>
+      <c r="BK158" s="28"/>
+      <c r="BL158" s="28"/>
+      <c r="BR158" s="28"/>
+      <c r="BS158" s="28"/>
+      <c r="BY158" s="28"/>
+      <c r="BZ158" s="28"/>
       <c r="CE158" s="38"/>
-      <c r="CG158" s="38"/>
-      <c r="CI158" s="38"/>
-      <c r="CK158" s="38"/>
+      <c r="CF158" s="28"/>
+      <c r="CG158" s="28"/>
+      <c r="CM158" s="28"/>
+      <c r="CN158" s="28"/>
+      <c r="CT158" s="28"/>
+      <c r="CU158" s="28"/>
+      <c r="DA158" s="28"/>
+      <c r="DB158" s="28"/>
+      <c r="DH158" s="28"/>
+      <c r="DI158" s="28"/>
+      <c r="DO158" s="28"/>
+      <c r="DP158" s="28"/>
+      <c r="DV158" s="28"/>
+      <c r="DW158" s="28"/>
+      <c r="EC158" s="28"/>
+      <c r="ED158" s="28"/>
+      <c r="EJ158" s="28"/>
+      <c r="EK158" s="28"/>
+      <c r="EQ158" s="28"/>
+      <c r="ER158" s="28"/>
+      <c r="EX158" s="28"/>
+      <c r="EY158" s="28"/>
+      <c r="FE158" s="28"/>
+      <c r="FF158" s="28"/>
+      <c r="FL158" s="28"/>
+      <c r="FM158" s="28"/>
+      <c r="FS158" s="28"/>
+      <c r="FT158" s="28"/>
+      <c r="FZ158" s="28"/>
+      <c r="GA158" s="28"/>
+      <c r="GG158" s="28"/>
+      <c r="GH158" s="28"/>
+      <c r="GN158" s="28"/>
+      <c r="GO158" s="28"/>
+      <c r="GU158" s="28"/>
+      <c r="GV158" s="28"/>
+      <c r="HB158" s="28"/>
+      <c r="HC158" s="28"/>
+    </row>
+    <row r="159" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A159" s="25"/>
+      <c r="B159" s="26"/>
+      <c r="C159" s="47" t="s">
+        <v>193</v>
+      </c>
+      <c r="D159" s="29"/>
+      <c r="E159" s="13"/>
+      <c r="F159" s="13"/>
+      <c r="G159" s="13"/>
+      <c r="H159" s="5"/>
+      <c r="N159" s="28"/>
+      <c r="O159" s="28"/>
+      <c r="U159" s="28"/>
+      <c r="V159" s="28"/>
+      <c r="AB159" s="28"/>
+      <c r="AC159" s="28"/>
+      <c r="AI159" s="28"/>
+      <c r="AJ159" s="28"/>
+      <c r="AP159" s="28"/>
+      <c r="AQ159" s="28"/>
+      <c r="AW159" s="28"/>
+      <c r="AX159" s="28"/>
+      <c r="BD159" s="28"/>
+      <c r="BE159" s="28"/>
+      <c r="BK159" s="28"/>
+      <c r="BL159" s="28"/>
+      <c r="BR159" s="28"/>
+      <c r="BS159" s="28"/>
+      <c r="BY159" s="28"/>
+      <c r="BZ159" s="28"/>
+      <c r="CE159" s="38"/>
+      <c r="CF159" s="28"/>
+      <c r="CG159" s="28"/>
+      <c r="CM159" s="28"/>
+      <c r="CN159" s="28"/>
+      <c r="CT159" s="28"/>
+      <c r="CU159" s="28"/>
+      <c r="DA159" s="28"/>
+      <c r="DB159" s="28"/>
+      <c r="DH159" s="28"/>
+      <c r="DI159" s="28"/>
+      <c r="DO159" s="28"/>
+      <c r="DP159" s="28"/>
+      <c r="DV159" s="28"/>
+      <c r="DW159" s="28"/>
+      <c r="EC159" s="28"/>
+      <c r="ED159" s="28"/>
+      <c r="EJ159" s="28"/>
+      <c r="EK159" s="28"/>
+      <c r="EQ159" s="28"/>
+      <c r="ER159" s="28"/>
+      <c r="EX159" s="28"/>
+      <c r="EY159" s="28"/>
+      <c r="FE159" s="28"/>
+      <c r="FF159" s="28"/>
+      <c r="FL159" s="28"/>
+      <c r="FM159" s="28"/>
+      <c r="FS159" s="28"/>
+      <c r="FT159" s="28"/>
+      <c r="FZ159" s="28"/>
+      <c r="GA159" s="28"/>
+      <c r="GG159" s="28"/>
+      <c r="GH159" s="28"/>
+      <c r="GN159" s="28"/>
+      <c r="GO159" s="28"/>
+      <c r="GU159" s="28"/>
+      <c r="GV159" s="28"/>
+      <c r="HB159" s="28"/>
+      <c r="HC159" s="28"/>
+    </row>
+    <row r="160" spans="1:211">
+      <c r="A160" s="14"/>
+      <c r="B160" s="14"/>
+      <c r="CE160" s="38"/>
+      <c r="CG160" s="38"/>
+      <c r="CI160" s="38"/>
+      <c r="CK160" s="38"/>
     </row>
   </sheetData>
   <sortState ref="A125:GL149">
@@ -14978,7 +15138,7 @@
     <mergeCell ref="A86:C86"/>
     <mergeCell ref="A125:C125"/>
   </mergeCells>
-  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU157 DJ8:DN157 DC8:DG157 EE8:EI157 CA8:CE157 AY8:BC157 AR8:AV157 AK8:AO157 AD8:AH157 BF66:BJ157 BM66:BQ157 BT66:BX157 W78:AA157 P60:T157 CV60:CZ157 CO69:CS157 DX114:EB157 CH60:CL157 EL8:EP157 ES8:EW157 EZ8:FD157 FG8:FK157 FN8:FR157 FU8:FY157 GB8:GF157 GI8:GM157 GP8:GT157 GW8:HA157 J69:M157">
+  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU159 DJ8:DN159 DC8:DG159 EE8:EI159 CA8:CE159 AY8:BC159 AR8:AV159 AK8:AO159 AD8:AH159 BF66:BJ159 BM66:BQ159 BT66:BX159 W78:AA159 P60:T159 CV60:CZ159 CO69:CS159 DX114:EB159 CH60:CL159 EL8:EP159 ES8:EW159 EZ8:FD159 FG8:FK159 FN8:FR159 FU8:FY159 GB8:GF159 GI8:GM159 GP8:GT159 GW8:HA159 J69:M159">
     <cfRule type="expression" dxfId="24" priority="92">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -15004,7 +15164,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A158:HC158">
+  <conditionalFormatting sqref="A160:HC160">
     <cfRule type="expression" dxfId="16" priority="91">
       <formula>TRUE</formula>
     </cfRule>
@@ -15050,9 +15210,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AO238"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15182,6 +15342,15 @@
     <row r="9" spans="1:41">
       <c r="A9" s="36">
         <v>5</v>
+      </c>
+      <c r="B9" s="33">
+        <v>41724</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:41">

</xml_diff>

<commit_message>
-Validation of having at least one item in RFQ detail list inside RFQ Form. -Bug resolved: Overlay layer for validations black in IE8. -Reason field required when the vendor choses no quote.
</commit_message>
<xml_diff>
--- a/AQPM Gantt.xlsx
+++ b/AQPM Gantt.xlsx
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="199">
   <si>
     <t>Plan</t>
   </si>
@@ -774,6 +774,21 @@
   </si>
   <si>
     <t>Export Sales Report component processed without RFQ</t>
+  </si>
+  <si>
+    <t>Add Vendor's phone in RFQ form</t>
+  </si>
+  <si>
+    <t>Be able to Select RFQ as a winner in BOM</t>
+  </si>
+  <si>
+    <t>5 decimal places in RFQ form</t>
+  </si>
+  <si>
+    <t>I removed the overlay layer for Dialogs</t>
+  </si>
+  <si>
+    <t>Validation with black background in IE8</t>
   </si>
 </sst>
 </file>
@@ -1920,13 +1935,13 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:HC160"/>
+  <dimension ref="A2:HC163"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="FO125" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="7" topLeftCell="J146" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="F137" sqref="F137"/>
+      <selection pane="bottomRight" activeCell="L157" sqref="L157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25"/>
@@ -15120,13 +15135,226 @@
       <c r="HB159" s="28"/>
       <c r="HC159" s="28"/>
     </row>
-    <row r="160" spans="1:211">
-      <c r="A160" s="14"/>
-      <c r="B160" s="14"/>
+    <row r="160" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A160" s="25"/>
+      <c r="B160" s="26"/>
+      <c r="C160" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="D160" s="29"/>
+      <c r="E160" s="13"/>
+      <c r="F160" s="13"/>
+      <c r="G160" s="13"/>
+      <c r="H160" s="5"/>
+      <c r="N160" s="28"/>
+      <c r="O160" s="28"/>
+      <c r="U160" s="28"/>
+      <c r="V160" s="28"/>
+      <c r="AB160" s="28"/>
+      <c r="AC160" s="28"/>
+      <c r="AI160" s="28"/>
+      <c r="AJ160" s="28"/>
+      <c r="AP160" s="28"/>
+      <c r="AQ160" s="28"/>
+      <c r="AW160" s="28"/>
+      <c r="AX160" s="28"/>
+      <c r="BD160" s="28"/>
+      <c r="BE160" s="28"/>
+      <c r="BK160" s="28"/>
+      <c r="BL160" s="28"/>
+      <c r="BR160" s="28"/>
+      <c r="BS160" s="28"/>
+      <c r="BY160" s="28"/>
+      <c r="BZ160" s="28"/>
       <c r="CE160" s="38"/>
-      <c r="CG160" s="38"/>
-      <c r="CI160" s="38"/>
-      <c r="CK160" s="38"/>
+      <c r="CF160" s="28"/>
+      <c r="CG160" s="28"/>
+      <c r="CM160" s="28"/>
+      <c r="CN160" s="28"/>
+      <c r="CT160" s="28"/>
+      <c r="CU160" s="28"/>
+      <c r="DA160" s="28"/>
+      <c r="DB160" s="28"/>
+      <c r="DH160" s="28"/>
+      <c r="DI160" s="28"/>
+      <c r="DO160" s="28"/>
+      <c r="DP160" s="28"/>
+      <c r="DV160" s="28"/>
+      <c r="DW160" s="28"/>
+      <c r="EC160" s="28"/>
+      <c r="ED160" s="28"/>
+      <c r="EJ160" s="28"/>
+      <c r="EK160" s="28"/>
+      <c r="EQ160" s="28"/>
+      <c r="ER160" s="28"/>
+      <c r="EX160" s="28"/>
+      <c r="EY160" s="28"/>
+      <c r="FE160" s="28"/>
+      <c r="FF160" s="28"/>
+      <c r="FL160" s="28"/>
+      <c r="FM160" s="28"/>
+      <c r="FS160" s="28"/>
+      <c r="FT160" s="28"/>
+      <c r="FZ160" s="28"/>
+      <c r="GA160" s="28"/>
+      <c r="GG160" s="28"/>
+      <c r="GH160" s="28"/>
+      <c r="GN160" s="28"/>
+      <c r="GO160" s="28"/>
+      <c r="GU160" s="28"/>
+      <c r="GV160" s="28"/>
+      <c r="HB160" s="28"/>
+      <c r="HC160" s="28"/>
+    </row>
+    <row r="161" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A161" s="25"/>
+      <c r="B161" s="26"/>
+      <c r="C161" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="D161" s="29"/>
+      <c r="E161" s="13"/>
+      <c r="F161" s="13"/>
+      <c r="G161" s="13"/>
+      <c r="H161" s="5"/>
+      <c r="N161" s="28"/>
+      <c r="O161" s="28"/>
+      <c r="U161" s="28"/>
+      <c r="V161" s="28"/>
+      <c r="AB161" s="28"/>
+      <c r="AC161" s="28"/>
+      <c r="AI161" s="28"/>
+      <c r="AJ161" s="28"/>
+      <c r="AP161" s="28"/>
+      <c r="AQ161" s="28"/>
+      <c r="AW161" s="28"/>
+      <c r="AX161" s="28"/>
+      <c r="BD161" s="28"/>
+      <c r="BE161" s="28"/>
+      <c r="BK161" s="28"/>
+      <c r="BL161" s="28"/>
+      <c r="BR161" s="28"/>
+      <c r="BS161" s="28"/>
+      <c r="BY161" s="28"/>
+      <c r="BZ161" s="28"/>
+      <c r="CE161" s="38"/>
+      <c r="CF161" s="28"/>
+      <c r="CG161" s="28"/>
+      <c r="CM161" s="28"/>
+      <c r="CN161" s="28"/>
+      <c r="CT161" s="28"/>
+      <c r="CU161" s="28"/>
+      <c r="DA161" s="28"/>
+      <c r="DB161" s="28"/>
+      <c r="DH161" s="28"/>
+      <c r="DI161" s="28"/>
+      <c r="DO161" s="28"/>
+      <c r="DP161" s="28"/>
+      <c r="DV161" s="28"/>
+      <c r="DW161" s="28"/>
+      <c r="EC161" s="28"/>
+      <c r="ED161" s="28"/>
+      <c r="EJ161" s="28"/>
+      <c r="EK161" s="28"/>
+      <c r="EQ161" s="28"/>
+      <c r="ER161" s="28"/>
+      <c r="EX161" s="28"/>
+      <c r="EY161" s="28"/>
+      <c r="FE161" s="28"/>
+      <c r="FF161" s="28"/>
+      <c r="FL161" s="28"/>
+      <c r="FM161" s="28"/>
+      <c r="FS161" s="28"/>
+      <c r="FT161" s="28"/>
+      <c r="FZ161" s="28"/>
+      <c r="GA161" s="28"/>
+      <c r="GG161" s="28"/>
+      <c r="GH161" s="28"/>
+      <c r="GN161" s="28"/>
+      <c r="GO161" s="28"/>
+      <c r="GU161" s="28"/>
+      <c r="GV161" s="28"/>
+      <c r="HB161" s="28"/>
+      <c r="HC161" s="28"/>
+    </row>
+    <row r="162" spans="1:211" ht="18.95" customHeight="1">
+      <c r="A162" s="25"/>
+      <c r="B162" s="26"/>
+      <c r="C162" s="47" t="s">
+        <v>196</v>
+      </c>
+      <c r="D162" s="29"/>
+      <c r="E162" s="13"/>
+      <c r="F162" s="13"/>
+      <c r="G162" s="13"/>
+      <c r="H162" s="5"/>
+      <c r="N162" s="28"/>
+      <c r="O162" s="28"/>
+      <c r="U162" s="28"/>
+      <c r="V162" s="28"/>
+      <c r="AB162" s="28"/>
+      <c r="AC162" s="28"/>
+      <c r="AI162" s="28"/>
+      <c r="AJ162" s="28"/>
+      <c r="AP162" s="28"/>
+      <c r="AQ162" s="28"/>
+      <c r="AW162" s="28"/>
+      <c r="AX162" s="28"/>
+      <c r="BD162" s="28"/>
+      <c r="BE162" s="28"/>
+      <c r="BK162" s="28"/>
+      <c r="BL162" s="28"/>
+      <c r="BR162" s="28"/>
+      <c r="BS162" s="28"/>
+      <c r="BY162" s="28"/>
+      <c r="BZ162" s="28"/>
+      <c r="CE162" s="38"/>
+      <c r="CF162" s="28"/>
+      <c r="CG162" s="28"/>
+      <c r="CM162" s="28"/>
+      <c r="CN162" s="28"/>
+      <c r="CT162" s="28"/>
+      <c r="CU162" s="28"/>
+      <c r="DA162" s="28"/>
+      <c r="DB162" s="28"/>
+      <c r="DH162" s="28"/>
+      <c r="DI162" s="28"/>
+      <c r="DO162" s="28"/>
+      <c r="DP162" s="28"/>
+      <c r="DV162" s="28"/>
+      <c r="DW162" s="28"/>
+      <c r="EC162" s="28"/>
+      <c r="ED162" s="28"/>
+      <c r="EJ162" s="28"/>
+      <c r="EK162" s="28"/>
+      <c r="EQ162" s="28"/>
+      <c r="ER162" s="28"/>
+      <c r="EX162" s="28"/>
+      <c r="EY162" s="28"/>
+      <c r="FE162" s="28"/>
+      <c r="FF162" s="28"/>
+      <c r="FL162" s="28"/>
+      <c r="FM162" s="28"/>
+      <c r="FS162" s="28"/>
+      <c r="FT162" s="28"/>
+      <c r="FZ162" s="28"/>
+      <c r="GA162" s="28"/>
+      <c r="GG162" s="28"/>
+      <c r="GH162" s="28"/>
+      <c r="GN162" s="28"/>
+      <c r="GO162" s="28"/>
+      <c r="GU162" s="28"/>
+      <c r="GV162" s="28"/>
+      <c r="HB162" s="28"/>
+      <c r="HC162" s="28"/>
+    </row>
+    <row r="163" spans="1:211">
+      <c r="A163" s="14"/>
+      <c r="B163" s="14"/>
+      <c r="CE163" s="38"/>
+      <c r="CG163" s="38"/>
+      <c r="CI163" s="38"/>
+      <c r="CK163" s="38"/>
     </row>
   </sheetData>
   <sortState ref="A125:GL149">
@@ -15138,7 +15366,7 @@
     <mergeCell ref="A86:C86"/>
     <mergeCell ref="A125:C125"/>
   </mergeCells>
-  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU159 DJ8:DN159 DC8:DG159 EE8:EI159 CA8:CE159 AY8:BC159 AR8:AV159 AK8:AO159 AD8:AH159 BF66:BJ159 BM66:BQ159 BT66:BX159 W78:AA159 P60:T159 CV60:CZ159 CO69:CS159 DX114:EB159 CH60:CL159 EL8:EP159 ES8:EW159 EZ8:FD159 FG8:FK159 FN8:FR159 FU8:FY159 GB8:GF159 GI8:GM159 GP8:GT159 GW8:HA159 J69:M159">
+  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU162 DJ8:DN162 DC8:DG162 EE8:EI162 CA8:CE162 AY8:BC162 AR8:AV162 AK8:AO162 AD8:AH162 BF66:BJ162 BM66:BQ162 BT66:BX162 W78:AA162 P60:T162 CV60:CZ162 CO69:CS162 DX114:EB162 CH60:CL162 EL8:EP162 ES8:EW162 EZ8:FD162 FG8:FK162 FN8:FR162 FU8:FY162 GB8:GF162 GI8:GM162 GP8:GT162 GW8:HA162 J69:M162">
     <cfRule type="expression" dxfId="24" priority="92">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -15164,7 +15392,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A160:HC160">
+  <conditionalFormatting sqref="A163:HC163">
     <cfRule type="expression" dxfId="16" priority="91">
       <formula>TRUE</formula>
     </cfRule>
@@ -15212,7 +15440,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15352,10 +15580,28 @@
       <c r="D9" s="36" t="s">
         <v>192</v>
       </c>
+      <c r="E9" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="10" spans="1:41">
       <c r="A10" s="36">
         <v>6</v>
+      </c>
+      <c r="B10" s="33">
+        <v>41738</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:41">

</xml_diff>

<commit_message>
-Bug solved: Importing all EAV from SalesDB.
</commit_message>
<xml_diff>
--- a/AQPM Gantt.xlsx
+++ b/AQPM Gantt.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="10305" yWindow="4335" windowWidth="10230" windowHeight="4350"/>
@@ -11,7 +11,7 @@
     <sheet name="Issues" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'APQM Gantt'!$A$7:$EK$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'APQM Gantt'!$A$7:$EK$129</definedName>
     <definedName name="Actual" localSheetId="0">('APQM Gantt'!PeriodInActual*('APQM Gantt'!$F1&gt;0))*'APQM Gantt'!PeriodInPlan</definedName>
     <definedName name="Actual">(PeriodInActual*(#REF!&gt;0))*PeriodInPlan</definedName>
     <definedName name="ActualBeyond" localSheetId="0">'APQM Gantt'!PeriodInActual*('APQM Gantt'!$F1&gt;0)</definedName>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="202">
   <si>
     <t>Plan</t>
   </si>
@@ -644,9 +644,6 @@
     <t>Use FS Commodities.</t>
   </si>
   <si>
-    <t>Leyend when sending RFQ depending id Aerospacial or Automotive</t>
-  </si>
-  <si>
     <t>Remove EAU validation from BOM Form</t>
   </si>
   <si>
@@ -683,9 +680,6 @@
     <t>Sales comments in BOM</t>
   </si>
   <si>
-    <t>RFQ form without javascript</t>
-  </si>
-  <si>
     <t>Manfucaturing Location and Ship fields belongs to RFQ as well</t>
   </si>
   <si>
@@ -698,9 +692,6 @@
     <t>Don’t delete records, just set to inactive</t>
   </si>
   <si>
-    <t>Close RFQ after  hiting save or cancel</t>
-  </si>
-  <si>
     <t>Remove from SIF List column Cost Model Loc</t>
   </si>
   <si>
@@ -789,16 +780,34 @@
   </si>
   <si>
     <t>Validation with black background in IE8</t>
+  </si>
+  <si>
+    <t>Leyend when sending RFQ depending if Aerospacial or Automotive</t>
+  </si>
+  <si>
+    <t>Move old data of Lead Times to new columns</t>
+  </si>
+  <si>
+    <t>EAUs are being imported only for the first 3 years</t>
+  </si>
+  <si>
+    <t>[% per Award Yr] column is not standarized, therefore my code was not found them</t>
+  </si>
+  <si>
+    <t>Attachments in IE8</t>
+  </si>
+  <si>
+    <t>Close RFQ after hiting save or cancel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -950,7 +959,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1028,14 +1037,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1075,6 +1078,21 @@
       <top/>
       <bottom style="thin">
         <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1243,9 +1261,6 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1264,14 +1279,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1285,134 +1303,6 @@
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
   <dxfs count="25">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1668,6 +1558,134 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1690,16 +1708,66 @@
 </styleSheet>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="155" min="1" page="10" val="140"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>152400</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>247650</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2049" name="Spinner 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="24">
   <autoFilter ref="A4:F238"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="5"/>
-    <tableColumn id="2" name="Date" dataDxfId="4"/>
-    <tableColumn id="3" name="Creator" dataDxfId="3"/>
-    <tableColumn id="4" name="Issue" dataDxfId="2"/>
-    <tableColumn id="5" name="Status" dataDxfId="1"/>
-    <tableColumn id="6" name="Solution" dataDxfId="0"/>
+    <tableColumn id="1" name="#" dataDxfId="23"/>
+    <tableColumn id="2" name="Date" dataDxfId="22"/>
+    <tableColumn id="3" name="Creator" dataDxfId="21"/>
+    <tableColumn id="4" name="Issue" dataDxfId="20"/>
+    <tableColumn id="5" name="Status" dataDxfId="19"/>
+    <tableColumn id="6" name="Solution" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1931,20 +1999,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:HC163"/>
+  <dimension ref="A2:HC166"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="J146" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="7" topLeftCell="J116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="L157" sqref="L157"/>
+      <selection pane="bottomRight" activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.375" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
@@ -1957,22 +2025,22 @@
     <col min="212" max="16384" width="2.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:211" ht="15" customHeight="1">
-      <c r="A2" s="56" t="s">
+    <row r="2" spans="1:211" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:211" ht="21" customHeight="1">
-      <c r="A3" s="56"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
+    <row r="3" spans="1:211" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="54"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
       <c r="D3" s="19" t="s">
         <v>13</v>
       </c>
@@ -2003,35 +2071,35 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:211" ht="21" customHeight="1">
-      <c r="A4" s="56"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
+    <row r="4" spans="1:211" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="44"/>
       <c r="E4" s="32"/>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:211" ht="28.5">
+    <row r="5" spans="1:211" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B5" s="22"/>
       <c r="C5" s="15"/>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="52" t="s">
+      <c r="F5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="52" t="s">
+      <c r="H5" s="51" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="11"/>
@@ -2642,7 +2710,7 @@
         <v>41756</v>
       </c>
     </row>
-    <row r="6" spans="1:211" ht="13.5" customHeight="1">
+    <row r="6" spans="1:211" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>34</v>
       </c>
@@ -2687,7 +2755,7 @@
       <c r="X6" s="23"/>
       <c r="Y6" s="23"/>
     </row>
-    <row r="7" spans="1:211" ht="15.75" customHeight="1">
+    <row r="7" spans="1:211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -3304,7 +3372,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:211" ht="18.95" customHeight="1">
+    <row r="8" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>15</v>
       </c>
@@ -3388,7 +3456,7 @@
       <c r="HB8" s="28"/>
       <c r="HC8" s="28"/>
     </row>
-    <row r="9" spans="1:211" ht="18.95" customHeight="1">
+    <row r="9" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>27</v>
       </c>
@@ -3474,7 +3542,7 @@
       <c r="HB9" s="28"/>
       <c r="HC9" s="28"/>
     </row>
-    <row r="10" spans="1:211" ht="18.95" customHeight="1">
+    <row r="10" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>16</v>
       </c>
@@ -3558,7 +3626,7 @@
       <c r="HB10" s="28"/>
       <c r="HC10" s="28"/>
     </row>
-    <row r="11" spans="1:211" ht="18.95" customHeight="1">
+    <row r="11" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>15</v>
       </c>
@@ -3642,7 +3710,7 @@
       <c r="HB11" s="28"/>
       <c r="HC11" s="28"/>
     </row>
-    <row r="12" spans="1:211" ht="18.95" customHeight="1">
+    <row r="12" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>15</v>
       </c>
@@ -3722,7 +3790,7 @@
       <c r="HB12" s="28"/>
       <c r="HC12" s="28"/>
     </row>
-    <row r="13" spans="1:211" ht="18.95" customHeight="1">
+    <row r="13" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>20</v>
       </c>
@@ -3809,7 +3877,7 @@
       <c r="HB13" s="28"/>
       <c r="HC13" s="28"/>
     </row>
-    <row r="14" spans="1:211" ht="18.95" customHeight="1">
+    <row r="14" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>16</v>
       </c>
@@ -3893,7 +3961,7 @@
       <c r="HB14" s="28"/>
       <c r="HC14" s="28"/>
     </row>
-    <row r="15" spans="1:211" ht="18.95" customHeight="1">
+    <row r="15" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>15</v>
       </c>
@@ -3979,7 +4047,7 @@
       <c r="HB15" s="28"/>
       <c r="HC15" s="28"/>
     </row>
-    <row r="16" spans="1:211" ht="18.95" customHeight="1">
+    <row r="16" spans="1:211" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>16</v>
       </c>
@@ -4063,15 +4131,15 @@
       <c r="HB16" s="28"/>
       <c r="HC16" s="28"/>
     </row>
-    <row r="17" spans="1:211" ht="18.95" customHeight="1">
+    <row r="17" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="26"/>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="50" t="s">
+      <c r="D17" s="49" t="s">
         <v>92</v>
       </c>
       <c r="E17" s="43"/>
@@ -4143,12 +4211,12 @@
       <c r="HB17" s="28"/>
       <c r="HC17" s="28"/>
     </row>
-    <row r="18" spans="1:211" ht="18.95" customHeight="1">
+    <row r="18" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="26"/>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="47" t="s">
         <v>90</v>
       </c>
       <c r="D18" s="41"/>
@@ -4221,15 +4289,15 @@
       <c r="HB18" s="28"/>
       <c r="HC18" s="28"/>
     </row>
-    <row r="19" spans="1:211" ht="18.95" customHeight="1">
+    <row r="19" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="26"/>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="50" t="s">
+      <c r="D19" s="49" t="s">
         <v>92</v>
       </c>
       <c r="E19" s="43"/>
@@ -4301,15 +4369,15 @@
       <c r="HB19" s="28"/>
       <c r="HC19" s="28"/>
     </row>
-    <row r="20" spans="1:211" ht="18.95" customHeight="1">
+    <row r="20" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="26"/>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="50" t="s">
+      <c r="D20" s="49" t="s">
         <v>92</v>
       </c>
       <c r="E20" s="43"/>
@@ -4381,7 +4449,7 @@
       <c r="HB20" s="28"/>
       <c r="HC20" s="28"/>
     </row>
-    <row r="21" spans="1:211" ht="18.95" customHeight="1">
+    <row r="21" spans="1:211" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>111</v>
       </c>
@@ -4465,7 +4533,7 @@
       <c r="HB21" s="28"/>
       <c r="HC21" s="28"/>
     </row>
-    <row r="22" spans="1:211" ht="18.95" customHeight="1">
+    <row r="22" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>111</v>
       </c>
@@ -4543,7 +4611,7 @@
       <c r="HB22" s="28"/>
       <c r="HC22" s="28"/>
     </row>
-    <row r="23" spans="1:211" ht="18.95" customHeight="1">
+    <row r="23" spans="1:211" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>15</v>
       </c>
@@ -4627,7 +4695,7 @@
       <c r="HB23" s="28"/>
       <c r="HC23" s="28"/>
     </row>
-    <row r="24" spans="1:211" ht="18.95" customHeight="1">
+    <row r="24" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>18</v>
       </c>
@@ -4711,7 +4779,7 @@
       <c r="HB24" s="28"/>
       <c r="HC24" s="28"/>
     </row>
-    <row r="25" spans="1:211" ht="18.95" customHeight="1">
+    <row r="25" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>18</v>
       </c>
@@ -4795,7 +4863,7 @@
       <c r="HB25" s="28"/>
       <c r="HC25" s="28"/>
     </row>
-    <row r="26" spans="1:211" ht="18.95" customHeight="1">
+    <row r="26" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>18</v>
       </c>
@@ -4879,7 +4947,7 @@
       <c r="HB26" s="28"/>
       <c r="HC26" s="28"/>
     </row>
-    <row r="27" spans="1:211" ht="18.95" customHeight="1">
+    <row r="27" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>18</v>
       </c>
@@ -4963,7 +5031,7 @@
       <c r="HB27" s="28"/>
       <c r="HC27" s="28"/>
     </row>
-    <row r="28" spans="1:211" ht="18.95" customHeight="1">
+    <row r="28" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
       <c r="B28" s="26"/>
       <c r="C28" s="40" t="s">
@@ -5039,7 +5107,7 @@
       <c r="HB28" s="28"/>
       <c r="HC28" s="28"/>
     </row>
-    <row r="29" spans="1:211" ht="18.95" customHeight="1">
+    <row r="29" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>20</v>
       </c>
@@ -5117,7 +5185,7 @@
       <c r="HB29" s="28"/>
       <c r="HC29" s="28"/>
     </row>
-    <row r="30" spans="1:211" ht="18.95" customHeight="1">
+    <row r="30" spans="1:211" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>24</v>
       </c>
@@ -5195,7 +5263,7 @@
       <c r="HB30" s="28"/>
       <c r="HC30" s="28"/>
     </row>
-    <row r="31" spans="1:211" ht="18.95" customHeight="1">
+    <row r="31" spans="1:211" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>18</v>
       </c>
@@ -5279,7 +5347,7 @@
       <c r="HB31" s="28"/>
       <c r="HC31" s="28"/>
     </row>
-    <row r="32" spans="1:211" ht="18.95" customHeight="1">
+    <row r="32" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>20</v>
       </c>
@@ -5357,7 +5425,7 @@
       <c r="HB32" s="28"/>
       <c r="HC32" s="28"/>
     </row>
-    <row r="33" spans="1:211" ht="18.95" customHeight="1">
+    <row r="33" spans="1:211" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>18</v>
       </c>
@@ -5435,7 +5503,7 @@
       <c r="HB33" s="28"/>
       <c r="HC33" s="28"/>
     </row>
-    <row r="34" spans="1:211" ht="18.95" customHeight="1">
+    <row r="34" spans="1:211" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>16</v>
       </c>
@@ -5513,7 +5581,7 @@
       <c r="HB34" s="28"/>
       <c r="HC34" s="28"/>
     </row>
-    <row r="35" spans="1:211" ht="18.95" customHeight="1">
+    <row r="35" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>25</v>
       </c>
@@ -5591,7 +5659,7 @@
       <c r="HB35" s="28"/>
       <c r="HC35" s="28"/>
     </row>
-    <row r="36" spans="1:211" ht="18.95" customHeight="1">
+    <row r="36" spans="1:211" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>25</v>
       </c>
@@ -5669,7 +5737,7 @@
       <c r="HB36" s="28"/>
       <c r="HC36" s="28"/>
     </row>
-    <row r="37" spans="1:211" ht="18.95" customHeight="1">
+    <row r="37" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>20</v>
       </c>
@@ -5747,14 +5815,14 @@
       <c r="HB37" s="28"/>
       <c r="HC37" s="28"/>
     </row>
-    <row r="38" spans="1:211" ht="18.95" customHeight="1">
+    <row r="38" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B38" s="26">
         <v>2</v>
       </c>
-      <c r="C38" s="48" t="s">
+      <c r="C38" s="47" t="s">
         <v>26</v>
       </c>
       <c r="D38" s="29">
@@ -5831,7 +5899,7 @@
       <c r="HB38" s="28"/>
       <c r="HC38" s="28"/>
     </row>
-    <row r="39" spans="1:211" ht="18.95" customHeight="1">
+    <row r="39" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>18</v>
       </c>
@@ -5915,7 +5983,7 @@
       <c r="HB39" s="28"/>
       <c r="HC39" s="28"/>
     </row>
-    <row r="40" spans="1:211" ht="18.95" customHeight="1">
+    <row r="40" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>25</v>
       </c>
@@ -5993,7 +6061,7 @@
       <c r="HB40" s="28"/>
       <c r="HC40" s="28"/>
     </row>
-    <row r="41" spans="1:211" ht="18.95" customHeight="1">
+    <row r="41" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>25</v>
       </c>
@@ -6071,7 +6139,7 @@
       <c r="HB41" s="28"/>
       <c r="HC41" s="28"/>
     </row>
-    <row r="42" spans="1:211" ht="18.95" customHeight="1">
+    <row r="42" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>16</v>
       </c>
@@ -6149,7 +6217,7 @@
       <c r="HB42" s="28"/>
       <c r="HC42" s="28"/>
     </row>
-    <row r="43" spans="1:211" ht="18.95" customHeight="1">
+    <row r="43" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>18</v>
       </c>
@@ -6229,7 +6297,7 @@
       <c r="HB43" s="28"/>
       <c r="HC43" s="28"/>
     </row>
-    <row r="44" spans="1:211" ht="18.95" customHeight="1">
+    <row r="44" spans="1:211" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
         <v>111</v>
       </c>
@@ -6307,7 +6375,7 @@
       <c r="HB44" s="28"/>
       <c r="HC44" s="28"/>
     </row>
-    <row r="45" spans="1:211" ht="18.95" customHeight="1">
+    <row r="45" spans="1:211" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>25</v>
       </c>
@@ -6385,7 +6453,7 @@
       <c r="HB45" s="28"/>
       <c r="HC45" s="28"/>
     </row>
-    <row r="46" spans="1:211" ht="18.95" customHeight="1">
+    <row r="46" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
         <v>25</v>
       </c>
@@ -6463,7 +6531,7 @@
       <c r="HB46" s="28"/>
       <c r="HC46" s="28"/>
     </row>
-    <row r="47" spans="1:211" ht="18.95" customHeight="1">
+    <row r="47" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
         <v>18</v>
       </c>
@@ -6542,7 +6610,7 @@
       <c r="HB47" s="28"/>
       <c r="HC47" s="28"/>
     </row>
-    <row r="48" spans="1:211" ht="18.95" customHeight="1">
+    <row r="48" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
         <v>18</v>
       </c>
@@ -6620,7 +6688,7 @@
       <c r="HB48" s="28"/>
       <c r="HC48" s="28"/>
     </row>
-    <row r="49" spans="1:211" ht="18.95" customHeight="1">
+    <row r="49" spans="1:211" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
         <v>18</v>
       </c>
@@ -6698,7 +6766,7 @@
       <c r="HB49" s="28"/>
       <c r="HC49" s="28"/>
     </row>
-    <row r="50" spans="1:211" ht="18.95" customHeight="1">
+    <row r="50" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
         <v>18</v>
       </c>
@@ -6776,7 +6844,7 @@
       <c r="HB50" s="28"/>
       <c r="HC50" s="28"/>
     </row>
-    <row r="51" spans="1:211" ht="18.95" customHeight="1">
+    <row r="51" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
         <v>18</v>
       </c>
@@ -6860,7 +6928,7 @@
       <c r="HB51" s="28"/>
       <c r="HC51" s="28"/>
     </row>
-    <row r="52" spans="1:211" ht="18.95" customHeight="1">
+    <row r="52" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
         <v>16</v>
       </c>
@@ -6938,7 +7006,7 @@
       <c r="HB52" s="28"/>
       <c r="HC52" s="28"/>
     </row>
-    <row r="53" spans="1:211" ht="18.95" customHeight="1">
+    <row r="53" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="25" t="s">
         <v>18</v>
       </c>
@@ -7016,7 +7084,7 @@
       <c r="HB53" s="28"/>
       <c r="HC53" s="28"/>
     </row>
-    <row r="54" spans="1:211" ht="18.95" customHeight="1">
+    <row r="54" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="25" t="s">
         <v>24</v>
       </c>
@@ -7096,7 +7164,7 @@
       <c r="HB54" s="28"/>
       <c r="HC54" s="28"/>
     </row>
-    <row r="55" spans="1:211" ht="18.95" customHeight="1">
+    <row r="55" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="25" t="s">
         <v>15</v>
       </c>
@@ -7176,7 +7244,7 @@
       <c r="HB55" s="28"/>
       <c r="HC55" s="28"/>
     </row>
-    <row r="56" spans="1:211" ht="18.95" customHeight="1">
+    <row r="56" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
         <v>24</v>
       </c>
@@ -7254,7 +7322,7 @@
       <c r="HB56" s="28"/>
       <c r="HC56" s="28"/>
     </row>
-    <row r="57" spans="1:211" ht="18.95" customHeight="1">
+    <row r="57" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="25" t="s">
         <v>20</v>
       </c>
@@ -7332,14 +7400,14 @@
       <c r="HB57" s="28"/>
       <c r="HC57" s="28"/>
     </row>
-    <row r="58" spans="1:211" ht="18.95" customHeight="1">
+    <row r="58" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B58" s="26">
         <v>3</v>
       </c>
-      <c r="C58" s="48" t="s">
+      <c r="C58" s="47" t="s">
         <v>30</v>
       </c>
       <c r="D58" s="29">
@@ -7416,14 +7484,14 @@
       <c r="HB58" s="28"/>
       <c r="HC58" s="28"/>
     </row>
-    <row r="59" spans="1:211" ht="18.95" customHeight="1">
+    <row r="59" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B59" s="26">
         <v>3</v>
       </c>
-      <c r="C59" s="48" t="s">
+      <c r="C59" s="47" t="s">
         <v>65</v>
       </c>
       <c r="D59" s="29">
@@ -7500,7 +7568,7 @@
       <c r="HB59" s="28"/>
       <c r="HC59" s="28"/>
     </row>
-    <row r="60" spans="1:211" ht="18.95" customHeight="1">
+    <row r="60" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="25" t="s">
         <v>20</v>
       </c>
@@ -7584,7 +7652,7 @@
       <c r="HB60" s="28"/>
       <c r="HC60" s="28"/>
     </row>
-    <row r="61" spans="1:211" ht="18.95" customHeight="1">
+    <row r="61" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="25" t="s">
         <v>20</v>
       </c>
@@ -7664,7 +7732,7 @@
       <c r="HB61" s="28"/>
       <c r="HC61" s="28"/>
     </row>
-    <row r="62" spans="1:211" ht="18.95" customHeight="1">
+    <row r="62" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
         <v>27</v>
       </c>
@@ -7742,7 +7810,7 @@
       <c r="HB62" s="28"/>
       <c r="HC62" s="28"/>
     </row>
-    <row r="63" spans="1:211" ht="18.95" customHeight="1">
+    <row r="63" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="25" t="s">
         <v>20</v>
       </c>
@@ -7822,7 +7890,7 @@
       <c r="HB63" s="28"/>
       <c r="HC63" s="28"/>
     </row>
-    <row r="64" spans="1:211" ht="18.95" customHeight="1">
+    <row r="64" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
         <v>16</v>
       </c>
@@ -7902,7 +7970,7 @@
       <c r="HB64" s="28"/>
       <c r="HC64" s="28"/>
     </row>
-    <row r="65" spans="1:211" ht="18.95" customHeight="1">
+    <row r="65" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="25" t="s">
         <v>27</v>
       </c>
@@ -7980,7 +8048,7 @@
       <c r="HB65" s="28"/>
       <c r="HC65" s="28"/>
     </row>
-    <row r="66" spans="1:211" ht="18.95" customHeight="1">
+    <row r="66" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="25" t="s">
         <v>18</v>
       </c>
@@ -8062,7 +8130,7 @@
       <c r="HB66" s="28"/>
       <c r="HC66" s="28"/>
     </row>
-    <row r="67" spans="1:211" ht="18.95" customHeight="1">
+    <row r="67" spans="1:211" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="25" t="s">
         <v>27</v>
       </c>
@@ -8144,7 +8212,7 @@
       <c r="HB67" s="28"/>
       <c r="HC67" s="28"/>
     </row>
-    <row r="68" spans="1:211" ht="18.95" customHeight="1">
+    <row r="68" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="25"/>
       <c r="B68" s="26"/>
       <c r="C68" s="40"/>
@@ -8212,7 +8280,7 @@
       <c r="HB68" s="28"/>
       <c r="HC68" s="28"/>
     </row>
-    <row r="69" spans="1:211" ht="18.95" customHeight="1">
+    <row r="69" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="25"/>
       <c r="B69" s="26"/>
       <c r="C69" s="27"/>
@@ -8280,12 +8348,12 @@
       <c r="HB69" s="28"/>
       <c r="HC69" s="28"/>
     </row>
-    <row r="70" spans="1:211" ht="18.95" customHeight="1">
-      <c r="A70" s="55" t="s">
+    <row r="70" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="55"/>
-      <c r="C70" s="55"/>
+      <c r="B70" s="53"/>
+      <c r="C70" s="53"/>
       <c r="D70" s="29"/>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
@@ -8350,14 +8418,14 @@
       <c r="HB70" s="28"/>
       <c r="HC70" s="28"/>
     </row>
-    <row r="71" spans="1:211" ht="18.95" customHeight="1">
+    <row r="71" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B71" s="26">
         <v>3</v>
       </c>
-      <c r="C71" s="48" t="s">
+      <c r="C71" s="47" t="s">
         <v>79</v>
       </c>
       <c r="D71" s="29">
@@ -8434,7 +8502,7 @@
       <c r="HB71" s="28"/>
       <c r="HC71" s="28"/>
     </row>
-    <row r="72" spans="1:211" ht="18.95" customHeight="1">
+    <row r="72" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="25" t="s">
         <v>24</v>
       </c>
@@ -8518,7 +8586,7 @@
       <c r="HB72" s="28"/>
       <c r="HC72" s="28"/>
     </row>
-    <row r="73" spans="1:211" ht="18.95" customHeight="1">
+    <row r="73" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="25" t="s">
         <v>18</v>
       </c>
@@ -8602,14 +8670,14 @@
       <c r="HB73" s="28"/>
       <c r="HC73" s="28"/>
     </row>
-    <row r="74" spans="1:211" ht="18.95" customHeight="1">
+    <row r="74" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B74" s="26">
         <v>3</v>
       </c>
-      <c r="C74" s="53" t="s">
+      <c r="C74" s="52" t="s">
         <v>75</v>
       </c>
       <c r="D74" s="29">
@@ -8686,14 +8754,14 @@
       <c r="HB74" s="28"/>
       <c r="HC74" s="28"/>
     </row>
-    <row r="75" spans="1:211" ht="18.95" customHeight="1">
+    <row r="75" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B75" s="26">
         <v>3</v>
       </c>
-      <c r="C75" s="53" t="s">
+      <c r="C75" s="52" t="s">
         <v>114</v>
       </c>
       <c r="D75" s="29">
@@ -8770,14 +8838,14 @@
       <c r="HB75" s="28"/>
       <c r="HC75" s="28"/>
     </row>
-    <row r="76" spans="1:211" ht="18.95" customHeight="1">
+    <row r="76" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B76" s="26">
         <v>3</v>
       </c>
-      <c r="C76" s="53" t="s">
+      <c r="C76" s="52" t="s">
         <v>73</v>
       </c>
       <c r="D76" s="29">
@@ -8854,7 +8922,7 @@
       <c r="HB76" s="28"/>
       <c r="HC76" s="28"/>
     </row>
-    <row r="77" spans="1:211" ht="18.95" customHeight="1">
+    <row r="77" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="25" t="s">
         <v>27</v>
       </c>
@@ -8885,7 +8953,7 @@
       <c r="V77" s="28"/>
       <c r="W77" s="39"/>
       <c r="X77" s="39"/>
-      <c r="Y77" s="49"/>
+      <c r="Y77" s="48"/>
       <c r="AB77" s="28"/>
       <c r="AC77" s="28"/>
       <c r="AI77" s="28"/>
@@ -8941,7 +9009,7 @@
       <c r="HB77" s="28"/>
       <c r="HC77" s="28"/>
     </row>
-    <row r="78" spans="1:211" ht="18.95" customHeight="1">
+    <row r="78" spans="1:211" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="25" t="s">
         <v>18</v>
       </c>
@@ -9025,7 +9093,7 @@
       <c r="HB78" s="28"/>
       <c r="HC78" s="28"/>
     </row>
-    <row r="79" spans="1:211" ht="18.95" customHeight="1">
+    <row r="79" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="25" t="s">
         <v>24</v>
       </c>
@@ -9103,7 +9171,7 @@
       <c r="HB79" s="28"/>
       <c r="HC79" s="28"/>
     </row>
-    <row r="80" spans="1:211" ht="18.95" customHeight="1">
+    <row r="80" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="25" t="s">
         <v>25</v>
       </c>
@@ -9183,7 +9251,7 @@
       <c r="HB80" s="28"/>
       <c r="HC80" s="28"/>
     </row>
-    <row r="81" spans="1:211" ht="18.95" customHeight="1">
+    <row r="81" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="25"/>
       <c r="B81" s="26"/>
       <c r="C81" s="27"/>
@@ -9251,14 +9319,14 @@
       <c r="HB81" s="28"/>
       <c r="HC81" s="28"/>
     </row>
-    <row r="82" spans="1:211" ht="18.95" customHeight="1">
+    <row r="82" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B82" s="26">
         <v>1</v>
       </c>
-      <c r="C82" s="51" t="s">
+      <c r="C82" s="50" t="s">
         <v>112</v>
       </c>
       <c r="D82" s="29">
@@ -9329,14 +9397,14 @@
       <c r="HB82" s="28"/>
       <c r="HC82" s="28"/>
     </row>
-    <row r="83" spans="1:211" ht="18.95" customHeight="1">
+    <row r="83" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B83" s="26">
         <v>1</v>
       </c>
-      <c r="C83" s="51" t="s">
+      <c r="C83" s="50" t="s">
         <v>110</v>
       </c>
       <c r="D83" s="29">
@@ -9407,7 +9475,7 @@
       <c r="HB83" s="28"/>
       <c r="HC83" s="28"/>
     </row>
-    <row r="84" spans="1:211" ht="18.95" customHeight="1">
+    <row r="84" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="25"/>
       <c r="B84" s="26"/>
       <c r="C84" s="27"/>
@@ -9475,7 +9543,7 @@
       <c r="HB84" s="28"/>
       <c r="HC84" s="28"/>
     </row>
-    <row r="85" spans="1:211" ht="18.95" customHeight="1">
+    <row r="85" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="25"/>
       <c r="B85" s="26"/>
       <c r="C85" s="27"/>
@@ -9543,12 +9611,12 @@
       <c r="HB85" s="28"/>
       <c r="HC85" s="28"/>
     </row>
-    <row r="86" spans="1:211" ht="18.95" customHeight="1">
-      <c r="A86" s="55" t="s">
+    <row r="86" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="B86" s="55"/>
-      <c r="C86" s="55"/>
+      <c r="B86" s="53"/>
+      <c r="C86" s="53"/>
       <c r="D86" s="29"/>
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
@@ -9613,12 +9681,12 @@
       <c r="HB86" s="28"/>
       <c r="HC86" s="28"/>
     </row>
-    <row r="87" spans="1:211" ht="18.95" customHeight="1">
+    <row r="87" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="25"/>
       <c r="B87" s="26">
         <v>5</v>
       </c>
-      <c r="C87" s="53" t="s">
+      <c r="C87" s="52" t="s">
         <v>116</v>
       </c>
       <c r="D87" s="29"/>
@@ -9691,7 +9759,7 @@
       <c r="HB87" s="28"/>
       <c r="HC87" s="28"/>
     </row>
-    <row r="88" spans="1:211" ht="18.95" customHeight="1">
+    <row r="88" spans="1:211" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="25"/>
       <c r="B88" s="26">
         <v>5</v>
@@ -9769,7 +9837,7 @@
       <c r="HB88" s="28"/>
       <c r="HC88" s="28"/>
     </row>
-    <row r="89" spans="1:211" ht="18.95" customHeight="1">
+    <row r="89" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="25"/>
       <c r="B89" s="26">
         <v>5</v>
@@ -9847,12 +9915,12 @@
       <c r="HB89" s="28"/>
       <c r="HC89" s="28"/>
     </row>
-    <row r="90" spans="1:211" ht="18.95" customHeight="1">
+    <row r="90" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="25"/>
       <c r="B90" s="26">
         <v>5</v>
       </c>
-      <c r="C90" s="53" t="s">
+      <c r="C90" s="52" t="s">
         <v>119</v>
       </c>
       <c r="D90" s="29"/>
@@ -9925,7 +9993,7 @@
       <c r="HB90" s="28"/>
       <c r="HC90" s="28"/>
     </row>
-    <row r="91" spans="1:211" ht="18.95" customHeight="1">
+    <row r="91" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="25"/>
       <c r="B91" s="26">
         <v>5</v>
@@ -10004,12 +10072,12 @@
       <c r="HB91" s="28"/>
       <c r="HC91" s="28"/>
     </row>
-    <row r="92" spans="1:211" ht="18.95" customHeight="1">
+    <row r="92" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="25"/>
       <c r="B92" s="26">
         <v>5</v>
       </c>
-      <c r="C92" s="53" t="s">
+      <c r="C92" s="52" t="s">
         <v>115</v>
       </c>
       <c r="D92" s="29"/>
@@ -10082,12 +10150,12 @@
       <c r="HB92" s="28"/>
       <c r="HC92" s="28"/>
     </row>
-    <row r="93" spans="1:211" ht="18.95" customHeight="1">
+    <row r="93" spans="1:211" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="25"/>
       <c r="B93" s="26">
         <v>5</v>
       </c>
-      <c r="C93" s="53" t="s">
+      <c r="C93" s="52" t="s">
         <v>118</v>
       </c>
       <c r="D93" s="29"/>
@@ -10160,7 +10228,7 @@
       <c r="HB93" s="28"/>
       <c r="HC93" s="28"/>
     </row>
-    <row r="94" spans="1:211" ht="18.95" customHeight="1">
+    <row r="94" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="25"/>
       <c r="B94" s="26">
         <v>5</v>
@@ -10239,12 +10307,12 @@
       <c r="HB94" s="28"/>
       <c r="HC94" s="28"/>
     </row>
-    <row r="95" spans="1:211" ht="18.95" customHeight="1">
+    <row r="95" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="25"/>
       <c r="B95" s="26">
         <v>4</v>
       </c>
-      <c r="C95" s="53" t="s">
+      <c r="C95" s="52" t="s">
         <v>127</v>
       </c>
       <c r="D95" s="29"/>
@@ -10317,12 +10385,12 @@
       <c r="HB95" s="28"/>
       <c r="HC95" s="28"/>
     </row>
-    <row r="96" spans="1:211" ht="18.95" customHeight="1">
+    <row r="96" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="25"/>
       <c r="B96" s="26">
         <v>4</v>
       </c>
-      <c r="C96" s="53" t="s">
+      <c r="C96" s="52" t="s">
         <v>124</v>
       </c>
       <c r="D96" s="29"/>
@@ -10396,12 +10464,12 @@
       <c r="HB96" s="28"/>
       <c r="HC96" s="28"/>
     </row>
-    <row r="97" spans="1:211" ht="18.95" customHeight="1">
+    <row r="97" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="25"/>
       <c r="B97" s="26">
         <v>4</v>
       </c>
-      <c r="C97" s="53" t="s">
+      <c r="C97" s="52" t="s">
         <v>126</v>
       </c>
       <c r="D97" s="29"/>
@@ -10475,12 +10543,12 @@
       <c r="HB97" s="28"/>
       <c r="HC97" s="28"/>
     </row>
-    <row r="98" spans="1:211" ht="18.95" customHeight="1">
+    <row r="98" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="25"/>
       <c r="B98" s="26">
         <v>3</v>
       </c>
-      <c r="C98" s="53" t="s">
+      <c r="C98" s="52" t="s">
         <v>132</v>
       </c>
       <c r="D98" s="29"/>
@@ -10554,12 +10622,12 @@
       <c r="HB98" s="28"/>
       <c r="HC98" s="28"/>
     </row>
-    <row r="99" spans="1:211" ht="18.95" customHeight="1">
+    <row r="99" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="25"/>
       <c r="B99" s="26">
         <v>3</v>
       </c>
-      <c r="C99" s="53" t="s">
+      <c r="C99" s="52" t="s">
         <v>134</v>
       </c>
       <c r="D99" s="29"/>
@@ -10633,12 +10701,12 @@
       <c r="HB99" s="28"/>
       <c r="HC99" s="28"/>
     </row>
-    <row r="100" spans="1:211" ht="18.95" customHeight="1">
+    <row r="100" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="25"/>
       <c r="B100" s="26">
         <v>1</v>
       </c>
-      <c r="C100" s="53" t="s">
+      <c r="C100" s="52" t="s">
         <v>130</v>
       </c>
       <c r="D100" s="29"/>
@@ -10712,12 +10780,12 @@
       <c r="HB100" s="28"/>
       <c r="HC100" s="28"/>
     </row>
-    <row r="101" spans="1:211" ht="18.95" customHeight="1">
+    <row r="101" spans="1:211" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="25"/>
       <c r="B101" s="26">
         <v>1</v>
       </c>
-      <c r="C101" s="53" t="s">
+      <c r="C101" s="52" t="s">
         <v>131</v>
       </c>
       <c r="D101" s="29"/>
@@ -10791,12 +10859,12 @@
       <c r="HB101" s="28"/>
       <c r="HC101" s="28"/>
     </row>
-    <row r="102" spans="1:211" ht="18.95" customHeight="1">
+    <row r="102" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="25"/>
       <c r="B102" s="26">
         <v>1</v>
       </c>
-      <c r="C102" s="53" t="s">
+      <c r="C102" s="52" t="s">
         <v>133</v>
       </c>
       <c r="D102" s="29"/>
@@ -10870,12 +10938,12 @@
       <c r="HB102" s="28"/>
       <c r="HC102" s="28"/>
     </row>
-    <row r="103" spans="1:211" ht="18.95" customHeight="1">
+    <row r="103" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="25"/>
       <c r="B103" s="26">
         <v>1</v>
       </c>
-      <c r="C103" s="53" t="s">
+      <c r="C103" s="52" t="s">
         <v>135</v>
       </c>
       <c r="D103" s="29"/>
@@ -10949,7 +11017,7 @@
       <c r="HB103" s="28"/>
       <c r="HC103" s="28"/>
     </row>
-    <row r="104" spans="1:211" ht="18.95" customHeight="1">
+    <row r="104" spans="1:211" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="25"/>
       <c r="B104" s="26">
         <v>3</v>
@@ -11028,7 +11096,7 @@
       <c r="HB104" s="28"/>
       <c r="HC104" s="28"/>
     </row>
-    <row r="105" spans="1:211" ht="18.95" customHeight="1">
+    <row r="105" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="25"/>
       <c r="B105" s="26">
         <v>3</v>
@@ -11107,12 +11175,12 @@
       <c r="HB105" s="28"/>
       <c r="HC105" s="28"/>
     </row>
-    <row r="106" spans="1:211" ht="18.95" customHeight="1">
+    <row r="106" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="25"/>
       <c r="B106" s="26">
         <v>2</v>
       </c>
-      <c r="C106" s="53" t="s">
+      <c r="C106" s="52" t="s">
         <v>122</v>
       </c>
       <c r="D106" s="29"/>
@@ -11185,12 +11253,12 @@
       <c r="HB106" s="28"/>
       <c r="HC106" s="28"/>
     </row>
-    <row r="107" spans="1:211" ht="18.95" customHeight="1">
+    <row r="107" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="25"/>
       <c r="B107" s="26">
         <v>2</v>
       </c>
-      <c r="C107" s="53" t="s">
+      <c r="C107" s="52" t="s">
         <v>141</v>
       </c>
       <c r="D107" s="29"/>
@@ -11264,12 +11332,12 @@
       <c r="HB107" s="28"/>
       <c r="HC107" s="28"/>
     </row>
-    <row r="108" spans="1:211" ht="18.95" customHeight="1">
+    <row r="108" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="25"/>
       <c r="B108" s="26">
         <v>3</v>
       </c>
-      <c r="C108" s="53" t="s">
+      <c r="C108" s="52" t="s">
         <v>145</v>
       </c>
       <c r="D108" s="29"/>
@@ -11344,12 +11412,12 @@
       <c r="HB108" s="28"/>
       <c r="HC108" s="28"/>
     </row>
-    <row r="109" spans="1:211" ht="18.95" customHeight="1">
+    <row r="109" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="25"/>
       <c r="B109" s="26">
         <v>1</v>
       </c>
-      <c r="C109" s="53" t="s">
+      <c r="C109" s="52" t="s">
         <v>129</v>
       </c>
       <c r="D109" s="29"/>
@@ -11423,10 +11491,10 @@
       <c r="HB109" s="28"/>
       <c r="HC109" s="28"/>
     </row>
-    <row r="110" spans="1:211" ht="18.95" customHeight="1">
+    <row r="110" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="25"/>
       <c r="B110" s="26"/>
-      <c r="C110" s="53" t="s">
+      <c r="C110" s="52" t="s">
         <v>143</v>
       </c>
       <c r="D110" s="29"/>
@@ -11500,12 +11568,12 @@
       <c r="HB110" s="28"/>
       <c r="HC110" s="28"/>
     </row>
-    <row r="111" spans="1:211" ht="18.95" customHeight="1">
+    <row r="111" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="25"/>
       <c r="B111" s="26">
         <v>3</v>
       </c>
-      <c r="C111" s="53" t="s">
+      <c r="C111" s="52" t="s">
         <v>144</v>
       </c>
       <c r="D111" s="29"/>
@@ -11579,10 +11647,10 @@
       <c r="HB111" s="28"/>
       <c r="HC111" s="28"/>
     </row>
-    <row r="112" spans="1:211" ht="18.95" customHeight="1">
+    <row r="112" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="25"/>
       <c r="B112" s="26"/>
-      <c r="C112" s="53" t="s">
+      <c r="C112" s="52" t="s">
         <v>146</v>
       </c>
       <c r="D112" s="29"/>
@@ -11656,12 +11724,12 @@
       <c r="HB112" s="28"/>
       <c r="HC112" s="28"/>
     </row>
-    <row r="113" spans="1:211" ht="18.95" customHeight="1">
+    <row r="113" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="25"/>
       <c r="B113" s="26">
         <v>1</v>
       </c>
-      <c r="C113" s="53" t="s">
+      <c r="C113" s="52" t="s">
         <v>140</v>
       </c>
       <c r="D113" s="29">
@@ -11739,11 +11807,11 @@
       <c r="HB113" s="28"/>
       <c r="HC113" s="28"/>
     </row>
-    <row r="114" spans="1:211" ht="18.95" customHeight="1">
+    <row r="114" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="25"/>
       <c r="B114" s="26"/>
-      <c r="C114" s="53" t="s">
-        <v>151</v>
+      <c r="C114" s="52" t="s">
+        <v>150</v>
       </c>
       <c r="D114" s="29"/>
       <c r="E114" s="13"/>
@@ -11816,11 +11884,11 @@
       <c r="HB114" s="28"/>
       <c r="HC114" s="28"/>
     </row>
-    <row r="115" spans="1:211" ht="18.95" customHeight="1">
+    <row r="115" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="25"/>
       <c r="B115" s="26"/>
-      <c r="C115" s="53" t="s">
-        <v>159</v>
+      <c r="C115" s="52" t="s">
+        <v>158</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="13">
@@ -11895,11 +11963,11 @@
       <c r="HB115" s="28"/>
       <c r="HC115" s="28"/>
     </row>
-    <row r="116" spans="1:211" ht="18.95" customHeight="1">
+    <row r="116" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="25"/>
       <c r="B116" s="26"/>
-      <c r="C116" s="53" t="s">
-        <v>161</v>
+      <c r="C116" s="52" t="s">
+        <v>160</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="13"/>
@@ -11972,11 +12040,11 @@
       <c r="HB116" s="28"/>
       <c r="HC116" s="28"/>
     </row>
-    <row r="117" spans="1:211" ht="18.95" customHeight="1">
+    <row r="117" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="25"/>
       <c r="B117" s="26"/>
-      <c r="C117" s="53" t="s">
-        <v>162</v>
+      <c r="C117" s="52" t="s">
+        <v>161</v>
       </c>
       <c r="D117" s="29"/>
       <c r="E117" s="13"/>
@@ -12049,11 +12117,11 @@
       <c r="HB117" s="28"/>
       <c r="HC117" s="28"/>
     </row>
-    <row r="118" spans="1:211" ht="18.95" customHeight="1">
+    <row r="118" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="25"/>
       <c r="B118" s="26"/>
-      <c r="C118" s="53" t="s">
-        <v>158</v>
+      <c r="C118" s="52" t="s">
+        <v>157</v>
       </c>
       <c r="D118" s="29"/>
       <c r="E118" s="13"/>
@@ -12126,11 +12194,11 @@
       <c r="HB118" s="28"/>
       <c r="HC118" s="28"/>
     </row>
-    <row r="119" spans="1:211" ht="18.95" customHeight="1">
+    <row r="119" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="25"/>
       <c r="B119" s="26"/>
-      <c r="C119" s="53" t="s">
-        <v>157</v>
+      <c r="C119" s="52" t="s">
+        <v>156</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="13"/>
@@ -12203,11 +12271,11 @@
       <c r="HB119" s="28"/>
       <c r="HC119" s="28"/>
     </row>
-    <row r="120" spans="1:211" ht="18.95" customHeight="1">
+    <row r="120" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="25"/>
       <c r="B120" s="26"/>
-      <c r="C120" s="53" t="s">
-        <v>160</v>
+      <c r="C120" s="52" t="s">
+        <v>159</v>
       </c>
       <c r="D120" s="29">
         <v>116</v>
@@ -12284,11 +12352,11 @@
       <c r="HB120" s="28"/>
       <c r="HC120" s="28"/>
     </row>
-    <row r="121" spans="1:211" ht="18.95" customHeight="1">
+    <row r="121" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="25"/>
       <c r="B121" s="26"/>
-      <c r="C121" s="53" t="s">
-        <v>176</v>
+      <c r="C121" s="52" t="s">
+        <v>173</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="13"/>
@@ -12361,11 +12429,11 @@
       <c r="HB121" s="28"/>
       <c r="HC121" s="28"/>
     </row>
-    <row r="122" spans="1:211" ht="18.95" customHeight="1">
+    <row r="122" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="25"/>
       <c r="B122" s="26"/>
-      <c r="C122" s="53" t="s">
-        <v>177</v>
+      <c r="C122" s="52" t="s">
+        <v>174</v>
       </c>
       <c r="D122" s="29"/>
       <c r="E122" s="13"/>
@@ -12438,10 +12506,10 @@
       <c r="HB122" s="28"/>
       <c r="HC122" s="28"/>
     </row>
-    <row r="123" spans="1:211" ht="18.95" customHeight="1">
+    <row r="123" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="25"/>
       <c r="B123" s="26"/>
-      <c r="C123" s="53"/>
+      <c r="C123" s="52"/>
       <c r="D123" s="29"/>
       <c r="E123" s="13"/>
       <c r="F123" s="13"/>
@@ -12507,10 +12575,10 @@
       <c r="HB123" s="28"/>
       <c r="HC123" s="28"/>
     </row>
-    <row r="124" spans="1:211" ht="18.95" customHeight="1">
+    <row r="124" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="25"/>
       <c r="B124" s="26"/>
-      <c r="C124" s="53"/>
+      <c r="C124" s="52"/>
       <c r="D124" s="29"/>
       <c r="E124" s="13"/>
       <c r="F124" s="13"/>
@@ -12576,12 +12644,12 @@
       <c r="HB124" s="28"/>
       <c r="HC124" s="28"/>
     </row>
-    <row r="125" spans="1:211" ht="18.95" customHeight="1">
-      <c r="A125" s="55" t="s">
+    <row r="125" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="B125" s="55"/>
-      <c r="C125" s="55"/>
+      <c r="B125" s="53"/>
+      <c r="C125" s="53"/>
       <c r="D125" s="29"/>
       <c r="E125" s="13"/>
       <c r="F125" s="13"/>
@@ -12647,13 +12715,13 @@
       <c r="HB125" s="28"/>
       <c r="HC125" s="28"/>
     </row>
-    <row r="126" spans="1:211" ht="18.95" customHeight="1">
+    <row r="126" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="25"/>
       <c r="B126" s="26">
         <v>5</v>
       </c>
-      <c r="C126" s="47" t="s">
-        <v>153</v>
+      <c r="C126" s="55" t="s">
+        <v>152</v>
       </c>
       <c r="D126" s="29"/>
       <c r="E126" s="13"/>
@@ -12720,13 +12788,13 @@
       <c r="HB126" s="28"/>
       <c r="HC126" s="28"/>
     </row>
-    <row r="127" spans="1:211" ht="18.95" customHeight="1">
+    <row r="127" spans="1:211" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="25"/>
       <c r="B127" s="26">
         <v>5</v>
       </c>
-      <c r="C127" s="47" t="s">
-        <v>155</v>
+      <c r="C127" s="55" t="s">
+        <v>154</v>
       </c>
       <c r="D127" s="29"/>
       <c r="E127" s="13"/>
@@ -12793,13 +12861,13 @@
       <c r="HB127" s="28"/>
       <c r="HC127" s="28"/>
     </row>
-    <row r="128" spans="1:211" ht="18.95" customHeight="1">
+    <row r="128" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="25"/>
       <c r="B128" s="26">
         <v>5</v>
       </c>
-      <c r="C128" s="47" t="s">
-        <v>163</v>
+      <c r="C128" s="55" t="s">
+        <v>165</v>
       </c>
       <c r="D128" s="29"/>
       <c r="E128" s="13"/>
@@ -12866,13 +12934,13 @@
       <c r="HB128" s="28"/>
       <c r="HC128" s="28"/>
     </row>
-    <row r="129" spans="1:211" ht="18.95" customHeight="1">
+    <row r="129" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="25"/>
       <c r="B129" s="26">
         <v>5</v>
       </c>
-      <c r="C129" s="47" t="s">
-        <v>167</v>
+      <c r="C129" s="55" t="s">
+        <v>181</v>
       </c>
       <c r="D129" s="29"/>
       <c r="E129" s="13"/>
@@ -12939,13 +13007,13 @@
       <c r="HB129" s="28"/>
       <c r="HC129" s="28"/>
     </row>
-    <row r="130" spans="1:211" ht="18.95" customHeight="1">
+    <row r="130" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="25"/>
       <c r="B130" s="26">
-        <v>4</v>
-      </c>
-      <c r="C130" s="47" t="s">
-        <v>164</v>
+        <v>5</v>
+      </c>
+      <c r="C130" s="55" t="s">
+        <v>177</v>
       </c>
       <c r="D130" s="29"/>
       <c r="E130" s="13"/>
@@ -13012,13 +13080,13 @@
       <c r="HB130" s="28"/>
       <c r="HC130" s="28"/>
     </row>
-    <row r="131" spans="1:211" ht="18.95" customHeight="1">
+    <row r="131" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="25"/>
       <c r="B131" s="26">
-        <v>3</v>
-      </c>
-      <c r="C131" s="47" t="s">
-        <v>142</v>
+        <v>5</v>
+      </c>
+      <c r="C131" s="55" t="s">
+        <v>200</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="13"/>
@@ -13085,13 +13153,13 @@
       <c r="HB131" s="28"/>
       <c r="HC131" s="28"/>
     </row>
-    <row r="132" spans="1:211" ht="18.95" customHeight="1">
+    <row r="132" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="25"/>
       <c r="B132" s="26">
-        <v>3</v>
-      </c>
-      <c r="C132" s="47" t="s">
-        <v>149</v>
+        <v>4</v>
+      </c>
+      <c r="C132" s="55" t="s">
+        <v>162</v>
       </c>
       <c r="D132" s="29"/>
       <c r="E132" s="13"/>
@@ -13158,23 +13226,25 @@
       <c r="HB132" s="28"/>
       <c r="HC132" s="28"/>
     </row>
-    <row r="133" spans="1:211" ht="18.95" customHeight="1">
+    <row r="133" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="25"/>
       <c r="B133" s="26">
-        <v>3</v>
-      </c>
-      <c r="C133" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="D133" s="29">
-        <v>116</v>
-      </c>
-      <c r="E133" s="13">
-        <v>1</v>
-      </c>
-      <c r="F133" s="13"/>
-      <c r="G133" s="13"/>
-      <c r="H133" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="C133" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="D133" s="29"/>
+      <c r="E133" s="13"/>
+      <c r="F133" s="13">
+        <v>171</v>
+      </c>
+      <c r="G133" s="13">
+        <v>1</v>
+      </c>
+      <c r="H133" s="5">
+        <v>1</v>
+      </c>
       <c r="N133" s="28"/>
       <c r="O133" s="28"/>
       <c r="U133" s="28"/>
@@ -13235,13 +13305,13 @@
       <c r="HB133" s="28"/>
       <c r="HC133" s="28"/>
     </row>
-    <row r="134" spans="1:211" ht="18.95" customHeight="1">
+    <row r="134" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="25"/>
       <c r="B134" s="26">
-        <v>3</v>
-      </c>
-      <c r="C134" s="47" t="s">
-        <v>152</v>
+        <v>4</v>
+      </c>
+      <c r="C134" s="55" t="s">
+        <v>182</v>
       </c>
       <c r="D134" s="29"/>
       <c r="E134" s="13"/>
@@ -13308,13 +13378,13 @@
       <c r="HB134" s="28"/>
       <c r="HC134" s="28"/>
     </row>
-    <row r="135" spans="1:211" ht="18.95" customHeight="1">
+    <row r="135" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="25"/>
       <c r="B135" s="26">
-        <v>3</v>
-      </c>
-      <c r="C135" s="47" t="s">
-        <v>150</v>
+        <v>4</v>
+      </c>
+      <c r="C135" s="55" t="s">
+        <v>187</v>
       </c>
       <c r="D135" s="29"/>
       <c r="E135" s="13"/>
@@ -13381,13 +13451,13 @@
       <c r="HB135" s="28"/>
       <c r="HC135" s="28"/>
     </row>
-    <row r="136" spans="1:211" ht="18.95" customHeight="1">
+    <row r="136" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="25"/>
       <c r="B136" s="26">
-        <v>3</v>
-      </c>
-      <c r="C136" s="54" t="s">
-        <v>136</v>
+        <v>4</v>
+      </c>
+      <c r="C136" s="55" t="s">
+        <v>190</v>
       </c>
       <c r="D136" s="29"/>
       <c r="E136" s="13"/>
@@ -13414,6 +13484,7 @@
       <c r="BS136" s="28"/>
       <c r="BY136" s="28"/>
       <c r="BZ136" s="28"/>
+      <c r="CE136" s="38"/>
       <c r="CF136" s="28"/>
       <c r="CG136" s="28"/>
       <c r="CM136" s="28"/>
@@ -13453,25 +13524,19 @@
       <c r="HB136" s="28"/>
       <c r="HC136" s="28"/>
     </row>
-    <row r="137" spans="1:211" ht="18.95" customHeight="1">
+    <row r="137" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="25"/>
       <c r="B137" s="26">
-        <v>3</v>
-      </c>
-      <c r="C137" s="47" t="s">
-        <v>171</v>
+        <v>4</v>
+      </c>
+      <c r="C137" s="55" t="s">
+        <v>191</v>
       </c>
       <c r="D137" s="29"/>
       <c r="E137" s="13"/>
-      <c r="F137" s="13">
-        <v>171</v>
-      </c>
-      <c r="G137" s="13">
-        <v>1</v>
-      </c>
-      <c r="H137" s="5">
-        <v>1</v>
-      </c>
+      <c r="F137" s="13"/>
+      <c r="G137" s="13"/>
+      <c r="H137" s="5"/>
       <c r="N137" s="28"/>
       <c r="O137" s="28"/>
       <c r="U137" s="28"/>
@@ -13532,13 +13597,13 @@
       <c r="HB137" s="28"/>
       <c r="HC137" s="28"/>
     </row>
-    <row r="138" spans="1:211" ht="18.95" customHeight="1">
+    <row r="138" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="25"/>
       <c r="B138" s="26">
         <v>3</v>
       </c>
-      <c r="C138" s="47" t="s">
-        <v>172</v>
+      <c r="C138" s="55" t="s">
+        <v>151</v>
       </c>
       <c r="D138" s="29"/>
       <c r="E138" s="13"/>
@@ -13605,13 +13670,13 @@
       <c r="HB138" s="28"/>
       <c r="HC138" s="28"/>
     </row>
-    <row r="139" spans="1:211" ht="18.95" customHeight="1">
+    <row r="139" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="25"/>
       <c r="B139" s="26">
         <v>3</v>
       </c>
-      <c r="C139" s="47" t="s">
-        <v>173</v>
+      <c r="C139" s="55" t="s">
+        <v>196</v>
       </c>
       <c r="D139" s="29"/>
       <c r="E139" s="13"/>
@@ -13678,12 +13743,12 @@
       <c r="HB139" s="28"/>
       <c r="HC139" s="28"/>
     </row>
-    <row r="140" spans="1:211" ht="18.95" customHeight="1">
+    <row r="140" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="25"/>
       <c r="B140" s="26">
         <v>3</v>
       </c>
-      <c r="C140" s="47" t="s">
+      <c r="C140" s="55" t="s">
         <v>169</v>
       </c>
       <c r="D140" s="29"/>
@@ -13751,13 +13816,13 @@
       <c r="HB140" s="28"/>
       <c r="HC140" s="28"/>
     </row>
-    <row r="141" spans="1:211" ht="18.95" customHeight="1">
+    <row r="141" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="25"/>
       <c r="B141" s="26">
-        <v>2</v>
-      </c>
-      <c r="C141" s="47" t="s">
-        <v>174</v>
+        <v>3</v>
+      </c>
+      <c r="C141" s="55" t="s">
+        <v>171</v>
       </c>
       <c r="D141" s="29"/>
       <c r="E141" s="13"/>
@@ -13824,13 +13889,13 @@
       <c r="HB141" s="28"/>
       <c r="HC141" s="28"/>
     </row>
-    <row r="142" spans="1:211" ht="18.95" customHeight="1">
+    <row r="142" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="25"/>
       <c r="B142" s="26">
-        <v>2</v>
-      </c>
-      <c r="C142" s="47" t="s">
-        <v>148</v>
+        <v>3</v>
+      </c>
+      <c r="C142" s="55" t="s">
+        <v>175</v>
       </c>
       <c r="D142" s="29"/>
       <c r="E142" s="13"/>
@@ -13897,13 +13962,13 @@
       <c r="HB142" s="28"/>
       <c r="HC142" s="28"/>
     </row>
-    <row r="143" spans="1:211" ht="18.95" customHeight="1">
+    <row r="143" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="25"/>
       <c r="B143" s="26">
-        <v>2</v>
-      </c>
-      <c r="C143" s="47" t="s">
-        <v>170</v>
+        <v>3</v>
+      </c>
+      <c r="C143" s="55" t="s">
+        <v>176</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="13"/>
@@ -13970,13 +14035,13 @@
       <c r="HB143" s="28"/>
       <c r="HC143" s="28"/>
     </row>
-    <row r="144" spans="1:211" ht="18.95" customHeight="1">
+    <row r="144" spans="1:211" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="25"/>
       <c r="B144" s="26">
-        <v>2</v>
-      </c>
-      <c r="C144" s="47" t="s">
-        <v>168</v>
+        <v>3</v>
+      </c>
+      <c r="C144" s="55" t="s">
+        <v>180</v>
       </c>
       <c r="D144" s="29"/>
       <c r="E144" s="13"/>
@@ -14043,22 +14108,16 @@
       <c r="HB144" s="28"/>
       <c r="HC144" s="28"/>
     </row>
-    <row r="145" spans="1:211" ht="18.95" customHeight="1">
-      <c r="A145" s="25" t="s">
-        <v>20</v>
-      </c>
+    <row r="145" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="25"/>
       <c r="B145" s="26">
-        <v>1</v>
-      </c>
-      <c r="C145" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="D145" s="29">
-        <v>112</v>
-      </c>
-      <c r="E145" s="13">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C145" s="55" t="s">
+        <v>192</v>
+      </c>
+      <c r="D145" s="29"/>
+      <c r="E145" s="13"/>
       <c r="F145" s="13"/>
       <c r="G145" s="13"/>
       <c r="H145" s="5"/>
@@ -14082,6 +14141,7 @@
       <c r="BS145" s="28"/>
       <c r="BY145" s="28"/>
       <c r="BZ145" s="28"/>
+      <c r="CE145" s="38"/>
       <c r="CF145" s="28"/>
       <c r="CG145" s="28"/>
       <c r="CM145" s="28"/>
@@ -14121,27 +14181,19 @@
       <c r="HB145" s="28"/>
       <c r="HC145" s="28"/>
     </row>
-    <row r="146" spans="1:211" ht="18.95" customHeight="1">
-      <c r="A146" s="25" t="s">
-        <v>20</v>
-      </c>
+    <row r="146" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="25"/>
       <c r="B146" s="26">
-        <v>1</v>
-      </c>
-      <c r="C146" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D146" s="29">
-        <v>113</v>
-      </c>
-      <c r="E146" s="13">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C146" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="D146" s="29"/>
+      <c r="E146" s="13"/>
       <c r="F146" s="13"/>
       <c r="G146" s="13"/>
-      <c r="H146" s="5">
-        <v>0.5</v>
-      </c>
+      <c r="H146" s="5"/>
       <c r="N146" s="28"/>
       <c r="O146" s="28"/>
       <c r="U146" s="28"/>
@@ -14162,6 +14214,7 @@
       <c r="BS146" s="28"/>
       <c r="BY146" s="28"/>
       <c r="BZ146" s="28"/>
+      <c r="CE146" s="38"/>
       <c r="CF146" s="28"/>
       <c r="CG146" s="28"/>
       <c r="CM146" s="28"/>
@@ -14201,13 +14254,13 @@
       <c r="HB146" s="28"/>
       <c r="HC146" s="28"/>
     </row>
-    <row r="147" spans="1:211" ht="18.95" customHeight="1">
+    <row r="147" spans="1:211" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="25"/>
       <c r="B147" s="26">
-        <v>1</v>
-      </c>
-      <c r="C147" s="47" t="s">
-        <v>154</v>
+        <v>3</v>
+      </c>
+      <c r="C147" s="55" t="s">
+        <v>197</v>
       </c>
       <c r="D147" s="29"/>
       <c r="E147" s="13"/>
@@ -14274,13 +14327,13 @@
       <c r="HB147" s="28"/>
       <c r="HC147" s="28"/>
     </row>
-    <row r="148" spans="1:211" ht="18.95" customHeight="1">
+    <row r="148" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="25"/>
       <c r="B148" s="26">
-        <v>1</v>
-      </c>
-      <c r="C148" s="47" t="s">
-        <v>156</v>
+        <v>2</v>
+      </c>
+      <c r="C148" s="55" t="s">
+        <v>149</v>
       </c>
       <c r="D148" s="29"/>
       <c r="E148" s="13"/>
@@ -14347,22 +14400,16 @@
       <c r="HB148" s="28"/>
       <c r="HC148" s="28"/>
     </row>
-    <row r="149" spans="1:211" ht="18.95" customHeight="1">
-      <c r="A149" s="25" t="s">
-        <v>18</v>
-      </c>
+    <row r="149" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="25"/>
       <c r="B149" s="26">
-        <v>1</v>
-      </c>
-      <c r="C149" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="D149" s="29">
-        <v>100</v>
-      </c>
-      <c r="E149" s="13">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C149" s="55" t="s">
+        <v>170</v>
+      </c>
+      <c r="D149" s="29"/>
+      <c r="E149" s="13"/>
       <c r="F149" s="13"/>
       <c r="G149" s="13"/>
       <c r="H149" s="5"/>
@@ -14386,6 +14433,7 @@
       <c r="BS149" s="28"/>
       <c r="BY149" s="28"/>
       <c r="BZ149" s="28"/>
+      <c r="CE149" s="38"/>
       <c r="CF149" s="28"/>
       <c r="CG149" s="28"/>
       <c r="CM149" s="28"/>
@@ -14425,11 +14473,13 @@
       <c r="HB149" s="28"/>
       <c r="HC149" s="28"/>
     </row>
-    <row r="150" spans="1:211" ht="18.95" customHeight="1">
+    <row r="150" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="25"/>
-      <c r="B150" s="26"/>
-      <c r="C150" s="47" t="s">
-        <v>178</v>
+      <c r="B150" s="26">
+        <v>2</v>
+      </c>
+      <c r="C150" s="55" t="s">
+        <v>166</v>
       </c>
       <c r="D150" s="29"/>
       <c r="E150" s="13"/>
@@ -14496,11 +14546,13 @@
       <c r="HB150" s="28"/>
       <c r="HC150" s="28"/>
     </row>
-    <row r="151" spans="1:211" ht="18.95" customHeight="1">
+    <row r="151" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="25"/>
-      <c r="B151" s="26"/>
-      <c r="C151" s="47" t="s">
-        <v>179</v>
+      <c r="B151" s="26">
+        <v>2</v>
+      </c>
+      <c r="C151" s="55" t="s">
+        <v>148</v>
       </c>
       <c r="D151" s="29"/>
       <c r="E151" s="13"/>
@@ -14567,11 +14619,13 @@
       <c r="HB151" s="28"/>
       <c r="HC151" s="28"/>
     </row>
-    <row r="152" spans="1:211" ht="18.95" customHeight="1">
+    <row r="152" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="25"/>
-      <c r="B152" s="26"/>
-      <c r="C152" s="47" t="s">
-        <v>184</v>
+      <c r="B152" s="26">
+        <v>2</v>
+      </c>
+      <c r="C152" s="55" t="s">
+        <v>167</v>
       </c>
       <c r="D152" s="29"/>
       <c r="E152" s="13"/>
@@ -14638,11 +14692,13 @@
       <c r="HB152" s="28"/>
       <c r="HC152" s="28"/>
     </row>
-    <row r="153" spans="1:211" ht="18.95" customHeight="1">
+    <row r="153" spans="1:211" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="25"/>
-      <c r="B153" s="26"/>
-      <c r="C153" s="47" t="s">
-        <v>180</v>
+      <c r="B153" s="26">
+        <v>2</v>
+      </c>
+      <c r="C153" s="55" t="s">
+        <v>201</v>
       </c>
       <c r="D153" s="29"/>
       <c r="E153" s="13"/>
@@ -14709,11 +14765,13 @@
       <c r="HB153" s="28"/>
       <c r="HC153" s="28"/>
     </row>
-    <row r="154" spans="1:211" ht="18.95" customHeight="1">
+    <row r="154" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="25"/>
-      <c r="B154" s="26"/>
-      <c r="C154" s="47" t="s">
-        <v>181</v>
+      <c r="B154" s="26">
+        <v>2</v>
+      </c>
+      <c r="C154" s="55" t="s">
+        <v>178</v>
       </c>
       <c r="D154" s="29"/>
       <c r="E154" s="13"/>
@@ -14780,11 +14838,13 @@
       <c r="HB154" s="28"/>
       <c r="HC154" s="28"/>
     </row>
-    <row r="155" spans="1:211" ht="18.95" customHeight="1">
+    <row r="155" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="25"/>
-      <c r="B155" s="26"/>
-      <c r="C155" s="47" t="s">
-        <v>182</v>
+      <c r="B155" s="26">
+        <v>2</v>
+      </c>
+      <c r="C155" s="55" t="s">
+        <v>179</v>
       </c>
       <c r="D155" s="29"/>
       <c r="E155" s="13"/>
@@ -14851,11 +14911,13 @@
       <c r="HB155" s="28"/>
       <c r="HC155" s="28"/>
     </row>
-    <row r="156" spans="1:211" ht="18.95" customHeight="1">
+    <row r="156" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="25"/>
-      <c r="B156" s="26"/>
-      <c r="C156" s="47" t="s">
-        <v>183</v>
+      <c r="B156" s="26">
+        <v>1</v>
+      </c>
+      <c r="C156" s="55" t="s">
+        <v>142</v>
       </c>
       <c r="D156" s="29"/>
       <c r="E156" s="13"/>
@@ -14922,14 +14984,20 @@
       <c r="HB156" s="28"/>
       <c r="HC156" s="28"/>
     </row>
-    <row r="157" spans="1:211" ht="18.95" customHeight="1">
+    <row r="157" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="25"/>
-      <c r="B157" s="26"/>
-      <c r="C157" s="47" t="s">
-        <v>185</v>
-      </c>
-      <c r="D157" s="29"/>
-      <c r="E157" s="13"/>
+      <c r="B157" s="26">
+        <v>1</v>
+      </c>
+      <c r="C157" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="D157" s="29">
+        <v>116</v>
+      </c>
+      <c r="E157" s="13">
+        <v>1</v>
+      </c>
       <c r="F157" s="13"/>
       <c r="G157" s="13"/>
       <c r="H157" s="5"/>
@@ -14993,14 +15061,22 @@
       <c r="HB157" s="28"/>
       <c r="HC157" s="28"/>
     </row>
-    <row r="158" spans="1:211" ht="18.95" customHeight="1">
-      <c r="A158" s="25"/>
-      <c r="B158" s="26"/>
-      <c r="C158" s="47" t="s">
-        <v>190</v>
-      </c>
-      <c r="D158" s="29"/>
-      <c r="E158" s="13"/>
+    <row r="158" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B158" s="26">
+        <v>1</v>
+      </c>
+      <c r="C158" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="D158" s="29">
+        <v>112</v>
+      </c>
+      <c r="E158" s="13">
+        <v>1</v>
+      </c>
       <c r="F158" s="13"/>
       <c r="G158" s="13"/>
       <c r="H158" s="5"/>
@@ -15024,7 +15100,6 @@
       <c r="BS158" s="28"/>
       <c r="BY158" s="28"/>
       <c r="BZ158" s="28"/>
-      <c r="CE158" s="38"/>
       <c r="CF158" s="28"/>
       <c r="CG158" s="28"/>
       <c r="CM158" s="28"/>
@@ -15064,17 +15139,27 @@
       <c r="HB158" s="28"/>
       <c r="HC158" s="28"/>
     </row>
-    <row r="159" spans="1:211" ht="18.95" customHeight="1">
-      <c r="A159" s="25"/>
-      <c r="B159" s="26"/>
-      <c r="C159" s="47" t="s">
-        <v>193</v>
-      </c>
-      <c r="D159" s="29"/>
-      <c r="E159" s="13"/>
+    <row r="159" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B159" s="26">
+        <v>1</v>
+      </c>
+      <c r="C159" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="D159" s="29">
+        <v>113</v>
+      </c>
+      <c r="E159" s="13">
+        <v>4</v>
+      </c>
       <c r="F159" s="13"/>
       <c r="G159" s="13"/>
-      <c r="H159" s="5"/>
+      <c r="H159" s="5">
+        <v>0.5</v>
+      </c>
       <c r="N159" s="28"/>
       <c r="O159" s="28"/>
       <c r="U159" s="28"/>
@@ -15095,7 +15180,6 @@
       <c r="BS159" s="28"/>
       <c r="BY159" s="28"/>
       <c r="BZ159" s="28"/>
-      <c r="CE159" s="38"/>
       <c r="CF159" s="28"/>
       <c r="CG159" s="28"/>
       <c r="CM159" s="28"/>
@@ -15135,11 +15219,13 @@
       <c r="HB159" s="28"/>
       <c r="HC159" s="28"/>
     </row>
-    <row r="160" spans="1:211" ht="18.95" customHeight="1">
+    <row r="160" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="25"/>
-      <c r="B160" s="26"/>
-      <c r="C160" s="47" t="s">
-        <v>194</v>
+      <c r="B160" s="26">
+        <v>1</v>
+      </c>
+      <c r="C160" s="55" t="s">
+        <v>153</v>
       </c>
       <c r="D160" s="29"/>
       <c r="E160" s="13"/>
@@ -15206,11 +15292,13 @@
       <c r="HB160" s="28"/>
       <c r="HC160" s="28"/>
     </row>
-    <row r="161" spans="1:211" ht="18.95" customHeight="1">
+    <row r="161" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="25"/>
-      <c r="B161" s="26"/>
-      <c r="C161" s="47" t="s">
-        <v>195</v>
+      <c r="B161" s="26">
+        <v>1</v>
+      </c>
+      <c r="C161" s="55" t="s">
+        <v>155</v>
       </c>
       <c r="D161" s="29"/>
       <c r="E161" s="13"/>
@@ -15277,14 +15365,22 @@
       <c r="HB161" s="28"/>
       <c r="HC161" s="28"/>
     </row>
-    <row r="162" spans="1:211" ht="18.95" customHeight="1">
-      <c r="A162" s="25"/>
-      <c r="B162" s="26"/>
-      <c r="C162" s="47" t="s">
-        <v>196</v>
-      </c>
-      <c r="D162" s="29"/>
-      <c r="E162" s="13"/>
+    <row r="162" spans="1:211" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B162" s="26">
+        <v>1</v>
+      </c>
+      <c r="C162" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D162" s="29">
+        <v>100</v>
+      </c>
+      <c r="E162" s="13">
+        <v>1</v>
+      </c>
       <c r="F162" s="13"/>
       <c r="G162" s="13"/>
       <c r="H162" s="5"/>
@@ -15308,7 +15404,6 @@
       <c r="BS162" s="28"/>
       <c r="BY162" s="28"/>
       <c r="BZ162" s="28"/>
-      <c r="CE162" s="38"/>
       <c r="CF162" s="28"/>
       <c r="CG162" s="28"/>
       <c r="CM162" s="28"/>
@@ -15348,17 +15443,227 @@
       <c r="HB162" s="28"/>
       <c r="HC162" s="28"/>
     </row>
-    <row r="163" spans="1:211">
-      <c r="A163" s="14"/>
-      <c r="B163" s="14"/>
-      <c r="CE163" s="38"/>
-      <c r="CG163" s="38"/>
-      <c r="CI163" s="38"/>
-      <c r="CK163" s="38"/>
+    <row r="163" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="25"/>
+      <c r="B163" s="26">
+        <v>1</v>
+      </c>
+      <c r="C163" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="D163" s="29"/>
+      <c r="E163" s="13"/>
+      <c r="F163" s="13"/>
+      <c r="G163" s="13"/>
+      <c r="H163" s="5"/>
+      <c r="N163" s="28"/>
+      <c r="O163" s="28"/>
+      <c r="U163" s="28"/>
+      <c r="V163" s="28"/>
+      <c r="AB163" s="28"/>
+      <c r="AC163" s="28"/>
+      <c r="AI163" s="28"/>
+      <c r="AJ163" s="28"/>
+      <c r="AP163" s="28"/>
+      <c r="AQ163" s="28"/>
+      <c r="AW163" s="28"/>
+      <c r="AX163" s="28"/>
+      <c r="BD163" s="28"/>
+      <c r="BE163" s="28"/>
+      <c r="BK163" s="28"/>
+      <c r="BL163" s="28"/>
+      <c r="BR163" s="28"/>
+      <c r="BS163" s="28"/>
+      <c r="BY163" s="28"/>
+      <c r="BZ163" s="28"/>
+      <c r="CF163" s="28"/>
+      <c r="CG163" s="28"/>
+      <c r="CM163" s="28"/>
+      <c r="CN163" s="28"/>
+      <c r="CT163" s="28"/>
+      <c r="CU163" s="28"/>
+      <c r="DA163" s="28"/>
+      <c r="DB163" s="28"/>
+      <c r="DH163" s="28"/>
+      <c r="DI163" s="28"/>
+      <c r="DO163" s="28"/>
+      <c r="DP163" s="28"/>
+      <c r="DV163" s="28"/>
+      <c r="DW163" s="28"/>
+      <c r="EC163" s="28"/>
+      <c r="ED163" s="28"/>
+      <c r="EJ163" s="28"/>
+      <c r="EK163" s="28"/>
+      <c r="EQ163" s="28"/>
+      <c r="ER163" s="28"/>
+      <c r="EX163" s="28"/>
+      <c r="EY163" s="28"/>
+      <c r="FE163" s="28"/>
+      <c r="FF163" s="28"/>
+      <c r="FL163" s="28"/>
+      <c r="FM163" s="28"/>
+      <c r="FS163" s="28"/>
+      <c r="FT163" s="28"/>
+      <c r="FZ163" s="28"/>
+      <c r="GA163" s="28"/>
+      <c r="GG163" s="28"/>
+      <c r="GH163" s="28"/>
+      <c r="GN163" s="28"/>
+      <c r="GO163" s="28"/>
+      <c r="GU163" s="28"/>
+      <c r="GV163" s="28"/>
+      <c r="HB163" s="28"/>
+      <c r="HC163" s="28"/>
+    </row>
+    <row r="164" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="25"/>
+      <c r="B164" s="26"/>
+      <c r="C164" s="55"/>
+      <c r="D164" s="29"/>
+      <c r="E164" s="13"/>
+      <c r="F164" s="13"/>
+      <c r="G164" s="13"/>
+      <c r="H164" s="5"/>
+      <c r="N164" s="28"/>
+      <c r="O164" s="28"/>
+      <c r="U164" s="28"/>
+      <c r="V164" s="28"/>
+      <c r="AB164" s="28"/>
+      <c r="AC164" s="28"/>
+      <c r="AI164" s="28"/>
+      <c r="AJ164" s="28"/>
+      <c r="AP164" s="28"/>
+      <c r="AQ164" s="28"/>
+      <c r="AW164" s="28"/>
+      <c r="AX164" s="28"/>
+      <c r="BD164" s="28"/>
+      <c r="BE164" s="28"/>
+      <c r="BK164" s="28"/>
+      <c r="BL164" s="28"/>
+      <c r="BR164" s="28"/>
+      <c r="BS164" s="28"/>
+      <c r="BY164" s="28"/>
+      <c r="BZ164" s="28"/>
+      <c r="CE164" s="38"/>
+      <c r="CF164" s="28"/>
+      <c r="CG164" s="28"/>
+      <c r="CM164" s="28"/>
+      <c r="CN164" s="28"/>
+      <c r="CT164" s="28"/>
+      <c r="CU164" s="28"/>
+      <c r="DA164" s="28"/>
+      <c r="DB164" s="28"/>
+      <c r="DH164" s="28"/>
+      <c r="DI164" s="28"/>
+      <c r="DO164" s="28"/>
+      <c r="DP164" s="28"/>
+      <c r="DV164" s="28"/>
+      <c r="DW164" s="28"/>
+      <c r="EC164" s="28"/>
+      <c r="ED164" s="28"/>
+      <c r="EJ164" s="28"/>
+      <c r="EK164" s="28"/>
+      <c r="EQ164" s="28"/>
+      <c r="ER164" s="28"/>
+      <c r="EX164" s="28"/>
+      <c r="EY164" s="28"/>
+      <c r="FE164" s="28"/>
+      <c r="FF164" s="28"/>
+      <c r="FL164" s="28"/>
+      <c r="FM164" s="28"/>
+      <c r="FS164" s="28"/>
+      <c r="FT164" s="28"/>
+      <c r="FZ164" s="28"/>
+      <c r="GA164" s="28"/>
+      <c r="GG164" s="28"/>
+      <c r="GH164" s="28"/>
+      <c r="GN164" s="28"/>
+      <c r="GO164" s="28"/>
+      <c r="GU164" s="28"/>
+      <c r="GV164" s="28"/>
+      <c r="HB164" s="28"/>
+      <c r="HC164" s="28"/>
+    </row>
+    <row r="165" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="25"/>
+      <c r="B165" s="26"/>
+      <c r="C165" s="55"/>
+      <c r="D165" s="29"/>
+      <c r="E165" s="13"/>
+      <c r="F165" s="13"/>
+      <c r="G165" s="13"/>
+      <c r="H165" s="5"/>
+      <c r="N165" s="28"/>
+      <c r="O165" s="28"/>
+      <c r="U165" s="28"/>
+      <c r="V165" s="28"/>
+      <c r="AB165" s="28"/>
+      <c r="AC165" s="28"/>
+      <c r="AI165" s="28"/>
+      <c r="AJ165" s="28"/>
+      <c r="AP165" s="28"/>
+      <c r="AQ165" s="28"/>
+      <c r="AW165" s="28"/>
+      <c r="AX165" s="28"/>
+      <c r="BD165" s="28"/>
+      <c r="BE165" s="28"/>
+      <c r="BK165" s="28"/>
+      <c r="BL165" s="28"/>
+      <c r="BR165" s="28"/>
+      <c r="BS165" s="28"/>
+      <c r="BY165" s="28"/>
+      <c r="BZ165" s="28"/>
+      <c r="CE165" s="38"/>
+      <c r="CF165" s="28"/>
+      <c r="CG165" s="28"/>
+      <c r="CM165" s="28"/>
+      <c r="CN165" s="28"/>
+      <c r="CT165" s="28"/>
+      <c r="CU165" s="28"/>
+      <c r="DA165" s="28"/>
+      <c r="DB165" s="28"/>
+      <c r="DH165" s="28"/>
+      <c r="DI165" s="28"/>
+      <c r="DO165" s="28"/>
+      <c r="DP165" s="28"/>
+      <c r="DV165" s="28"/>
+      <c r="DW165" s="28"/>
+      <c r="EC165" s="28"/>
+      <c r="ED165" s="28"/>
+      <c r="EJ165" s="28"/>
+      <c r="EK165" s="28"/>
+      <c r="EQ165" s="28"/>
+      <c r="ER165" s="28"/>
+      <c r="EX165" s="28"/>
+      <c r="EY165" s="28"/>
+      <c r="FE165" s="28"/>
+      <c r="FF165" s="28"/>
+      <c r="FL165" s="28"/>
+      <c r="FM165" s="28"/>
+      <c r="FS165" s="28"/>
+      <c r="FT165" s="28"/>
+      <c r="FZ165" s="28"/>
+      <c r="GA165" s="28"/>
+      <c r="GG165" s="28"/>
+      <c r="GH165" s="28"/>
+      <c r="GN165" s="28"/>
+      <c r="GO165" s="28"/>
+      <c r="GU165" s="28"/>
+      <c r="GV165" s="28"/>
+      <c r="HB165" s="28"/>
+      <c r="HC165" s="28"/>
+    </row>
+    <row r="166" spans="1:211" x14ac:dyDescent="0.25">
+      <c r="A166" s="14"/>
+      <c r="B166" s="14"/>
+      <c r="CE166" s="38"/>
+      <c r="CG166" s="38"/>
+      <c r="CI166" s="38"/>
+      <c r="CK166" s="38"/>
     </row>
   </sheetData>
-  <sortState ref="A125:GL149">
-    <sortCondition descending="1" ref="B125:B149"/>
+  <sortState ref="A126:HC165">
+    <sortCondition descending="1" ref="B126:B165"/>
   </sortState>
   <mergeCells count="4">
     <mergeCell ref="A70:C70"/>
@@ -15366,84 +15671,113 @@
     <mergeCell ref="A86:C86"/>
     <mergeCell ref="A125:C125"/>
   </mergeCells>
-  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU162 DJ8:DN162 DC8:DG162 EE8:EI162 CA8:CE162 AY8:BC162 AR8:AV162 AK8:AO162 AD8:AH162 BF66:BJ162 BM66:BQ162 BT66:BX162 W78:AA162 P60:T162 CV60:CZ162 CO69:CS162 DX114:EB162 CH60:CL162 EL8:EP162 ES8:EW162 EZ8:FD162 FG8:FK162 FN8:FR162 FU8:FY162 GB8:GF162 GI8:GM162 GP8:GT162 GW8:HA162 J69:M162">
-    <cfRule type="expression" dxfId="24" priority="92">
+  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU165 DJ8:DN165 DC8:DG165 EE8:EI165 CA8:CE165 AY8:BC165 AR8:AV165 AK8:AO165 AD8:AH165 BF66:BJ165 BM66:BQ165 BT66:BX165 W78:AA165 P60:T165 CV60:CZ165 CO69:CS165 DX114:EB165 CH60:CL165 EL8:EP165 ES8:EW165 EZ8:FD165 FG8:FK165 FN8:FR165 FU8:FY165 GB8:GF165 GI8:GM165 GP8:GT165 GW8:HA165 J69:M165">
+    <cfRule type="expression" dxfId="17" priority="92">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="93">
+    <cfRule type="expression" dxfId="16" priority="93">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="94">
+    <cfRule type="expression" dxfId="15" priority="94">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="95">
+    <cfRule type="expression" dxfId="14" priority="95">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="96">
+    <cfRule type="expression" dxfId="13" priority="96">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="97">
+    <cfRule type="expression" dxfId="12" priority="97">
       <formula>J$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="98">
+    <cfRule type="expression" dxfId="11" priority="98">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="99">
+    <cfRule type="expression" dxfId="10" priority="99">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A163:HC163">
-    <cfRule type="expression" dxfId="16" priority="91">
+  <conditionalFormatting sqref="A166:HC166">
+    <cfRule type="expression" dxfId="9" priority="91">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:HC7">
-    <cfRule type="expression" dxfId="15" priority="90">
+    <cfRule type="expression" dxfId="8" priority="90">
       <formula>J$7=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL56:CL57">
-    <cfRule type="expression" dxfId="14" priority="81">
+    <cfRule type="expression" dxfId="7" priority="81">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="82">
+    <cfRule type="expression" dxfId="6" priority="82">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="83">
+    <cfRule type="expression" dxfId="5" priority="83">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="84">
+    <cfRule type="expression" dxfId="4" priority="84">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="85">
+    <cfRule type="expression" dxfId="3" priority="85">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="86">
+    <cfRule type="expression" dxfId="2" priority="86">
       <formula>CL$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="87">
+    <cfRule type="expression" dxfId="1" priority="87">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="88">
+    <cfRule type="expression" dxfId="0" priority="88">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2049" r:id="rId4" name="Spinner 1">
+              <controlPr defaultSize="0" print="0" autoPict="0" altText="Period Highlight Spin Control">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>152400</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>247650</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AO238"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.625" style="36" customWidth="1"/>
     <col min="2" max="2" width="11.375" style="33" customWidth="1"/>
@@ -15456,12 +15790,12 @@
     <col min="42" max="16384" width="9" style="36"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:41" ht="33.75">
+    <row r="2" spans="1:41" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:41" s="34" customFormat="1">
+    <row r="4" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>61</v>
       </c>
@@ -15484,7 +15818,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="36">
         <v>1</v>
       </c>
@@ -15507,7 +15841,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="36">
         <v>2</v>
       </c>
@@ -15515,16 +15849,16 @@
         <v>41690</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AO6" s="35" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="36">
         <v>3</v>
       </c>
@@ -15532,22 +15866,22 @@
         <v>41705</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E7" s="34" t="s">
         <v>56</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AO7" s="35" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="36">
         <v>4</v>
       </c>
@@ -15555,19 +15889,19 @@
         <v>41705</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E8" s="34" t="s">
         <v>58</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:41">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="36">
         <v>5</v>
       </c>
@@ -15575,19 +15909,19 @@
         <v>41724</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E9" s="34" t="s">
         <v>56</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:41">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="36">
         <v>6</v>
       </c>
@@ -15595,1151 +15929,1166 @@
         <v>41738</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E10" s="34" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="36">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:41">
+      <c r="B11" s="33">
+        <v>41751</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="36">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="36">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:41">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="36">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:41">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="36">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:41">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="36">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="36">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="36">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="36">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="36">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="36">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="36">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="36">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="36">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="36">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="36">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="36">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="36">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="36">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="36">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="36">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="36">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="36">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="36">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="36">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="36">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="36">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="36">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="36">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="36">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="36">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="36">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="36">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="36">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="36">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="36">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="36">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="36">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="36">
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="36">
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="36">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="36">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="36">
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="36">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="36">
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="36">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="36">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="36">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="36">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="36">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="36">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="36">
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="36">
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="36">
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="36">
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="36">
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="36">
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="36">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="36">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="36">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="36">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="36">
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="36">
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="36">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="36">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="36">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="36">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="36">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="36">
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="36">
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="36">
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="36">
         <v>78</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="36">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="36">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="36">
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="36">
         <v>82</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="36">
         <v>83</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="36">
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="36">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="36">
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="36">
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="36">
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="36">
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="36">
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="36">
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="36">
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="36">
         <v>93</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="36">
         <v>94</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="36">
         <v>95</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="36">
         <v>96</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="36">
         <v>97</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="36">
         <v>98</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="36">
         <v>99</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="36">
         <v>100</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="36">
         <v>101</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="36">
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="36">
         <v>103</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="36">
         <v>104</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="36">
         <v>105</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="36">
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="36">
         <v>107</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="36">
         <v>108</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="36">
         <v>109</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="36">
         <v>110</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="36">
         <v>111</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="36">
         <v>112</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="36">
         <v>113</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="36">
         <v>114</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="36">
         <v>115</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="36">
         <v>116</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="36">
         <v>117</v>
       </c>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="36">
         <v>118</v>
       </c>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="36">
         <v>119</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="36">
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="36">
         <v>121</v>
       </c>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="36">
         <v>122</v>
       </c>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="36">
         <v>123</v>
       </c>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="36">
         <v>124</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="36">
         <v>125</v>
       </c>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="36">
         <v>126</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="36">
         <v>127</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="36">
         <v>128</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="36">
         <v>129</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="36">
         <v>130</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="36">
         <v>131</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="36">
         <v>132</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="36">
         <v>133</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="36">
         <v>134</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="36">
         <v>135</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="36">
         <v>136</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="36">
         <v>137</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="36">
         <v>138</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="36">
         <v>139</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="36">
         <v>140</v>
       </c>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="36">
         <v>141</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="36">
         <v>142</v>
       </c>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="36">
         <v>143</v>
       </c>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="36">
         <v>144</v>
       </c>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="36">
         <v>145</v>
       </c>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="36">
         <v>146</v>
       </c>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="36">
         <v>147</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="36">
         <v>148</v>
       </c>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="36">
         <v>149</v>
       </c>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="36">
         <v>150</v>
       </c>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="36">
         <v>151</v>
       </c>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="36">
         <v>152</v>
       </c>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="36">
         <v>153</v>
       </c>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="36">
         <v>154</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="36">
         <v>155</v>
       </c>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="36">
         <v>156</v>
       </c>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="36">
         <v>157</v>
       </c>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="36">
         <v>158</v>
       </c>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="36">
         <v>159</v>
       </c>
     </row>
-    <row r="164" spans="1:1">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="36">
         <v>160</v>
       </c>
     </row>
-    <row r="165" spans="1:1">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="36">
         <v>161</v>
       </c>
     </row>
-    <row r="166" spans="1:1">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="36">
         <v>162</v>
       </c>
     </row>
-    <row r="167" spans="1:1">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="36">
         <v>163</v>
       </c>
     </row>
-    <row r="168" spans="1:1">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="36">
         <v>164</v>
       </c>
     </row>
-    <row r="169" spans="1:1">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="36">
         <v>165</v>
       </c>
     </row>
-    <row r="170" spans="1:1">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="36">
         <v>166</v>
       </c>
     </row>
-    <row r="171" spans="1:1">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="36">
         <v>167</v>
       </c>
     </row>
-    <row r="172" spans="1:1">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="36">
         <v>168</v>
       </c>
     </row>
-    <row r="173" spans="1:1">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="36">
         <v>169</v>
       </c>
     </row>
-    <row r="174" spans="1:1">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="36">
         <v>170</v>
       </c>
     </row>
-    <row r="175" spans="1:1">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="36">
         <v>171</v>
       </c>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="36">
         <v>172</v>
       </c>
     </row>
-    <row r="177" spans="1:1">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="36">
         <v>173</v>
       </c>
     </row>
-    <row r="178" spans="1:1">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="36">
         <v>174</v>
       </c>
     </row>
-    <row r="179" spans="1:1">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="36">
         <v>175</v>
       </c>
     </row>
-    <row r="180" spans="1:1">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="36">
         <v>176</v>
       </c>
     </row>
-    <row r="181" spans="1:1">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="36">
         <v>177</v>
       </c>
     </row>
-    <row r="182" spans="1:1">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="36">
         <v>178</v>
       </c>
     </row>
-    <row r="183" spans="1:1">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="36">
         <v>179</v>
       </c>
     </row>
-    <row r="184" spans="1:1">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="36">
         <v>180</v>
       </c>
     </row>
-    <row r="185" spans="1:1">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="36">
         <v>181</v>
       </c>
     </row>
-    <row r="186" spans="1:1">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="36">
         <v>182</v>
       </c>
     </row>
-    <row r="187" spans="1:1">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="36">
         <v>183</v>
       </c>
     </row>
-    <row r="188" spans="1:1">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="36">
         <v>184</v>
       </c>
     </row>
-    <row r="189" spans="1:1">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="36">
         <v>185</v>
       </c>
     </row>
-    <row r="190" spans="1:1">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="36">
         <v>186</v>
       </c>
     </row>
-    <row r="191" spans="1:1">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="36">
         <v>187</v>
       </c>
     </row>
-    <row r="192" spans="1:1">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="36">
         <v>188</v>
       </c>
     </row>
-    <row r="193" spans="1:1">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="36">
         <v>189</v>
       </c>
     </row>
-    <row r="194" spans="1:1">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="36">
         <v>190</v>
       </c>
     </row>
-    <row r="195" spans="1:1">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="36">
         <v>191</v>
       </c>
     </row>
-    <row r="196" spans="1:1">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="36">
         <v>192</v>
       </c>
     </row>
-    <row r="197" spans="1:1">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="36">
         <v>193</v>
       </c>
     </row>
-    <row r="198" spans="1:1">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="36">
         <v>194</v>
       </c>
     </row>
-    <row r="199" spans="1:1">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="36">
         <v>195</v>
       </c>
     </row>
-    <row r="200" spans="1:1">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="36">
         <v>196</v>
       </c>
     </row>
-    <row r="201" spans="1:1">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="36">
         <v>197</v>
       </c>
     </row>
-    <row r="202" spans="1:1">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="36">
         <v>198</v>
       </c>
     </row>
-    <row r="203" spans="1:1">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="36">
         <v>199</v>
       </c>
     </row>
-    <row r="204" spans="1:1">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="36">
         <v>200</v>
       </c>
     </row>
-    <row r="205" spans="1:1">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="36">
         <v>201</v>
       </c>
     </row>
-    <row r="206" spans="1:1">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="36">
         <v>202</v>
       </c>
     </row>
-    <row r="207" spans="1:1">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="36">
         <v>203</v>
       </c>
     </row>
-    <row r="208" spans="1:1">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="36">
         <v>204</v>
       </c>
     </row>
-    <row r="209" spans="1:1">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="36">
         <v>205</v>
       </c>
     </row>
-    <row r="210" spans="1:1">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="36">
         <v>206</v>
       </c>
     </row>
-    <row r="211" spans="1:1">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="36">
         <v>207</v>
       </c>
     </row>
-    <row r="212" spans="1:1">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="36">
         <v>208</v>
       </c>
     </row>
-    <row r="213" spans="1:1">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="36">
         <v>209</v>
       </c>
     </row>
-    <row r="214" spans="1:1">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="36">
         <v>210</v>
       </c>
     </row>
-    <row r="215" spans="1:1">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="36">
         <v>211</v>
       </c>
     </row>
-    <row r="216" spans="1:1">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" s="36">
         <v>212</v>
       </c>
     </row>
-    <row r="217" spans="1:1">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A217" s="36">
         <v>213</v>
       </c>
     </row>
-    <row r="218" spans="1:1">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A218" s="36">
         <v>214</v>
       </c>
     </row>
-    <row r="219" spans="1:1">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A219" s="36">
         <v>215</v>
       </c>
     </row>
-    <row r="220" spans="1:1">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A220" s="36">
         <v>216</v>
       </c>
     </row>
-    <row r="221" spans="1:1">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="36">
         <v>217</v>
       </c>
     </row>
-    <row r="222" spans="1:1">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A222" s="36">
         <v>218</v>
       </c>
     </row>
-    <row r="223" spans="1:1">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A223" s="36">
         <v>219</v>
       </c>
     </row>
-    <row r="224" spans="1:1">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A224" s="36">
         <v>220</v>
       </c>
     </row>
-    <row r="225" spans="1:1">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A225" s="36">
         <v>221</v>
       </c>
     </row>
-    <row r="226" spans="1:1">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A226" s="36">
         <v>222</v>
       </c>
     </row>
-    <row r="227" spans="1:1">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A227" s="36">
         <v>223</v>
       </c>
     </row>
-    <row r="228" spans="1:1">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="36">
         <v>224</v>
       </c>
     </row>
-    <row r="229" spans="1:1">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A229" s="36">
         <v>225</v>
       </c>
     </row>
-    <row r="230" spans="1:1">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A230" s="36">
         <v>226</v>
       </c>
     </row>
-    <row r="231" spans="1:1">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="36">
         <v>227</v>
       </c>
     </row>
-    <row r="232" spans="1:1">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A232" s="36">
         <v>228</v>
       </c>
     </row>
-    <row r="233" spans="1:1">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A233" s="36">
         <v>229</v>
       </c>
     </row>
-    <row r="234" spans="1:1">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A234" s="36">
         <v>230</v>
       </c>
     </row>
-    <row r="235" spans="1:1">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A235" s="36">
         <v>231</v>
       </c>
     </row>
-    <row r="236" spans="1:1">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A236" s="36">
         <v>232</v>
       </c>
     </row>
-    <row r="237" spans="1:1">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="36">
         <v>233</v>
       </c>
     </row>
-    <row r="238" spans="1:1">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A238" s="36">
         <v>234</v>
       </c>

</xml_diff>

<commit_message>
Saving on RFQEAV when creating new RFQs.
</commit_message>
<xml_diff>
--- a/AQPM Gantt.xlsx
+++ b/AQPM Gantt.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Issues" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'APQM Gantt'!$A$7:$EK$129</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'APQM Gantt'!$A$7:$EK$130</definedName>
     <definedName name="Actual" localSheetId="0">('APQM Gantt'!PeriodInActual*('APQM Gantt'!$F1&gt;0))*'APQM Gantt'!PeriodInPlan</definedName>
     <definedName name="Actual">(PeriodInActual*(#REF!&gt;0))*PeriodInPlan</definedName>
     <definedName name="ActualBeyond" localSheetId="0">'APQM Gantt'!PeriodInActual*('APQM Gantt'!$F1&gt;0)</definedName>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="202">
   <si>
     <t>Plan</t>
   </si>
@@ -1279,17 +1279,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1302,7 +1302,233 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="41">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1759,15 +1985,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="40">
   <autoFilter ref="A4:F238"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="23"/>
-    <tableColumn id="2" name="Date" dataDxfId="22"/>
-    <tableColumn id="3" name="Creator" dataDxfId="21"/>
-    <tableColumn id="4" name="Issue" dataDxfId="20"/>
-    <tableColumn id="5" name="Status" dataDxfId="19"/>
-    <tableColumn id="6" name="Solution" dataDxfId="18"/>
+    <tableColumn id="1" name="#" dataDxfId="39"/>
+    <tableColumn id="2" name="Date" dataDxfId="38"/>
+    <tableColumn id="3" name="Creator" dataDxfId="37"/>
+    <tableColumn id="4" name="Issue" dataDxfId="36"/>
+    <tableColumn id="5" name="Status" dataDxfId="35"/>
+    <tableColumn id="6" name="Solution" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2003,13 +2229,13 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:HC166"/>
+  <dimension ref="A2:HC167"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="J116" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="7" topLeftCell="J122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="C145" sqref="C145"/>
+      <selection pane="bottomRight" activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
@@ -2026,11 +2252,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:211" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
@@ -2038,9 +2264,9 @@
       <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:211" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
       <c r="D3" s="19" t="s">
         <v>13</v>
       </c>
@@ -2072,9 +2298,9 @@
       </c>
     </row>
     <row r="4" spans="1:211" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
+      <c r="A4" s="56"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="44"/>
       <c r="E4" s="32"/>
       <c r="F4" s="18"/>
@@ -8349,11 +8575,11 @@
       <c r="HC69" s="28"/>
     </row>
     <row r="70" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="53" t="s">
+      <c r="A70" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="53"/>
-      <c r="C70" s="53"/>
+      <c r="B70" s="55"/>
+      <c r="C70" s="55"/>
       <c r="D70" s="29"/>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
@@ -9612,11 +9838,11 @@
       <c r="HC85" s="28"/>
     </row>
     <row r="86" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="53" t="s">
+      <c r="A86" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="B86" s="53"/>
-      <c r="C86" s="53"/>
+      <c r="B86" s="55"/>
+      <c r="C86" s="55"/>
       <c r="D86" s="29"/>
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
@@ -12645,11 +12871,11 @@
       <c r="HC124" s="28"/>
     </row>
     <row r="125" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="53" t="s">
+      <c r="A125" s="55" t="s">
         <v>147</v>
       </c>
-      <c r="B125" s="53"/>
-      <c r="C125" s="53"/>
+      <c r="B125" s="55"/>
+      <c r="C125" s="55"/>
       <c r="D125" s="29"/>
       <c r="E125" s="13"/>
       <c r="F125" s="13"/>
@@ -12720,7 +12946,7 @@
       <c r="B126" s="26">
         <v>5</v>
       </c>
-      <c r="C126" s="55" t="s">
+      <c r="C126" s="53" t="s">
         <v>152</v>
       </c>
       <c r="D126" s="29"/>
@@ -12788,13 +13014,13 @@
       <c r="HB126" s="28"/>
       <c r="HC126" s="28"/>
     </row>
-    <row r="127" spans="1:211" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="25"/>
       <c r="B127" s="26">
         <v>5</v>
       </c>
-      <c r="C127" s="55" t="s">
-        <v>154</v>
+      <c r="C127" s="53" t="s">
+        <v>152</v>
       </c>
       <c r="D127" s="29"/>
       <c r="E127" s="13"/>
@@ -12861,13 +13087,13 @@
       <c r="HB127" s="28"/>
       <c r="HC127" s="28"/>
     </row>
-    <row r="128" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:211" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="25"/>
       <c r="B128" s="26">
         <v>5</v>
       </c>
-      <c r="C128" s="55" t="s">
-        <v>165</v>
+      <c r="C128" s="53" t="s">
+        <v>154</v>
       </c>
       <c r="D128" s="29"/>
       <c r="E128" s="13"/>
@@ -12939,8 +13165,8 @@
       <c r="B129" s="26">
         <v>5</v>
       </c>
-      <c r="C129" s="55" t="s">
-        <v>181</v>
+      <c r="C129" s="53" t="s">
+        <v>165</v>
       </c>
       <c r="D129" s="29"/>
       <c r="E129" s="13"/>
@@ -13012,8 +13238,8 @@
       <c r="B130" s="26">
         <v>5</v>
       </c>
-      <c r="C130" s="55" t="s">
-        <v>177</v>
+      <c r="C130" s="53" t="s">
+        <v>181</v>
       </c>
       <c r="D130" s="29"/>
       <c r="E130" s="13"/>
@@ -13085,8 +13311,8 @@
       <c r="B131" s="26">
         <v>5</v>
       </c>
-      <c r="C131" s="55" t="s">
-        <v>200</v>
+      <c r="C131" s="53" t="s">
+        <v>177</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="13"/>
@@ -13156,10 +13382,10 @@
     <row r="132" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="25"/>
       <c r="B132" s="26">
-        <v>4</v>
-      </c>
-      <c r="C132" s="55" t="s">
-        <v>162</v>
+        <v>5</v>
+      </c>
+      <c r="C132" s="53" t="s">
+        <v>200</v>
       </c>
       <c r="D132" s="29"/>
       <c r="E132" s="13"/>
@@ -13231,20 +13457,14 @@
       <c r="B133" s="26">
         <v>4</v>
       </c>
-      <c r="C133" s="55" t="s">
-        <v>168</v>
+      <c r="C133" s="53" t="s">
+        <v>162</v>
       </c>
       <c r="D133" s="29"/>
       <c r="E133" s="13"/>
-      <c r="F133" s="13">
-        <v>171</v>
-      </c>
-      <c r="G133" s="13">
-        <v>1</v>
-      </c>
-      <c r="H133" s="5">
-        <v>1</v>
-      </c>
+      <c r="F133" s="13"/>
+      <c r="G133" s="13"/>
+      <c r="H133" s="5"/>
       <c r="N133" s="28"/>
       <c r="O133" s="28"/>
       <c r="U133" s="28"/>
@@ -13310,14 +13530,20 @@
       <c r="B134" s="26">
         <v>4</v>
       </c>
-      <c r="C134" s="55" t="s">
-        <v>182</v>
+      <c r="C134" s="53" t="s">
+        <v>168</v>
       </c>
       <c r="D134" s="29"/>
       <c r="E134" s="13"/>
-      <c r="F134" s="13"/>
-      <c r="G134" s="13"/>
-      <c r="H134" s="5"/>
+      <c r="F134" s="13">
+        <v>171</v>
+      </c>
+      <c r="G134" s="13">
+        <v>1</v>
+      </c>
+      <c r="H134" s="5">
+        <v>1</v>
+      </c>
       <c r="N134" s="28"/>
       <c r="O134" s="28"/>
       <c r="U134" s="28"/>
@@ -13383,8 +13609,8 @@
       <c r="B135" s="26">
         <v>4</v>
       </c>
-      <c r="C135" s="55" t="s">
-        <v>187</v>
+      <c r="C135" s="53" t="s">
+        <v>182</v>
       </c>
       <c r="D135" s="29"/>
       <c r="E135" s="13"/>
@@ -13456,8 +13682,8 @@
       <c r="B136" s="26">
         <v>4</v>
       </c>
-      <c r="C136" s="55" t="s">
-        <v>190</v>
+      <c r="C136" s="53" t="s">
+        <v>187</v>
       </c>
       <c r="D136" s="29"/>
       <c r="E136" s="13"/>
@@ -13529,8 +13755,8 @@
       <c r="B137" s="26">
         <v>4</v>
       </c>
-      <c r="C137" s="55" t="s">
-        <v>191</v>
+      <c r="C137" s="53" t="s">
+        <v>190</v>
       </c>
       <c r="D137" s="29"/>
       <c r="E137" s="13"/>
@@ -13600,10 +13826,10 @@
     <row r="138" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="25"/>
       <c r="B138" s="26">
-        <v>3</v>
-      </c>
-      <c r="C138" s="55" t="s">
-        <v>151</v>
+        <v>4</v>
+      </c>
+      <c r="C138" s="53" t="s">
+        <v>191</v>
       </c>
       <c r="D138" s="29"/>
       <c r="E138" s="13"/>
@@ -13675,8 +13901,8 @@
       <c r="B139" s="26">
         <v>3</v>
       </c>
-      <c r="C139" s="55" t="s">
-        <v>196</v>
+      <c r="C139" s="53" t="s">
+        <v>151</v>
       </c>
       <c r="D139" s="29"/>
       <c r="E139" s="13"/>
@@ -13748,8 +13974,8 @@
       <c r="B140" s="26">
         <v>3</v>
       </c>
-      <c r="C140" s="55" t="s">
-        <v>169</v>
+      <c r="C140" s="53" t="s">
+        <v>196</v>
       </c>
       <c r="D140" s="29"/>
       <c r="E140" s="13"/>
@@ -13821,8 +14047,8 @@
       <c r="B141" s="26">
         <v>3</v>
       </c>
-      <c r="C141" s="55" t="s">
-        <v>171</v>
+      <c r="C141" s="53" t="s">
+        <v>169</v>
       </c>
       <c r="D141" s="29"/>
       <c r="E141" s="13"/>
@@ -13894,8 +14120,8 @@
       <c r="B142" s="26">
         <v>3</v>
       </c>
-      <c r="C142" s="55" t="s">
-        <v>175</v>
+      <c r="C142" s="53" t="s">
+        <v>171</v>
       </c>
       <c r="D142" s="29"/>
       <c r="E142" s="13"/>
@@ -13967,8 +14193,8 @@
       <c r="B143" s="26">
         <v>3</v>
       </c>
-      <c r="C143" s="55" t="s">
-        <v>176</v>
+      <c r="C143" s="53" t="s">
+        <v>175</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="13"/>
@@ -14035,13 +14261,13 @@
       <c r="HB143" s="28"/>
       <c r="HC143" s="28"/>
     </row>
-    <row r="144" spans="1:211" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="25"/>
       <c r="B144" s="26">
         <v>3</v>
       </c>
-      <c r="C144" s="55" t="s">
-        <v>180</v>
+      <c r="C144" s="53" t="s">
+        <v>176</v>
       </c>
       <c r="D144" s="29"/>
       <c r="E144" s="13"/>
@@ -14108,13 +14334,13 @@
       <c r="HB144" s="28"/>
       <c r="HC144" s="28"/>
     </row>
-    <row r="145" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:211" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="25"/>
       <c r="B145" s="26">
         <v>3</v>
       </c>
-      <c r="C145" s="55" t="s">
-        <v>192</v>
+      <c r="C145" s="53" t="s">
+        <v>180</v>
       </c>
       <c r="D145" s="29"/>
       <c r="E145" s="13"/>
@@ -14186,8 +14412,8 @@
       <c r="B146" s="26">
         <v>3</v>
       </c>
-      <c r="C146" s="55" t="s">
-        <v>193</v>
+      <c r="C146" s="53" t="s">
+        <v>192</v>
       </c>
       <c r="D146" s="29"/>
       <c r="E146" s="13"/>
@@ -14254,13 +14480,13 @@
       <c r="HB146" s="28"/>
       <c r="HC146" s="28"/>
     </row>
-    <row r="147" spans="1:211" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="25"/>
       <c r="B147" s="26">
         <v>3</v>
       </c>
-      <c r="C147" s="55" t="s">
-        <v>197</v>
+      <c r="C147" s="53" t="s">
+        <v>193</v>
       </c>
       <c r="D147" s="29"/>
       <c r="E147" s="13"/>
@@ -14327,13 +14553,13 @@
       <c r="HB147" s="28"/>
       <c r="HC147" s="28"/>
     </row>
-    <row r="148" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:211" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="25"/>
       <c r="B148" s="26">
-        <v>2</v>
-      </c>
-      <c r="C148" s="55" t="s">
-        <v>149</v>
+        <v>3</v>
+      </c>
+      <c r="C148" s="53" t="s">
+        <v>197</v>
       </c>
       <c r="D148" s="29"/>
       <c r="E148" s="13"/>
@@ -14405,8 +14631,8 @@
       <c r="B149" s="26">
         <v>2</v>
       </c>
-      <c r="C149" s="55" t="s">
-        <v>170</v>
+      <c r="C149" s="53" t="s">
+        <v>149</v>
       </c>
       <c r="D149" s="29"/>
       <c r="E149" s="13"/>
@@ -14478,8 +14704,8 @@
       <c r="B150" s="26">
         <v>2</v>
       </c>
-      <c r="C150" s="55" t="s">
-        <v>166</v>
+      <c r="C150" s="53" t="s">
+        <v>170</v>
       </c>
       <c r="D150" s="29"/>
       <c r="E150" s="13"/>
@@ -14551,8 +14777,8 @@
       <c r="B151" s="26">
         <v>2</v>
       </c>
-      <c r="C151" s="55" t="s">
-        <v>148</v>
+      <c r="C151" s="53" t="s">
+        <v>166</v>
       </c>
       <c r="D151" s="29"/>
       <c r="E151" s="13"/>
@@ -14624,8 +14850,8 @@
       <c r="B152" s="26">
         <v>2</v>
       </c>
-      <c r="C152" s="55" t="s">
-        <v>167</v>
+      <c r="C152" s="53" t="s">
+        <v>148</v>
       </c>
       <c r="D152" s="29"/>
       <c r="E152" s="13"/>
@@ -14692,13 +14918,13 @@
       <c r="HB152" s="28"/>
       <c r="HC152" s="28"/>
     </row>
-    <row r="153" spans="1:211" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="25"/>
       <c r="B153" s="26">
         <v>2</v>
       </c>
-      <c r="C153" s="55" t="s">
-        <v>201</v>
+      <c r="C153" s="53" t="s">
+        <v>167</v>
       </c>
       <c r="D153" s="29"/>
       <c r="E153" s="13"/>
@@ -14765,13 +14991,13 @@
       <c r="HB153" s="28"/>
       <c r="HC153" s="28"/>
     </row>
-    <row r="154" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:211" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="25"/>
       <c r="B154" s="26">
         <v>2</v>
       </c>
-      <c r="C154" s="55" t="s">
-        <v>178</v>
+      <c r="C154" s="53" t="s">
+        <v>201</v>
       </c>
       <c r="D154" s="29"/>
       <c r="E154" s="13"/>
@@ -14843,8 +15069,8 @@
       <c r="B155" s="26">
         <v>2</v>
       </c>
-      <c r="C155" s="55" t="s">
-        <v>179</v>
+      <c r="C155" s="53" t="s">
+        <v>178</v>
       </c>
       <c r="D155" s="29"/>
       <c r="E155" s="13"/>
@@ -14914,10 +15140,10 @@
     <row r="156" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="25"/>
       <c r="B156" s="26">
-        <v>1</v>
-      </c>
-      <c r="C156" s="55" t="s">
-        <v>142</v>
+        <v>2</v>
+      </c>
+      <c r="C156" s="53" t="s">
+        <v>179</v>
       </c>
       <c r="D156" s="29"/>
       <c r="E156" s="13"/>
@@ -14989,15 +15215,11 @@
       <c r="B157" s="26">
         <v>1</v>
       </c>
-      <c r="C157" s="55" t="s">
-        <v>139</v>
-      </c>
-      <c r="D157" s="29">
-        <v>116</v>
-      </c>
-      <c r="E157" s="13">
-        <v>1</v>
-      </c>
+      <c r="C157" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="D157" s="29"/>
+      <c r="E157" s="13"/>
       <c r="F157" s="13"/>
       <c r="G157" s="13"/>
       <c r="H157" s="5"/>
@@ -15062,17 +15284,15 @@
       <c r="HC157" s="28"/>
     </row>
     <row r="158" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="25" t="s">
-        <v>20</v>
-      </c>
+      <c r="A158" s="25"/>
       <c r="B158" s="26">
         <v>1</v>
       </c>
-      <c r="C158" s="55" t="s">
-        <v>74</v>
+      <c r="C158" s="53" t="s">
+        <v>139</v>
       </c>
       <c r="D158" s="29">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E158" s="13">
         <v>1</v>
@@ -15100,6 +15320,7 @@
       <c r="BS158" s="28"/>
       <c r="BY158" s="28"/>
       <c r="BZ158" s="28"/>
+      <c r="CE158" s="38"/>
       <c r="CF158" s="28"/>
       <c r="CG158" s="28"/>
       <c r="CM158" s="28"/>
@@ -15146,20 +15367,18 @@
       <c r="B159" s="26">
         <v>1</v>
       </c>
-      <c r="C159" s="56" t="s">
-        <v>44</v>
+      <c r="C159" s="53" t="s">
+        <v>74</v>
       </c>
       <c r="D159" s="29">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E159" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F159" s="13"/>
       <c r="G159" s="13"/>
-      <c r="H159" s="5">
-        <v>0.5</v>
-      </c>
+      <c r="H159" s="5"/>
       <c r="N159" s="28"/>
       <c r="O159" s="28"/>
       <c r="U159" s="28"/>
@@ -15220,18 +15439,26 @@
       <c r="HC159" s="28"/>
     </row>
     <row r="160" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="25"/>
+      <c r="A160" s="25" t="s">
+        <v>20</v>
+      </c>
       <c r="B160" s="26">
         <v>1</v>
       </c>
-      <c r="C160" s="55" t="s">
-        <v>153</v>
-      </c>
-      <c r="D160" s="29"/>
-      <c r="E160" s="13"/>
+      <c r="C160" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="D160" s="29">
+        <v>113</v>
+      </c>
+      <c r="E160" s="13">
+        <v>4</v>
+      </c>
       <c r="F160" s="13"/>
       <c r="G160" s="13"/>
-      <c r="H160" s="5"/>
+      <c r="H160" s="5">
+        <v>0.5</v>
+      </c>
       <c r="N160" s="28"/>
       <c r="O160" s="28"/>
       <c r="U160" s="28"/>
@@ -15252,7 +15479,6 @@
       <c r="BS160" s="28"/>
       <c r="BY160" s="28"/>
       <c r="BZ160" s="28"/>
-      <c r="CE160" s="38"/>
       <c r="CF160" s="28"/>
       <c r="CG160" s="28"/>
       <c r="CM160" s="28"/>
@@ -15297,8 +15523,8 @@
       <c r="B161" s="26">
         <v>1</v>
       </c>
-      <c r="C161" s="55" t="s">
-        <v>155</v>
+      <c r="C161" s="53" t="s">
+        <v>153</v>
       </c>
       <c r="D161" s="29"/>
       <c r="E161" s="13"/>
@@ -15365,22 +15591,16 @@
       <c r="HB161" s="28"/>
       <c r="HC161" s="28"/>
     </row>
-    <row r="162" spans="1:211" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="25" t="s">
-        <v>18</v>
-      </c>
+    <row r="162" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="25"/>
       <c r="B162" s="26">
         <v>1</v>
       </c>
-      <c r="C162" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="D162" s="29">
-        <v>100</v>
-      </c>
-      <c r="E162" s="13">
-        <v>1</v>
-      </c>
+      <c r="C162" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="D162" s="29"/>
+      <c r="E162" s="13"/>
       <c r="F162" s="13"/>
       <c r="G162" s="13"/>
       <c r="H162" s="5"/>
@@ -15404,6 +15624,7 @@
       <c r="BS162" s="28"/>
       <c r="BY162" s="28"/>
       <c r="BZ162" s="28"/>
+      <c r="CE162" s="38"/>
       <c r="CF162" s="28"/>
       <c r="CG162" s="28"/>
       <c r="CM162" s="28"/>
@@ -15443,16 +15664,22 @@
       <c r="HB162" s="28"/>
       <c r="HC162" s="28"/>
     </row>
-    <row r="163" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="25"/>
+    <row r="163" spans="1:211" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="B163" s="26">
         <v>1</v>
       </c>
-      <c r="C163" s="55" t="s">
-        <v>136</v>
-      </c>
-      <c r="D163" s="29"/>
-      <c r="E163" s="13"/>
+      <c r="C163" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D163" s="29">
+        <v>100</v>
+      </c>
+      <c r="E163" s="13">
+        <v>1</v>
+      </c>
       <c r="F163" s="13"/>
       <c r="G163" s="13"/>
       <c r="H163" s="5"/>
@@ -15517,8 +15744,12 @@
     </row>
     <row r="164" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="25"/>
-      <c r="B164" s="26"/>
-      <c r="C164" s="55"/>
+      <c r="B164" s="26">
+        <v>1</v>
+      </c>
+      <c r="C164" s="53" t="s">
+        <v>136</v>
+      </c>
       <c r="D164" s="29"/>
       <c r="E164" s="13"/>
       <c r="F164" s="13"/>
@@ -15544,7 +15775,6 @@
       <c r="BS164" s="28"/>
       <c r="BY164" s="28"/>
       <c r="BZ164" s="28"/>
-      <c r="CE164" s="38"/>
       <c r="CF164" s="28"/>
       <c r="CG164" s="28"/>
       <c r="CM164" s="28"/>
@@ -15587,7 +15817,7 @@
     <row r="165" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="25"/>
       <c r="B165" s="26"/>
-      <c r="C165" s="55"/>
+      <c r="C165" s="53"/>
       <c r="D165" s="29"/>
       <c r="E165" s="13"/>
       <c r="F165" s="13"/>
@@ -15653,13 +15883,82 @@
       <c r="HB165" s="28"/>
       <c r="HC165" s="28"/>
     </row>
-    <row r="166" spans="1:211" x14ac:dyDescent="0.25">
-      <c r="A166" s="14"/>
-      <c r="B166" s="14"/>
+    <row r="166" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="25"/>
+      <c r="B166" s="26"/>
+      <c r="C166" s="53"/>
+      <c r="D166" s="29"/>
+      <c r="E166" s="13"/>
+      <c r="F166" s="13"/>
+      <c r="G166" s="13"/>
+      <c r="H166" s="5"/>
+      <c r="N166" s="28"/>
+      <c r="O166" s="28"/>
+      <c r="U166" s="28"/>
+      <c r="V166" s="28"/>
+      <c r="AB166" s="28"/>
+      <c r="AC166" s="28"/>
+      <c r="AI166" s="28"/>
+      <c r="AJ166" s="28"/>
+      <c r="AP166" s="28"/>
+      <c r="AQ166" s="28"/>
+      <c r="AW166" s="28"/>
+      <c r="AX166" s="28"/>
+      <c r="BD166" s="28"/>
+      <c r="BE166" s="28"/>
+      <c r="BK166" s="28"/>
+      <c r="BL166" s="28"/>
+      <c r="BR166" s="28"/>
+      <c r="BS166" s="28"/>
+      <c r="BY166" s="28"/>
+      <c r="BZ166" s="28"/>
       <c r="CE166" s="38"/>
-      <c r="CG166" s="38"/>
-      <c r="CI166" s="38"/>
-      <c r="CK166" s="38"/>
+      <c r="CF166" s="28"/>
+      <c r="CG166" s="28"/>
+      <c r="CM166" s="28"/>
+      <c r="CN166" s="28"/>
+      <c r="CT166" s="28"/>
+      <c r="CU166" s="28"/>
+      <c r="DA166" s="28"/>
+      <c r="DB166" s="28"/>
+      <c r="DH166" s="28"/>
+      <c r="DI166" s="28"/>
+      <c r="DO166" s="28"/>
+      <c r="DP166" s="28"/>
+      <c r="DV166" s="28"/>
+      <c r="DW166" s="28"/>
+      <c r="EC166" s="28"/>
+      <c r="ED166" s="28"/>
+      <c r="EJ166" s="28"/>
+      <c r="EK166" s="28"/>
+      <c r="EQ166" s="28"/>
+      <c r="ER166" s="28"/>
+      <c r="EX166" s="28"/>
+      <c r="EY166" s="28"/>
+      <c r="FE166" s="28"/>
+      <c r="FF166" s="28"/>
+      <c r="FL166" s="28"/>
+      <c r="FM166" s="28"/>
+      <c r="FS166" s="28"/>
+      <c r="FT166" s="28"/>
+      <c r="FZ166" s="28"/>
+      <c r="GA166" s="28"/>
+      <c r="GG166" s="28"/>
+      <c r="GH166" s="28"/>
+      <c r="GN166" s="28"/>
+      <c r="GO166" s="28"/>
+      <c r="GU166" s="28"/>
+      <c r="GV166" s="28"/>
+      <c r="HB166" s="28"/>
+      <c r="HC166" s="28"/>
+    </row>
+    <row r="167" spans="1:211" x14ac:dyDescent="0.25">
+      <c r="A167" s="14"/>
+      <c r="B167" s="14"/>
+      <c r="CE167" s="38"/>
+      <c r="CG167" s="38"/>
+      <c r="CI167" s="38"/>
+      <c r="CK167" s="38"/>
     </row>
   </sheetData>
   <sortState ref="A126:HC165">
@@ -15671,65 +15970,91 @@
     <mergeCell ref="A86:C86"/>
     <mergeCell ref="A125:C125"/>
   </mergeCells>
-  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU165 DJ8:DN165 DC8:DG165 EE8:EI165 CA8:CE165 AY8:BC165 AR8:AV165 AK8:AO165 AD8:AH165 BF66:BJ165 BM66:BQ165 BT66:BX165 W78:AA165 P60:T165 CV60:CZ165 CO69:CS165 DX114:EB165 CH60:CL165 EL8:EP165 ES8:EW165 EZ8:FD165 FG8:FK165 FN8:FR165 FU8:FY165 GB8:GF165 GI8:GM165 GP8:GT165 GW8:HA165 J69:M165">
-    <cfRule type="expression" dxfId="17" priority="92">
+  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU125 DJ8:DN125 DC8:DG125 EE8:EI125 CA8:CE125 AY8:BC125 AR8:AV125 AK8:AO125 AD8:AH125 BF66:BJ125 BM66:BQ125 BT66:BX125 W78:AA125 P60:T125 CV60:CZ125 CO69:CS125 DX114:EB125 CH60:CL125 EL8:EP125 ES8:EW125 EZ8:FD125 FG8:FK125 FN8:FR125 FU8:FY125 GB8:GF125 GI8:GM125 GP8:GT125 GW8:HA125 J69:M125 J127:M166 GW127:HA166 GP127:GT166 GI127:GM166 GB127:GF166 FU127:FY166 FN127:FR166 FG127:FK166 EZ127:FD166 ES127:EW166 EL127:EP166 CH127:CL166 DX127:EB166 CO127:CS166 CV127:CZ166 P127:T166 W127:AA166 BT127:BX166 BM127:BQ166 BF127:BJ166 AD127:AH166 AK127:AO166 AR127:AV166 AY127:BC166 CA127:CE166 EE127:EI166 DC127:DG166 DJ127:DN166 DQ127:DU166">
+    <cfRule type="expression" dxfId="33" priority="100">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="93">
+    <cfRule type="expression" dxfId="32" priority="101">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="94">
+    <cfRule type="expression" dxfId="31" priority="102">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="95">
+    <cfRule type="expression" dxfId="30" priority="103">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="96">
+    <cfRule type="expression" dxfId="29" priority="104">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="97">
+    <cfRule type="expression" dxfId="28" priority="105">
       <formula>J$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="98">
+    <cfRule type="expression" dxfId="27" priority="106">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="99">
+    <cfRule type="expression" dxfId="26" priority="107">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A166:HC166">
-    <cfRule type="expression" dxfId="9" priority="91">
+  <conditionalFormatting sqref="A167:HC167">
+    <cfRule type="expression" dxfId="25" priority="99">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:HC7">
-    <cfRule type="expression" dxfId="8" priority="90">
+    <cfRule type="expression" dxfId="24" priority="98">
       <formula>J$7=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL56:CL57">
-    <cfRule type="expression" dxfId="7" priority="81">
+    <cfRule type="expression" dxfId="23" priority="89">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="82">
+    <cfRule type="expression" dxfId="22" priority="90">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="83">
+    <cfRule type="expression" dxfId="21" priority="91">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="84">
+    <cfRule type="expression" dxfId="20" priority="92">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="85">
+    <cfRule type="expression" dxfId="19" priority="93">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="86">
+    <cfRule type="expression" dxfId="18" priority="94">
       <formula>CL$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="87">
+    <cfRule type="expression" dxfId="17" priority="95">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="88">
+    <cfRule type="expression" dxfId="16" priority="96">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J126:M126 GW126:HA126 GP126:GT126 GI126:GM126 GB126:GF126 FU126:FY126 FN126:FR126 FG126:FK126 EZ126:FD126 ES126:EW126 EL126:EP126 CH126:CL126 DX126:EB126 CO126:CS126 CV126:CZ126 P126:T126 W126:AA126 BT126:BX126 BM126:BQ126 BF126:BJ126 AD126:AH126 AK126:AO126 AR126:AV126 AY126:BC126 CA126:CE126 EE126:EI126 DC126:DG126 DJ126:DN126 DQ126:DU126">
+    <cfRule type="expression" dxfId="15" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="6">
+      <formula>J$7=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Working with multiple EAUs per RFQ: -Move fields from RFQHeader to RFQEAV in CRUD and Entities:   *EstimatedAnnualVolume     *SG_A_Profit       *PackingPerUnit         *AssemblyCostPerUnit 	  *EAUCalendarYears
	  -Change RFQHeaderKey to RFQEAVKey in RFQDetailCRUD.
	  -Well written src properties of Register tags.
	  -Handsontable jquery plugin added.
</commit_message>
<xml_diff>
--- a/AQPM Gantt.xlsx
+++ b/AQPM Gantt.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="10305" yWindow="4335" windowWidth="10230" windowHeight="4350"/>
@@ -16,6 +16,7 @@
     <definedName name="Actual">(PeriodInActual*(#REF!&gt;0))*PeriodInPlan</definedName>
     <definedName name="ActualBeyond" localSheetId="0">'APQM Gantt'!PeriodInActual*('APQM Gantt'!$F1&gt;0)</definedName>
     <definedName name="ActualBeyond">PeriodInActual*(#REF!&gt;0)</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'APQM Gantt'!$A$1:$H$96</definedName>
     <definedName name="PercentComplete" localSheetId="0">'APQM Gantt'!PercentCompleteBeyond*'APQM Gantt'!PeriodInPlan</definedName>
     <definedName name="PercentComplete">PercentCompleteBeyond*PeriodInPlan</definedName>
     <definedName name="PercentCompleteBeyond" localSheetId="0">('APQM Gantt'!A$7=MEDIAN('APQM Gantt'!A$7,'APQM Gantt'!$F1,'APQM Gantt'!$F1+'APQM Gantt'!$G1)*('APQM Gantt'!$F1&gt;0))*(('APQM Gantt'!A$7&lt;(INT('APQM Gantt'!$F1+'APQM Gantt'!$G1*'APQM Gantt'!$H1)))+('APQM Gantt'!A$7='APQM Gantt'!$F1))*('APQM Gantt'!$H1&gt;0)</definedName>
@@ -28,7 +29,6 @@
     <definedName name="PeriodInPlan">#REF!=MEDIAN(#REF!,#REF!,#REF!+#REF!-1)</definedName>
     <definedName name="Plan" localSheetId="0">'APQM Gantt'!PeriodInPlan*('APQM Gantt'!$D1&gt;0)</definedName>
     <definedName name="Plan">PeriodInPlan*(#REF!&gt;0)</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'APQM Gantt'!$A$1:$H$96</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -42,10 +42,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="Q13" authorId="0">
+    <comment ref="Q13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA13" authorId="0">
+    <comment ref="AA13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="CL13" authorId="0">
+    <comment ref="CL13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -87,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DK103" authorId="0">
+    <comment ref="DK103" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DX108" authorId="0">
+    <comment ref="DX108" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="203">
   <si>
     <t>Plan</t>
   </si>
@@ -799,6 +799,9 @@
   <si>
     <t>Close RFQ after hiting save or cancel</t>
   </si>
+  <si>
+    <t>Buttons for check all items or uncheck them in BOM screen.</t>
+  </si>
 </sst>
 </file>
 
@@ -807,7 +810,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -957,6 +960,15 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="13"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1121,7 +1133,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1291,10 +1303,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Activity" xfId="2"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Label" xfId="5"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6"/>
@@ -1302,119 +1317,134 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="33">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1784,134 +1814,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1957,7 +1859,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2049" name="Spinner 1" hidden="1">
+            <xdr:cNvPr id="2049" name="Spinner 1" descr="Period Highlight Spin Control" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2049"/>
@@ -1966,7 +1868,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1974,6 +1876,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData fPrintsWithSheet="0"/>
@@ -1985,15 +1893,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A4:F238"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="39"/>
-    <tableColumn id="2" name="Date" dataDxfId="38"/>
-    <tableColumn id="3" name="Creator" dataDxfId="37"/>
-    <tableColumn id="4" name="Issue" dataDxfId="36"/>
-    <tableColumn id="5" name="Status" dataDxfId="35"/>
-    <tableColumn id="6" name="Solution" dataDxfId="34"/>
+    <tableColumn id="1" name="#" dataDxfId="5"/>
+    <tableColumn id="2" name="Date" dataDxfId="4"/>
+    <tableColumn id="3" name="Creator" dataDxfId="3"/>
+    <tableColumn id="4" name="Issue" dataDxfId="2"/>
+    <tableColumn id="5" name="Status" dataDxfId="1"/>
+    <tableColumn id="6" name="Solution" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2229,16 +2137,16 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:HC167"/>
+  <dimension ref="A2:HC170"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="J122" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="7" topLeftCell="J162" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="F126" sqref="F126"/>
+      <selection pane="bottomRight" activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.375" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
@@ -15960,6 +15868,14 @@
       <c r="CI167" s="38"/>
       <c r="CK167" s="38"/>
     </row>
+    <row r="169" spans="1:211" x14ac:dyDescent="0.25">
+      <c r="C169" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="170" spans="1:211" x14ac:dyDescent="0.25">
+      <c r="C170" s="57"/>
+    </row>
   </sheetData>
   <sortState ref="A126:HC165">
     <sortCondition descending="1" ref="B126:B165"/>
@@ -15971,90 +15887,90 @@
     <mergeCell ref="A125:C125"/>
   </mergeCells>
   <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU125 DJ8:DN125 DC8:DG125 EE8:EI125 CA8:CE125 AY8:BC125 AR8:AV125 AK8:AO125 AD8:AH125 BF66:BJ125 BM66:BQ125 BT66:BX125 W78:AA125 P60:T125 CV60:CZ125 CO69:CS125 DX114:EB125 CH60:CL125 EL8:EP125 ES8:EW125 EZ8:FD125 FG8:FK125 FN8:FR125 FU8:FY125 GB8:GF125 GI8:GM125 GP8:GT125 GW8:HA125 J69:M125 J127:M166 GW127:HA166 GP127:GT166 GI127:GM166 GB127:GF166 FU127:FY166 FN127:FR166 FG127:FK166 EZ127:FD166 ES127:EW166 EL127:EP166 CH127:CL166 DX127:EB166 CO127:CS166 CV127:CZ166 P127:T166 W127:AA166 BT127:BX166 BM127:BQ166 BF127:BJ166 AD127:AH166 AK127:AO166 AR127:AV166 AY127:BC166 CA127:CE166 EE127:EI166 DC127:DG166 DJ127:DN166 DQ127:DU166">
-    <cfRule type="expression" dxfId="33" priority="100">
+    <cfRule type="expression" dxfId="32" priority="100">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="101">
+    <cfRule type="expression" dxfId="31" priority="101">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="102">
+    <cfRule type="expression" dxfId="30" priority="102">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="103">
+    <cfRule type="expression" dxfId="29" priority="103">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="104">
+    <cfRule type="expression" dxfId="28" priority="104">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="105">
+    <cfRule type="expression" dxfId="27" priority="105">
       <formula>J$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="106">
+    <cfRule type="expression" dxfId="26" priority="106">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="107">
+    <cfRule type="expression" dxfId="25" priority="107">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A167:HC167">
-    <cfRule type="expression" dxfId="25" priority="99">
+    <cfRule type="expression" dxfId="24" priority="99">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:HC7">
-    <cfRule type="expression" dxfId="24" priority="98">
+    <cfRule type="expression" dxfId="23" priority="98">
       <formula>J$7=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL56:CL57">
-    <cfRule type="expression" dxfId="23" priority="89">
+    <cfRule type="expression" dxfId="22" priority="89">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="90">
+    <cfRule type="expression" dxfId="21" priority="90">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="91">
+    <cfRule type="expression" dxfId="20" priority="91">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="92">
+    <cfRule type="expression" dxfId="19" priority="92">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="93">
+    <cfRule type="expression" dxfId="18" priority="93">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="94">
+    <cfRule type="expression" dxfId="17" priority="94">
       <formula>CL$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="95">
+    <cfRule type="expression" dxfId="16" priority="95">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="96">
+    <cfRule type="expression" dxfId="15" priority="96">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J126:M126 GW126:HA126 GP126:GT126 GI126:GM126 GB126:GF126 FU126:FY126 FN126:FR126 FG126:FK126 EZ126:FD126 ES126:EW126 EL126:EP126 CH126:CL126 DX126:EB126 CO126:CS126 CV126:CZ126 P126:T126 W126:AA126 BT126:BX126 BM126:BQ126 BF126:BJ126 AD126:AH126 AK126:AO126 AR126:AV126 AY126:BC126 CA126:CE126 EE126:EI126 DC126:DG126 DJ126:DN126 DQ126:DU126">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>J$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16102,7 +16018,7 @@
       <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.625" style="36" customWidth="1"/>
     <col min="2" max="2" width="11.375" style="33" customWidth="1"/>

</xml_diff>

<commit_message>
-Highlighting rows already selected/awarded when selecting one BOM Detail for RFQ Summary
</commit_message>
<xml_diff>
--- a/AQPM Gantt.xlsx
+++ b/AQPM Gantt.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Issues" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'APQM Gantt'!$A$7:$EK$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'APQM Gantt'!$A$7:$EK$129</definedName>
     <definedName name="Actual" localSheetId="0">('APQM Gantt'!PeriodInActual*('APQM Gantt'!$F1&gt;0))*'APQM Gantt'!PeriodInPlan</definedName>
     <definedName name="Actual">(PeriodInActual*(#REF!&gt;0))*PeriodInPlan</definedName>
     <definedName name="ActualBeyond" localSheetId="0">'APQM Gantt'!PeriodInActual*('APQM Gantt'!$F1&gt;0)</definedName>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="203">
   <si>
     <t>Plan</t>
   </si>
@@ -1133,7 +1133,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1297,14 +1297,17 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1318,134 +1321,6 @@
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
   <dxfs count="33">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1814,6 +1689,134 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1893,15 +1896,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F238" totalsRowShown="0" headerRowDxfId="32">
   <autoFilter ref="A4:F238"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="5"/>
-    <tableColumn id="2" name="Date" dataDxfId="4"/>
-    <tableColumn id="3" name="Creator" dataDxfId="3"/>
-    <tableColumn id="4" name="Issue" dataDxfId="2"/>
-    <tableColumn id="5" name="Status" dataDxfId="1"/>
-    <tableColumn id="6" name="Solution" dataDxfId="0"/>
+    <tableColumn id="1" name="#" dataDxfId="31"/>
+    <tableColumn id="2" name="Date" dataDxfId="30"/>
+    <tableColumn id="3" name="Creator" dataDxfId="29"/>
+    <tableColumn id="4" name="Issue" dataDxfId="28"/>
+    <tableColumn id="5" name="Status" dataDxfId="27"/>
+    <tableColumn id="6" name="Solution" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2137,13 +2140,13 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:HC170"/>
+  <dimension ref="A2:HC169"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="9" ySplit="7" topLeftCell="J162" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="7" topLeftCell="J122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="C170" sqref="C170"/>
+      <selection pane="bottomRight" activeCell="H129" sqref="H129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
@@ -2160,11 +2163,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:211" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
@@ -2172,9 +2175,9 @@
       <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:211" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
       <c r="D3" s="19" t="s">
         <v>13</v>
       </c>
@@ -2206,9 +2209,9 @@
       </c>
     </row>
     <row r="4" spans="1:211" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="44"/>
       <c r="E4" s="32"/>
       <c r="F4" s="18"/>
@@ -8483,11 +8486,11 @@
       <c r="HC69" s="28"/>
     </row>
     <row r="70" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="55" t="s">
+      <c r="A70" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="55"/>
-      <c r="C70" s="55"/>
+      <c r="B70" s="56"/>
+      <c r="C70" s="56"/>
       <c r="D70" s="29"/>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
@@ -9746,11 +9749,11 @@
       <c r="HC85" s="28"/>
     </row>
     <row r="86" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="55" t="s">
+      <c r="A86" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="B86" s="55"/>
-      <c r="C86" s="55"/>
+      <c r="B86" s="56"/>
+      <c r="C86" s="56"/>
       <c r="D86" s="29"/>
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
@@ -12779,11 +12782,11 @@
       <c r="HC124" s="28"/>
     </row>
     <row r="125" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="55" t="s">
+      <c r="A125" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="B125" s="55"/>
-      <c r="C125" s="55"/>
+      <c r="B125" s="56"/>
+      <c r="C125" s="56"/>
       <c r="D125" s="29"/>
       <c r="E125" s="13"/>
       <c r="F125" s="13"/>
@@ -12922,13 +12925,13 @@
       <c r="HB126" s="28"/>
       <c r="HC126" s="28"/>
     </row>
-    <row r="127" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:211" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="25"/>
       <c r="B127" s="26">
         <v>5</v>
       </c>
       <c r="C127" s="53" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D127" s="29"/>
       <c r="E127" s="13"/>
@@ -12995,13 +12998,13 @@
       <c r="HB127" s="28"/>
       <c r="HC127" s="28"/>
     </row>
-    <row r="128" spans="1:211" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="25"/>
       <c r="B128" s="26">
         <v>5</v>
       </c>
       <c r="C128" s="53" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="D128" s="29"/>
       <c r="E128" s="13"/>
@@ -13073,14 +13076,16 @@
       <c r="B129" s="26">
         <v>5</v>
       </c>
-      <c r="C129" s="53" t="s">
-        <v>165</v>
+      <c r="C129" s="58" t="s">
+        <v>181</v>
       </c>
       <c r="D129" s="29"/>
       <c r="E129" s="13"/>
       <c r="F129" s="13"/>
       <c r="G129" s="13"/>
-      <c r="H129" s="5"/>
+      <c r="H129" s="5">
+        <v>1</v>
+      </c>
       <c r="N129" s="28"/>
       <c r="O129" s="28"/>
       <c r="U129" s="28"/>
@@ -13147,7 +13152,7 @@
         <v>5</v>
       </c>
       <c r="C130" s="53" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D130" s="29"/>
       <c r="E130" s="13"/>
@@ -13219,14 +13224,16 @@
       <c r="B131" s="26">
         <v>5</v>
       </c>
-      <c r="C131" s="53" t="s">
-        <v>177</v>
+      <c r="C131" s="58" t="s">
+        <v>200</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="13"/>
       <c r="F131" s="13"/>
       <c r="G131" s="13"/>
-      <c r="H131" s="5"/>
+      <c r="H131" s="5">
+        <v>1</v>
+      </c>
       <c r="N131" s="28"/>
       <c r="O131" s="28"/>
       <c r="U131" s="28"/>
@@ -13290,10 +13297,10 @@
     <row r="132" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="25"/>
       <c r="B132" s="26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C132" s="53" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="D132" s="29"/>
       <c r="E132" s="13"/>
@@ -13366,13 +13373,19 @@
         <v>4</v>
       </c>
       <c r="C133" s="53" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D133" s="29"/>
       <c r="E133" s="13"/>
-      <c r="F133" s="13"/>
-      <c r="G133" s="13"/>
-      <c r="H133" s="5"/>
+      <c r="F133" s="13">
+        <v>171</v>
+      </c>
+      <c r="G133" s="13">
+        <v>1</v>
+      </c>
+      <c r="H133" s="5">
+        <v>1</v>
+      </c>
       <c r="N133" s="28"/>
       <c r="O133" s="28"/>
       <c r="U133" s="28"/>
@@ -13439,19 +13452,13 @@
         <v>4</v>
       </c>
       <c r="C134" s="53" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="D134" s="29"/>
       <c r="E134" s="13"/>
-      <c r="F134" s="13">
-        <v>171</v>
-      </c>
-      <c r="G134" s="13">
-        <v>1</v>
-      </c>
-      <c r="H134" s="5">
-        <v>1</v>
-      </c>
+      <c r="F134" s="13"/>
+      <c r="G134" s="13"/>
+      <c r="H134" s="5"/>
       <c r="N134" s="28"/>
       <c r="O134" s="28"/>
       <c r="U134" s="28"/>
@@ -13518,7 +13525,7 @@
         <v>4</v>
       </c>
       <c r="C135" s="53" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D135" s="29"/>
       <c r="E135" s="13"/>
@@ -13591,7 +13598,7 @@
         <v>4</v>
       </c>
       <c r="C136" s="53" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D136" s="29"/>
       <c r="E136" s="13"/>
@@ -13664,7 +13671,7 @@
         <v>4</v>
       </c>
       <c r="C137" s="53" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D137" s="29"/>
       <c r="E137" s="13"/>
@@ -13734,10 +13741,10 @@
     <row r="138" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="25"/>
       <c r="B138" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C138" s="53" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="D138" s="29"/>
       <c r="E138" s="13"/>
@@ -13810,7 +13817,7 @@
         <v>3</v>
       </c>
       <c r="C139" s="53" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
       <c r="D139" s="29"/>
       <c r="E139" s="13"/>
@@ -13883,7 +13890,7 @@
         <v>3</v>
       </c>
       <c r="C140" s="53" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="D140" s="29"/>
       <c r="E140" s="13"/>
@@ -13956,7 +13963,7 @@
         <v>3</v>
       </c>
       <c r="C141" s="53" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D141" s="29"/>
       <c r="E141" s="13"/>
@@ -14029,7 +14036,7 @@
         <v>3</v>
       </c>
       <c r="C142" s="53" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D142" s="29"/>
       <c r="E142" s="13"/>
@@ -14102,7 +14109,7 @@
         <v>3</v>
       </c>
       <c r="C143" s="53" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="13"/>
@@ -14169,13 +14176,13 @@
       <c r="HB143" s="28"/>
       <c r="HC143" s="28"/>
     </row>
-    <row r="144" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:211" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="25"/>
       <c r="B144" s="26">
         <v>3</v>
       </c>
       <c r="C144" s="53" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D144" s="29"/>
       <c r="E144" s="13"/>
@@ -14242,13 +14249,13 @@
       <c r="HB144" s="28"/>
       <c r="HC144" s="28"/>
     </row>
-    <row r="145" spans="1:211" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="25"/>
       <c r="B145" s="26">
         <v>3</v>
       </c>
       <c r="C145" s="53" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="D145" s="29"/>
       <c r="E145" s="13"/>
@@ -14321,7 +14328,7 @@
         <v>3</v>
       </c>
       <c r="C146" s="53" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D146" s="29"/>
       <c r="E146" s="13"/>
@@ -14388,13 +14395,13 @@
       <c r="HB146" s="28"/>
       <c r="HC146" s="28"/>
     </row>
-    <row r="147" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:211" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="25"/>
       <c r="B147" s="26">
         <v>3</v>
       </c>
       <c r="C147" s="53" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D147" s="29"/>
       <c r="E147" s="13"/>
@@ -14461,13 +14468,13 @@
       <c r="HB147" s="28"/>
       <c r="HC147" s="28"/>
     </row>
-    <row r="148" spans="1:211" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="25"/>
       <c r="B148" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C148" s="53" t="s">
-        <v>197</v>
+        <v>149</v>
       </c>
       <c r="D148" s="29"/>
       <c r="E148" s="13"/>
@@ -14540,7 +14547,7 @@
         <v>2</v>
       </c>
       <c r="C149" s="53" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="D149" s="29"/>
       <c r="E149" s="13"/>
@@ -14613,7 +14620,7 @@
         <v>2</v>
       </c>
       <c r="C150" s="53" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D150" s="29"/>
       <c r="E150" s="13"/>
@@ -14686,7 +14693,7 @@
         <v>2</v>
       </c>
       <c r="C151" s="53" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="D151" s="29"/>
       <c r="E151" s="13"/>
@@ -14759,7 +14766,7 @@
         <v>2</v>
       </c>
       <c r="C152" s="53" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="D152" s="29"/>
       <c r="E152" s="13"/>
@@ -14826,13 +14833,13 @@
       <c r="HB152" s="28"/>
       <c r="HC152" s="28"/>
     </row>
-    <row r="153" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:211" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="25"/>
       <c r="B153" s="26">
         <v>2</v>
       </c>
       <c r="C153" s="53" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="D153" s="29"/>
       <c r="E153" s="13"/>
@@ -14899,13 +14906,13 @@
       <c r="HB153" s="28"/>
       <c r="HC153" s="28"/>
     </row>
-    <row r="154" spans="1:211" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="25"/>
       <c r="B154" s="26">
         <v>2</v>
       </c>
       <c r="C154" s="53" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="D154" s="29"/>
       <c r="E154" s="13"/>
@@ -14978,7 +14985,7 @@
         <v>2</v>
       </c>
       <c r="C155" s="53" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D155" s="29"/>
       <c r="E155" s="13"/>
@@ -15048,10 +15055,10 @@
     <row r="156" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="25"/>
       <c r="B156" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C156" s="53" t="s">
-        <v>179</v>
+        <v>142</v>
       </c>
       <c r="D156" s="29"/>
       <c r="E156" s="13"/>
@@ -15124,10 +15131,14 @@
         <v>1</v>
       </c>
       <c r="C157" s="53" t="s">
-        <v>142</v>
-      </c>
-      <c r="D157" s="29"/>
-      <c r="E157" s="13"/>
+        <v>139</v>
+      </c>
+      <c r="D157" s="29">
+        <v>116</v>
+      </c>
+      <c r="E157" s="13">
+        <v>1</v>
+      </c>
       <c r="F157" s="13"/>
       <c r="G157" s="13"/>
       <c r="H157" s="5"/>
@@ -15192,15 +15203,17 @@
       <c r="HC157" s="28"/>
     </row>
     <row r="158" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="25"/>
+      <c r="A158" s="25" t="s">
+        <v>20</v>
+      </c>
       <c r="B158" s="26">
         <v>1</v>
       </c>
       <c r="C158" s="53" t="s">
-        <v>139</v>
+        <v>74</v>
       </c>
       <c r="D158" s="29">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E158" s="13">
         <v>1</v>
@@ -15228,7 +15241,6 @@
       <c r="BS158" s="28"/>
       <c r="BY158" s="28"/>
       <c r="BZ158" s="28"/>
-      <c r="CE158" s="38"/>
       <c r="CF158" s="28"/>
       <c r="CG158" s="28"/>
       <c r="CM158" s="28"/>
@@ -15275,18 +15287,20 @@
       <c r="B159" s="26">
         <v>1</v>
       </c>
-      <c r="C159" s="53" t="s">
-        <v>74</v>
+      <c r="C159" s="54" t="s">
+        <v>44</v>
       </c>
       <c r="D159" s="29">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E159" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F159" s="13"/>
       <c r="G159" s="13"/>
-      <c r="H159" s="5"/>
+      <c r="H159" s="5">
+        <v>0.5</v>
+      </c>
       <c r="N159" s="28"/>
       <c r="O159" s="28"/>
       <c r="U159" s="28"/>
@@ -15347,26 +15361,18 @@
       <c r="HC159" s="28"/>
     </row>
     <row r="160" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="25" t="s">
-        <v>20</v>
-      </c>
+      <c r="A160" s="25"/>
       <c r="B160" s="26">
         <v>1</v>
       </c>
-      <c r="C160" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="D160" s="29">
-        <v>113</v>
-      </c>
-      <c r="E160" s="13">
-        <v>4</v>
-      </c>
+      <c r="C160" s="53" t="s">
+        <v>153</v>
+      </c>
+      <c r="D160" s="29"/>
+      <c r="E160" s="13"/>
       <c r="F160" s="13"/>
       <c r="G160" s="13"/>
-      <c r="H160" s="5">
-        <v>0.5</v>
-      </c>
+      <c r="H160" s="5"/>
       <c r="N160" s="28"/>
       <c r="O160" s="28"/>
       <c r="U160" s="28"/>
@@ -15387,6 +15393,7 @@
       <c r="BS160" s="28"/>
       <c r="BY160" s="28"/>
       <c r="BZ160" s="28"/>
+      <c r="CE160" s="38"/>
       <c r="CF160" s="28"/>
       <c r="CG160" s="28"/>
       <c r="CM160" s="28"/>
@@ -15432,7 +15439,7 @@
         <v>1</v>
       </c>
       <c r="C161" s="53" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D161" s="29"/>
       <c r="E161" s="13"/>
@@ -15499,16 +15506,22 @@
       <c r="HB161" s="28"/>
       <c r="HC161" s="28"/>
     </row>
-    <row r="162" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="25"/>
+    <row r="162" spans="1:211" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="B162" s="26">
         <v>1</v>
       </c>
-      <c r="C162" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="D162" s="29"/>
-      <c r="E162" s="13"/>
+      <c r="C162" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D162" s="29">
+        <v>100</v>
+      </c>
+      <c r="E162" s="13">
+        <v>1</v>
+      </c>
       <c r="F162" s="13"/>
       <c r="G162" s="13"/>
       <c r="H162" s="5"/>
@@ -15532,7 +15545,6 @@
       <c r="BS162" s="28"/>
       <c r="BY162" s="28"/>
       <c r="BZ162" s="28"/>
-      <c r="CE162" s="38"/>
       <c r="CF162" s="28"/>
       <c r="CG162" s="28"/>
       <c r="CM162" s="28"/>
@@ -15572,22 +15584,16 @@
       <c r="HB162" s="28"/>
       <c r="HC162" s="28"/>
     </row>
-    <row r="163" spans="1:211" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="25" t="s">
-        <v>18</v>
-      </c>
+    <row r="163" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="25"/>
       <c r="B163" s="26">
         <v>1</v>
       </c>
-      <c r="C163" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="D163" s="29">
-        <v>100</v>
-      </c>
-      <c r="E163" s="13">
-        <v>1</v>
-      </c>
+      <c r="C163" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="D163" s="29"/>
+      <c r="E163" s="13"/>
       <c r="F163" s="13"/>
       <c r="G163" s="13"/>
       <c r="H163" s="5"/>
@@ -15652,12 +15658,8 @@
     </row>
     <row r="164" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="25"/>
-      <c r="B164" s="26">
-        <v>1</v>
-      </c>
-      <c r="C164" s="53" t="s">
-        <v>136</v>
-      </c>
+      <c r="B164" s="26"/>
+      <c r="C164" s="53"/>
       <c r="D164" s="29"/>
       <c r="E164" s="13"/>
       <c r="F164" s="13"/>
@@ -15683,6 +15685,7 @@
       <c r="BS164" s="28"/>
       <c r="BY164" s="28"/>
       <c r="BZ164" s="28"/>
+      <c r="CE164" s="38"/>
       <c r="CF164" s="28"/>
       <c r="CG164" s="28"/>
       <c r="CM164" s="28"/>
@@ -15791,90 +15794,21 @@
       <c r="HB165" s="28"/>
       <c r="HC165" s="28"/>
     </row>
-    <row r="166" spans="1:211" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="25"/>
-      <c r="B166" s="26"/>
-      <c r="C166" s="53"/>
-      <c r="D166" s="29"/>
-      <c r="E166" s="13"/>
-      <c r="F166" s="13"/>
-      <c r="G166" s="13"/>
-      <c r="H166" s="5"/>
-      <c r="N166" s="28"/>
-      <c r="O166" s="28"/>
-      <c r="U166" s="28"/>
-      <c r="V166" s="28"/>
-      <c r="AB166" s="28"/>
-      <c r="AC166" s="28"/>
-      <c r="AI166" s="28"/>
-      <c r="AJ166" s="28"/>
-      <c r="AP166" s="28"/>
-      <c r="AQ166" s="28"/>
-      <c r="AW166" s="28"/>
-      <c r="AX166" s="28"/>
-      <c r="BD166" s="28"/>
-      <c r="BE166" s="28"/>
-      <c r="BK166" s="28"/>
-      <c r="BL166" s="28"/>
-      <c r="BR166" s="28"/>
-      <c r="BS166" s="28"/>
-      <c r="BY166" s="28"/>
-      <c r="BZ166" s="28"/>
+    <row r="166" spans="1:211" x14ac:dyDescent="0.25">
+      <c r="A166" s="14"/>
+      <c r="B166" s="14"/>
       <c r="CE166" s="38"/>
-      <c r="CF166" s="28"/>
-      <c r="CG166" s="28"/>
-      <c r="CM166" s="28"/>
-      <c r="CN166" s="28"/>
-      <c r="CT166" s="28"/>
-      <c r="CU166" s="28"/>
-      <c r="DA166" s="28"/>
-      <c r="DB166" s="28"/>
-      <c r="DH166" s="28"/>
-      <c r="DI166" s="28"/>
-      <c r="DO166" s="28"/>
-      <c r="DP166" s="28"/>
-      <c r="DV166" s="28"/>
-      <c r="DW166" s="28"/>
-      <c r="EC166" s="28"/>
-      <c r="ED166" s="28"/>
-      <c r="EJ166" s="28"/>
-      <c r="EK166" s="28"/>
-      <c r="EQ166" s="28"/>
-      <c r="ER166" s="28"/>
-      <c r="EX166" s="28"/>
-      <c r="EY166" s="28"/>
-      <c r="FE166" s="28"/>
-      <c r="FF166" s="28"/>
-      <c r="FL166" s="28"/>
-      <c r="FM166" s="28"/>
-      <c r="FS166" s="28"/>
-      <c r="FT166" s="28"/>
-      <c r="FZ166" s="28"/>
-      <c r="GA166" s="28"/>
-      <c r="GG166" s="28"/>
-      <c r="GH166" s="28"/>
-      <c r="GN166" s="28"/>
-      <c r="GO166" s="28"/>
-      <c r="GU166" s="28"/>
-      <c r="GV166" s="28"/>
-      <c r="HB166" s="28"/>
-      <c r="HC166" s="28"/>
-    </row>
-    <row r="167" spans="1:211" x14ac:dyDescent="0.25">
-      <c r="A167" s="14"/>
-      <c r="B167" s="14"/>
-      <c r="CE167" s="38"/>
-      <c r="CG167" s="38"/>
-      <c r="CI167" s="38"/>
-      <c r="CK167" s="38"/>
+      <c r="CG166" s="38"/>
+      <c r="CI166" s="38"/>
+      <c r="CK166" s="38"/>
+    </row>
+    <row r="168" spans="1:211" x14ac:dyDescent="0.25">
+      <c r="C168" s="14" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="169" spans="1:211" x14ac:dyDescent="0.25">
-      <c r="C169" s="14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="170" spans="1:211" x14ac:dyDescent="0.25">
-      <c r="C170" s="57"/>
+      <c r="C169" s="55"/>
     </row>
   </sheetData>
   <sortState ref="A126:HC165">
@@ -15886,91 +15820,65 @@
     <mergeCell ref="A86:C86"/>
     <mergeCell ref="A125:C125"/>
   </mergeCells>
-  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 DQ8:DU125 DJ8:DN125 DC8:DG125 EE8:EI125 CA8:CE125 AY8:BC125 AR8:AV125 AK8:AO125 AD8:AH125 BF66:BJ125 BM66:BQ125 BT66:BX125 W78:AA125 P60:T125 CV60:CZ125 CO69:CS125 DX114:EB125 CH60:CL125 EL8:EP125 ES8:EW125 EZ8:FD125 FG8:FK125 FN8:FR125 FU8:FY125 GB8:GF125 GI8:GM125 GP8:GT125 GW8:HA125 J69:M125 J127:M166 GW127:HA166 GP127:GT166 GI127:GM166 GB127:GF166 FU127:FY166 FN127:FR166 FG127:FK166 EZ127:FD166 ES127:EW166 EL127:EP166 CH127:CL166 DX127:EB166 CO127:CS166 CV127:CZ166 P127:T166 W127:AA166 BT127:BX166 BM127:BQ166 BF127:BJ166 AD127:AH166 AK127:AO166 AR127:AV166 AY127:BC166 CA127:CE166 EE127:EI166 DC127:DG166 DJ127:DN166 DQ127:DU166">
-    <cfRule type="expression" dxfId="32" priority="100">
+  <conditionalFormatting sqref="T31:T50 T52:T59 CL58:CL59 R58:R59 CV52:CV59 CO68:CR68 L68:M68 J68 Z76:AA77 W76:Y76 CV31:CV50 P8:T30 CV8:CZ30 AA8:AA12 BI8:BI42 BN8:BN42 BX8:BX46 R31:R54 S31:S59 P31:Q59 CW31:CZ59 CL14:CL54 CH8:CK59 CL8:CL12 BT8:BW65 BO8:BQ65 BM8:BM65 BJ8:BJ65 BF8:BH65 W8:Z65 AA14:AA65 BI44:BI65 BN44:BN65 BX48:BX65 CO8:CS67 J8:M67 W66:AA75 DX109:DX113 DX79:DX107 DX8:EB78 DY79:EB113 J69:M165 GW8:HA165 GP8:GT165 GI8:GM165 GB8:GF165 FU8:FY165 FN8:FR165 FG8:FK165 EZ8:FD165 ES8:EW165 EL8:EP165 CH60:CL165 DX114:EB165 CO69:CS165 CV60:CZ165 P60:T165 W78:AA165 BT66:BX165 BM66:BQ165 BF66:BJ165 AD8:AH165 AK8:AO165 AR8:AV165 AY8:BC165 CA8:CE165 EE8:EI165 DC8:DG165 DJ8:DN165 DQ8:DU165">
+    <cfRule type="expression" dxfId="25" priority="100">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="101">
+    <cfRule type="expression" dxfId="24" priority="101">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="102">
+    <cfRule type="expression" dxfId="23" priority="102">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="103">
+    <cfRule type="expression" dxfId="22" priority="103">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="104">
+    <cfRule type="expression" dxfId="21" priority="104">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="105">
+    <cfRule type="expression" dxfId="20" priority="105">
       <formula>J$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="106">
+    <cfRule type="expression" dxfId="19" priority="106">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="107">
+    <cfRule type="expression" dxfId="18" priority="107">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A167:HC167">
-    <cfRule type="expression" dxfId="24" priority="99">
+  <conditionalFormatting sqref="A166:HC166">
+    <cfRule type="expression" dxfId="17" priority="99">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:HC7">
-    <cfRule type="expression" dxfId="23" priority="98">
+    <cfRule type="expression" dxfId="16" priority="98">
       <formula>J$7=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL56:CL57">
-    <cfRule type="expression" dxfId="22" priority="89">
+    <cfRule type="expression" dxfId="15" priority="89">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="90">
+    <cfRule type="expression" dxfId="14" priority="90">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="91">
+    <cfRule type="expression" dxfId="13" priority="91">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="92">
+    <cfRule type="expression" dxfId="12" priority="92">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="93">
+    <cfRule type="expression" dxfId="11" priority="93">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="94">
+    <cfRule type="expression" dxfId="10" priority="94">
       <formula>CL$7=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="95">
+    <cfRule type="expression" dxfId="9" priority="95">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="96">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J126:M126 GW126:HA126 GP126:GT126 GI126:GM126 GB126:GF126 FU126:FY126 FN126:FR126 FG126:FK126 EZ126:FD126 ES126:EW126 EL126:EP126 CH126:CL126 DX126:EB126 CO126:CS126 CV126:CZ126 P126:T126 W126:AA126 BT126:BX126 BM126:BQ126 BF126:BJ126 AD126:AH126 AK126:AO126 AR126:AV126 AY126:BC126 CA126:CE126 EE126:EI126 DC126:DG126 DJ126:DN126 DQ126:DU126">
-    <cfRule type="expression" dxfId="14" priority="1">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="2">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="3">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="4">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="5">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="6">
-      <formula>J$7=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="7">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="8" priority="96">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>